<commit_message>
indexació matrimonis Linyola llibre 1857-1865
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Matrimonis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D63E070-F988-4751-9815-5AF81E5361D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2AA3B1-0A99-454F-B91B-85B07E26E7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C34A0C26-324D-4E17-B7B1-6D7DB0FCFBF8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t>Cognoms Familia</t>
   </si>
@@ -102,6 +102,183 @@
   </si>
   <si>
     <t>Gispert Camrubí</t>
+  </si>
+  <si>
+    <t>Gene Pujades</t>
+  </si>
+  <si>
+    <t>Crespo Roige</t>
+  </si>
+  <si>
+    <t>Gispert Marti</t>
+  </si>
+  <si>
+    <t>Balcells Boldu</t>
+  </si>
+  <si>
+    <t>Agulló Clop</t>
+  </si>
+  <si>
+    <t>Cascalló Mases</t>
+  </si>
+  <si>
+    <t>Botines Martí</t>
+  </si>
+  <si>
+    <t>Cascalló Clop</t>
+  </si>
+  <si>
+    <t>Jovell Torrent</t>
+  </si>
+  <si>
+    <t>Pedrós Vilamajó</t>
+  </si>
+  <si>
+    <t>Mas Vallés</t>
+  </si>
+  <si>
+    <t>Esteve Ribes</t>
+  </si>
+  <si>
+    <t>Roca Camrubi</t>
+  </si>
+  <si>
+    <t>Pasqual Curcó</t>
+  </si>
+  <si>
+    <t>Solà Blanco</t>
+  </si>
+  <si>
+    <t>Claver Mas</t>
+  </si>
+  <si>
+    <t>Balcells Ortis</t>
+  </si>
+  <si>
+    <t>Riu Vallés</t>
+  </si>
+  <si>
+    <t>Torrent Roiger</t>
+  </si>
+  <si>
+    <t>Trepat Fabregat</t>
+  </si>
+  <si>
+    <t>Coca Batlle</t>
+  </si>
+  <si>
+    <t>Roca ¿?</t>
+  </si>
+  <si>
+    <t>Cardona Coll</t>
+  </si>
+  <si>
+    <t>Domenjo Pallerola</t>
+  </si>
+  <si>
+    <t>Sunyé Civit</t>
+  </si>
+  <si>
+    <t>Torrades Vergé</t>
+  </si>
+  <si>
+    <t>Teixiné Huguet</t>
+  </si>
+  <si>
+    <t>Roig Bonell</t>
+  </si>
+  <si>
+    <t>Farell Pujol</t>
+  </si>
+  <si>
+    <t>Piulats Mas</t>
+  </si>
+  <si>
+    <t>Trepat Vallés</t>
+  </si>
+  <si>
+    <t>Bresolí Galceràn</t>
+  </si>
+  <si>
+    <t>Vall Martí</t>
+  </si>
+  <si>
+    <t>Coll Farré</t>
+  </si>
+  <si>
+    <t>Sol Martí</t>
+  </si>
+  <si>
+    <t>Viladrich Pujol</t>
+  </si>
+  <si>
+    <t>Gené Ginesta</t>
+  </si>
+  <si>
+    <t>Vergé Roige</t>
+  </si>
+  <si>
+    <t>Pedra Vallés</t>
+  </si>
+  <si>
+    <t>Solsona Cercós</t>
+  </si>
+  <si>
+    <t>Vila Jové</t>
+  </si>
+  <si>
+    <t>Masot Torres</t>
+  </si>
+  <si>
+    <t>Padulles Nabau</t>
+  </si>
+  <si>
+    <t>Niubó Roigé</t>
+  </si>
+  <si>
+    <t>Fabregat Duart</t>
+  </si>
+  <si>
+    <t>Pedrós Pedrós</t>
+  </si>
+  <si>
+    <t>Balagué Farré</t>
+  </si>
+  <si>
+    <t>Viola Serra</t>
+  </si>
+  <si>
+    <t>Bonell Balagué</t>
+  </si>
+  <si>
+    <t>Bonell Mas</t>
+  </si>
+  <si>
+    <t>Valentines Gené</t>
+  </si>
+  <si>
+    <t>Colell Pedrós</t>
+  </si>
+  <si>
+    <t>Monfà Pujol</t>
+  </si>
+  <si>
+    <t>Mas Vergé</t>
+  </si>
+  <si>
+    <t>Solsona Mas</t>
+  </si>
+  <si>
+    <t>Mosset Falcó</t>
+  </si>
+  <si>
+    <t>Plasa Boladeres</t>
+  </si>
+  <si>
+    <t>Martí Palou</t>
+  </si>
+  <si>
+    <t>Valles Roma</t>
   </si>
 </sst>
 </file>
@@ -453,16 +630,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="3" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
@@ -644,13 +822,728 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1758</v>
+        <v>1858</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1858</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1858</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1858</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1858</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1858</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1858</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1858</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1859</v>
+      </c>
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1859</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1859</v>
+      </c>
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1859</v>
+      </c>
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1859</v>
+      </c>
+      <c r="B27">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1859</v>
+      </c>
+      <c r="B28">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1859</v>
+      </c>
+      <c r="B29">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1859</v>
+      </c>
+      <c r="B30">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1860</v>
+      </c>
+      <c r="B31">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1860</v>
+      </c>
+      <c r="B32">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1860</v>
+      </c>
+      <c r="B33">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1860</v>
+      </c>
+      <c r="B34">
+        <v>28</v>
+      </c>
+      <c r="C34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1860</v>
+      </c>
+      <c r="B35">
+        <v>28</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1860</v>
+      </c>
+      <c r="B36">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1860</v>
+      </c>
+      <c r="B37">
+        <v>29</v>
+      </c>
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1860</v>
+      </c>
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1860</v>
+      </c>
+      <c r="B39">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1860</v>
+      </c>
+      <c r="B40">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1860</v>
+      </c>
+      <c r="B41">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1860</v>
+      </c>
+      <c r="B42">
+        <v>32</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1860</v>
+      </c>
+      <c r="B43">
+        <v>33</v>
+      </c>
+      <c r="C43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1860</v>
+      </c>
+      <c r="B44">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1860</v>
+      </c>
+      <c r="B45">
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1860</v>
+      </c>
+      <c r="B46">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1860</v>
+      </c>
+      <c r="B47">
+        <v>35</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1861</v>
+      </c>
+      <c r="B48">
+        <v>36</v>
+      </c>
+      <c r="C48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1861</v>
+      </c>
+      <c r="B49">
+        <v>36</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1861</v>
+      </c>
+      <c r="B50">
+        <v>37</v>
+      </c>
+      <c r="C50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1861</v>
+      </c>
+      <c r="B51">
+        <v>37</v>
+      </c>
+      <c r="C51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1861</v>
+      </c>
+      <c r="B52">
+        <v>38</v>
+      </c>
+      <c r="C52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1861</v>
+      </c>
+      <c r="B53">
+        <v>38</v>
+      </c>
+      <c r="C53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1861</v>
+      </c>
+      <c r="B54">
+        <v>39</v>
+      </c>
+      <c r="C54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1861</v>
+      </c>
+      <c r="B55">
+        <v>39</v>
+      </c>
+      <c r="C55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1861</v>
+      </c>
+      <c r="B56">
+        <v>40</v>
+      </c>
+      <c r="C56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1861</v>
+      </c>
+      <c r="B57">
+        <v>40</v>
+      </c>
+      <c r="C57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1861</v>
+      </c>
+      <c r="B58">
+        <v>41</v>
+      </c>
+      <c r="C58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1862</v>
+      </c>
+      <c r="B59">
+        <v>41</v>
+      </c>
+      <c r="C59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1862</v>
+      </c>
+      <c r="B60">
+        <v>42</v>
+      </c>
+      <c r="C60" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1862</v>
+      </c>
+      <c r="B61">
+        <v>42</v>
+      </c>
+      <c r="C61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1862</v>
+      </c>
+      <c r="B62">
+        <v>43</v>
+      </c>
+      <c r="C62" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1862</v>
+      </c>
+      <c r="B63">
+        <v>43</v>
+      </c>
+      <c r="C63" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1862</v>
+      </c>
+      <c r="B64">
+        <v>44</v>
+      </c>
+      <c r="C64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1862</v>
+      </c>
+      <c r="B65">
+        <v>46</v>
+      </c>
+      <c r="C65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1862</v>
+      </c>
+      <c r="B66">
+        <v>47</v>
+      </c>
+      <c r="C66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1863</v>
+      </c>
+      <c r="B67">
+        <v>49</v>
+      </c>
+      <c r="C67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1863</v>
+      </c>
+      <c r="B68">
+        <v>49</v>
+      </c>
+      <c r="C68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1863</v>
+      </c>
+      <c r="B69">
+        <v>50</v>
+      </c>
+      <c r="C69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1863</v>
+      </c>
+      <c r="B70">
+        <v>50</v>
+      </c>
+      <c r="C70" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1863</v>
+      </c>
+      <c r="B71">
+        <v>51</v>
+      </c>
+      <c r="C71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1863</v>
+      </c>
+      <c r="B72">
+        <v>52</v>
+      </c>
+      <c r="C72" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1863</v>
+      </c>
+      <c r="B73">
+        <v>53</v>
+      </c>
+      <c r="C73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1863</v>
+      </c>
+      <c r="B74">
+        <v>54</v>
+      </c>
+      <c r="C74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1863</v>
+      </c>
+      <c r="B75">
+        <v>54</v>
+      </c>
+      <c r="C75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1863</v>
+      </c>
+      <c r="B76">
+        <v>55</v>
+      </c>
+      <c r="C76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1863</v>
+      </c>
+      <c r="B77">
+        <v>55</v>
+      </c>
+      <c r="C77" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1863</v>
+      </c>
+      <c r="B78">
+        <v>55</v>
+      </c>
+      <c r="C78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1863</v>
+      </c>
+      <c r="B79">
+        <v>55</v>
+      </c>
+      <c r="C79" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>1863</v>
+      </c>
+      <c r="B80">
+        <v>55</v>
+      </c>
+      <c r="C80" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
indexació de cognoms del llibre de matrimonis Linyola anys 1857-1865 completa
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Matrimonis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2AA3B1-0A99-454F-B91B-85B07E26E7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D62E6C1-D24D-4B95-A520-310B65D37F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C34A0C26-324D-4E17-B7B1-6D7DB0FCFBF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$M$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="102">
   <si>
     <t>Cognoms Familia</t>
   </si>
@@ -279,6 +282,69 @@
   </si>
   <si>
     <t>Valles Roma</t>
+  </si>
+  <si>
+    <t>Vallés Roig</t>
+  </si>
+  <si>
+    <t>Camarasa Novell</t>
+  </si>
+  <si>
+    <t>Trepat Ginesta</t>
+  </si>
+  <si>
+    <t>Perera Ripoll</t>
+  </si>
+  <si>
+    <t>Darba Colell</t>
+  </si>
+  <si>
+    <t>Pinós Martí</t>
+  </si>
+  <si>
+    <t>Civit Martí</t>
+  </si>
+  <si>
+    <t>Pujades Droguet</t>
+  </si>
+  <si>
+    <t>Arderiu Vilaltella</t>
+  </si>
+  <si>
+    <t>Ginestà Prats</t>
+  </si>
+  <si>
+    <t>Planes Pujol</t>
+  </si>
+  <si>
+    <t>Vallés Mas</t>
+  </si>
+  <si>
+    <t>Escolà Formiguera</t>
+  </si>
+  <si>
+    <t>Martí Martí</t>
+  </si>
+  <si>
+    <t>Projecte</t>
+  </si>
+  <si>
+    <t>Rollo</t>
+  </si>
+  <si>
+    <t>Serie</t>
+  </si>
+  <si>
+    <t>Anys</t>
+  </si>
+  <si>
+    <t>SPN 2,02 C</t>
+  </si>
+  <si>
+    <t>A,6</t>
+  </si>
+  <si>
+    <t>1857-1865</t>
   </si>
 </sst>
 </file>
@@ -630,16 +696,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
@@ -648,7 +714,7 @@
     <col min="8" max="8" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -676,8 +742,20 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1857</v>
       </c>
@@ -687,8 +765,20 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K2">
+        <v>47</v>
+      </c>
+      <c r="L2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1857</v>
       </c>
@@ -698,8 +788,20 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3">
+        <v>47</v>
+      </c>
+      <c r="L3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1857</v>
       </c>
@@ -709,8 +811,20 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1857</v>
       </c>
@@ -720,8 +834,20 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5">
+        <v>47</v>
+      </c>
+      <c r="L5" t="s">
+        <v>100</v>
+      </c>
+      <c r="M5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1857</v>
       </c>
@@ -731,8 +857,20 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K6">
+        <v>47</v>
+      </c>
+      <c r="L6" t="s">
+        <v>100</v>
+      </c>
+      <c r="M6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1857</v>
       </c>
@@ -742,8 +880,20 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7">
+        <v>47</v>
+      </c>
+      <c r="L7" t="s">
+        <v>100</v>
+      </c>
+      <c r="M7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1857</v>
       </c>
@@ -753,8 +903,20 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8">
+        <v>47</v>
+      </c>
+      <c r="L8" t="s">
+        <v>100</v>
+      </c>
+      <c r="M8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1857</v>
       </c>
@@ -764,8 +926,20 @@
       <c r="C9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K9">
+        <v>47</v>
+      </c>
+      <c r="L9" t="s">
+        <v>100</v>
+      </c>
+      <c r="M9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1857</v>
       </c>
@@ -775,8 +949,20 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10">
+        <v>47</v>
+      </c>
+      <c r="L10" t="s">
+        <v>100</v>
+      </c>
+      <c r="M10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1857</v>
       </c>
@@ -786,8 +972,20 @@
       <c r="C11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K11">
+        <v>47</v>
+      </c>
+      <c r="L11" t="s">
+        <v>100</v>
+      </c>
+      <c r="M11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1857</v>
       </c>
@@ -797,8 +995,20 @@
       <c r="C12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12">
+        <v>47</v>
+      </c>
+      <c r="L12" t="s">
+        <v>100</v>
+      </c>
+      <c r="M12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1857</v>
       </c>
@@ -808,8 +1018,20 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>99</v>
+      </c>
+      <c r="K13">
+        <v>47</v>
+      </c>
+      <c r="L13" t="s">
+        <v>100</v>
+      </c>
+      <c r="M13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1857</v>
       </c>
@@ -819,8 +1041,20 @@
       <c r="C14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>99</v>
+      </c>
+      <c r="K14">
+        <v>47</v>
+      </c>
+      <c r="L14" t="s">
+        <v>100</v>
+      </c>
+      <c r="M14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1858</v>
       </c>
@@ -830,8 +1064,20 @@
       <c r="C15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15">
+        <v>47</v>
+      </c>
+      <c r="L15" t="s">
+        <v>100</v>
+      </c>
+      <c r="M15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1858</v>
       </c>
@@ -841,8 +1087,20 @@
       <c r="C16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>99</v>
+      </c>
+      <c r="K16">
+        <v>47</v>
+      </c>
+      <c r="L16" t="s">
+        <v>100</v>
+      </c>
+      <c r="M16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1858</v>
       </c>
@@ -852,8 +1110,20 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>99</v>
+      </c>
+      <c r="K17">
+        <v>47</v>
+      </c>
+      <c r="L17" t="s">
+        <v>100</v>
+      </c>
+      <c r="M17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1858</v>
       </c>
@@ -863,8 +1133,20 @@
       <c r="C18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18">
+        <v>47</v>
+      </c>
+      <c r="L18" t="s">
+        <v>100</v>
+      </c>
+      <c r="M18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1858</v>
       </c>
@@ -874,8 +1156,20 @@
       <c r="C19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>99</v>
+      </c>
+      <c r="K19">
+        <v>47</v>
+      </c>
+      <c r="L19" t="s">
+        <v>100</v>
+      </c>
+      <c r="M19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1858</v>
       </c>
@@ -885,8 +1179,20 @@
       <c r="C20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>99</v>
+      </c>
+      <c r="K20">
+        <v>47</v>
+      </c>
+      <c r="L20" t="s">
+        <v>100</v>
+      </c>
+      <c r="M20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1858</v>
       </c>
@@ -896,8 +1202,20 @@
       <c r="C21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>99</v>
+      </c>
+      <c r="K21">
+        <v>47</v>
+      </c>
+      <c r="L21" t="s">
+        <v>100</v>
+      </c>
+      <c r="M21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1858</v>
       </c>
@@ -907,8 +1225,20 @@
       <c r="C22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K22">
+        <v>47</v>
+      </c>
+      <c r="L22" t="s">
+        <v>100</v>
+      </c>
+      <c r="M22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1859</v>
       </c>
@@ -918,8 +1248,20 @@
       <c r="C23" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>99</v>
+      </c>
+      <c r="K23">
+        <v>47</v>
+      </c>
+      <c r="L23" t="s">
+        <v>100</v>
+      </c>
+      <c r="M23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1859</v>
       </c>
@@ -929,8 +1271,20 @@
       <c r="C24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24">
+        <v>47</v>
+      </c>
+      <c r="L24" t="s">
+        <v>100</v>
+      </c>
+      <c r="M24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1859</v>
       </c>
@@ -940,8 +1294,20 @@
       <c r="C25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>99</v>
+      </c>
+      <c r="K25">
+        <v>47</v>
+      </c>
+      <c r="L25" t="s">
+        <v>100</v>
+      </c>
+      <c r="M25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1859</v>
       </c>
@@ -951,8 +1317,20 @@
       <c r="C26" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>99</v>
+      </c>
+      <c r="K26">
+        <v>47</v>
+      </c>
+      <c r="L26" t="s">
+        <v>100</v>
+      </c>
+      <c r="M26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1859</v>
       </c>
@@ -962,8 +1340,20 @@
       <c r="C27" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>99</v>
+      </c>
+      <c r="K27">
+        <v>47</v>
+      </c>
+      <c r="L27" t="s">
+        <v>100</v>
+      </c>
+      <c r="M27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1859</v>
       </c>
@@ -973,8 +1363,20 @@
       <c r="C28" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>99</v>
+      </c>
+      <c r="K28">
+        <v>47</v>
+      </c>
+      <c r="L28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1859</v>
       </c>
@@ -984,8 +1386,20 @@
       <c r="C29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>99</v>
+      </c>
+      <c r="K29">
+        <v>47</v>
+      </c>
+      <c r="L29" t="s">
+        <v>100</v>
+      </c>
+      <c r="M29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1859</v>
       </c>
@@ -995,8 +1409,20 @@
       <c r="C30" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>99</v>
+      </c>
+      <c r="K30">
+        <v>47</v>
+      </c>
+      <c r="L30" t="s">
+        <v>100</v>
+      </c>
+      <c r="M30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1860</v>
       </c>
@@ -1006,8 +1432,20 @@
       <c r="C31" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K31">
+        <v>47</v>
+      </c>
+      <c r="L31" t="s">
+        <v>100</v>
+      </c>
+      <c r="M31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1860</v>
       </c>
@@ -1017,8 +1455,20 @@
       <c r="C32" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>99</v>
+      </c>
+      <c r="K32">
+        <v>47</v>
+      </c>
+      <c r="L32" t="s">
+        <v>100</v>
+      </c>
+      <c r="M32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1860</v>
       </c>
@@ -1028,8 +1478,20 @@
       <c r="C33" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33">
+        <v>47</v>
+      </c>
+      <c r="L33" t="s">
+        <v>100</v>
+      </c>
+      <c r="M33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1860</v>
       </c>
@@ -1039,8 +1501,20 @@
       <c r="C34" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>99</v>
+      </c>
+      <c r="K34">
+        <v>47</v>
+      </c>
+      <c r="L34" t="s">
+        <v>100</v>
+      </c>
+      <c r="M34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1860</v>
       </c>
@@ -1050,8 +1524,20 @@
       <c r="C35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>99</v>
+      </c>
+      <c r="K35">
+        <v>47</v>
+      </c>
+      <c r="L35" t="s">
+        <v>100</v>
+      </c>
+      <c r="M35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1860</v>
       </c>
@@ -1061,8 +1547,20 @@
       <c r="C36" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>99</v>
+      </c>
+      <c r="K36">
+        <v>47</v>
+      </c>
+      <c r="L36" t="s">
+        <v>100</v>
+      </c>
+      <c r="M36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1860</v>
       </c>
@@ -1072,8 +1570,20 @@
       <c r="C37" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>99</v>
+      </c>
+      <c r="K37">
+        <v>47</v>
+      </c>
+      <c r="L37" t="s">
+        <v>100</v>
+      </c>
+      <c r="M37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1860</v>
       </c>
@@ -1083,8 +1593,20 @@
       <c r="C38" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>99</v>
+      </c>
+      <c r="K38">
+        <v>47</v>
+      </c>
+      <c r="L38" t="s">
+        <v>100</v>
+      </c>
+      <c r="M38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1860</v>
       </c>
@@ -1094,8 +1616,20 @@
       <c r="C39" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>99</v>
+      </c>
+      <c r="K39">
+        <v>47</v>
+      </c>
+      <c r="L39" t="s">
+        <v>100</v>
+      </c>
+      <c r="M39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1860</v>
       </c>
@@ -1105,8 +1639,20 @@
       <c r="C40" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>99</v>
+      </c>
+      <c r="K40">
+        <v>47</v>
+      </c>
+      <c r="L40" t="s">
+        <v>100</v>
+      </c>
+      <c r="M40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1860</v>
       </c>
@@ -1116,8 +1662,20 @@
       <c r="C41" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>99</v>
+      </c>
+      <c r="K41">
+        <v>47</v>
+      </c>
+      <c r="L41" t="s">
+        <v>100</v>
+      </c>
+      <c r="M41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1860</v>
       </c>
@@ -1127,8 +1685,20 @@
       <c r="C42" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>99</v>
+      </c>
+      <c r="K42">
+        <v>47</v>
+      </c>
+      <c r="L42" t="s">
+        <v>100</v>
+      </c>
+      <c r="M42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1860</v>
       </c>
@@ -1138,8 +1708,20 @@
       <c r="C43" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>99</v>
+      </c>
+      <c r="K43">
+        <v>47</v>
+      </c>
+      <c r="L43" t="s">
+        <v>100</v>
+      </c>
+      <c r="M43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1860</v>
       </c>
@@ -1149,8 +1731,20 @@
       <c r="C44" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>99</v>
+      </c>
+      <c r="K44">
+        <v>47</v>
+      </c>
+      <c r="L44" t="s">
+        <v>100</v>
+      </c>
+      <c r="M44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1860</v>
       </c>
@@ -1160,8 +1754,20 @@
       <c r="C45" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>99</v>
+      </c>
+      <c r="K45">
+        <v>47</v>
+      </c>
+      <c r="L45" t="s">
+        <v>100</v>
+      </c>
+      <c r="M45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1860</v>
       </c>
@@ -1171,8 +1777,20 @@
       <c r="C46" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>99</v>
+      </c>
+      <c r="K46">
+        <v>47</v>
+      </c>
+      <c r="L46" t="s">
+        <v>100</v>
+      </c>
+      <c r="M46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1860</v>
       </c>
@@ -1182,8 +1800,20 @@
       <c r="C47" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>99</v>
+      </c>
+      <c r="K47">
+        <v>47</v>
+      </c>
+      <c r="L47" t="s">
+        <v>100</v>
+      </c>
+      <c r="M47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1861</v>
       </c>
@@ -1193,8 +1823,20 @@
       <c r="C48" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>99</v>
+      </c>
+      <c r="K48">
+        <v>47</v>
+      </c>
+      <c r="L48" t="s">
+        <v>100</v>
+      </c>
+      <c r="M48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1861</v>
       </c>
@@ -1204,8 +1846,20 @@
       <c r="C49" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>99</v>
+      </c>
+      <c r="K49">
+        <v>47</v>
+      </c>
+      <c r="L49" t="s">
+        <v>100</v>
+      </c>
+      <c r="M49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1861</v>
       </c>
@@ -1215,8 +1869,20 @@
       <c r="C50" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>99</v>
+      </c>
+      <c r="K50">
+        <v>47</v>
+      </c>
+      <c r="L50" t="s">
+        <v>100</v>
+      </c>
+      <c r="M50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1861</v>
       </c>
@@ -1226,8 +1892,20 @@
       <c r="C51" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>99</v>
+      </c>
+      <c r="K51">
+        <v>47</v>
+      </c>
+      <c r="L51" t="s">
+        <v>100</v>
+      </c>
+      <c r="M51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1861</v>
       </c>
@@ -1237,8 +1915,20 @@
       <c r="C52" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>99</v>
+      </c>
+      <c r="K52">
+        <v>47</v>
+      </c>
+      <c r="L52" t="s">
+        <v>100</v>
+      </c>
+      <c r="M52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1861</v>
       </c>
@@ -1248,8 +1938,20 @@
       <c r="C53" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>99</v>
+      </c>
+      <c r="K53">
+        <v>47</v>
+      </c>
+      <c r="L53" t="s">
+        <v>100</v>
+      </c>
+      <c r="M53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1861</v>
       </c>
@@ -1259,8 +1961,20 @@
       <c r="C54" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>99</v>
+      </c>
+      <c r="K54">
+        <v>47</v>
+      </c>
+      <c r="L54" t="s">
+        <v>100</v>
+      </c>
+      <c r="M54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1861</v>
       </c>
@@ -1270,8 +1984,20 @@
       <c r="C55" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>99</v>
+      </c>
+      <c r="K55">
+        <v>47</v>
+      </c>
+      <c r="L55" t="s">
+        <v>100</v>
+      </c>
+      <c r="M55" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1861</v>
       </c>
@@ -1281,8 +2007,20 @@
       <c r="C56" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>99</v>
+      </c>
+      <c r="K56">
+        <v>47</v>
+      </c>
+      <c r="L56" t="s">
+        <v>100</v>
+      </c>
+      <c r="M56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1861</v>
       </c>
@@ -1292,8 +2030,20 @@
       <c r="C57" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>99</v>
+      </c>
+      <c r="K57">
+        <v>47</v>
+      </c>
+      <c r="L57" t="s">
+        <v>100</v>
+      </c>
+      <c r="M57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1861</v>
       </c>
@@ -1303,8 +2053,20 @@
       <c r="C58" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>99</v>
+      </c>
+      <c r="K58">
+        <v>47</v>
+      </c>
+      <c r="L58" t="s">
+        <v>100</v>
+      </c>
+      <c r="M58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1862</v>
       </c>
@@ -1314,8 +2076,20 @@
       <c r="C59" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>99</v>
+      </c>
+      <c r="K59">
+        <v>47</v>
+      </c>
+      <c r="L59" t="s">
+        <v>100</v>
+      </c>
+      <c r="M59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1862</v>
       </c>
@@ -1325,8 +2099,20 @@
       <c r="C60" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>99</v>
+      </c>
+      <c r="K60">
+        <v>47</v>
+      </c>
+      <c r="L60" t="s">
+        <v>100</v>
+      </c>
+      <c r="M60" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1862</v>
       </c>
@@ -1336,8 +2122,20 @@
       <c r="C61" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>99</v>
+      </c>
+      <c r="K61">
+        <v>47</v>
+      </c>
+      <c r="L61" t="s">
+        <v>100</v>
+      </c>
+      <c r="M61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1862</v>
       </c>
@@ -1347,8 +2145,20 @@
       <c r="C62" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>99</v>
+      </c>
+      <c r="K62">
+        <v>47</v>
+      </c>
+      <c r="L62" t="s">
+        <v>100</v>
+      </c>
+      <c r="M62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1862</v>
       </c>
@@ -1358,8 +2168,20 @@
       <c r="C63" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>99</v>
+      </c>
+      <c r="K63">
+        <v>47</v>
+      </c>
+      <c r="L63" t="s">
+        <v>100</v>
+      </c>
+      <c r="M63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1862</v>
       </c>
@@ -1369,8 +2191,20 @@
       <c r="C64" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>99</v>
+      </c>
+      <c r="K64">
+        <v>47</v>
+      </c>
+      <c r="L64" t="s">
+        <v>100</v>
+      </c>
+      <c r="M64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1862</v>
       </c>
@@ -1380,8 +2214,20 @@
       <c r="C65" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>99</v>
+      </c>
+      <c r="K65">
+        <v>47</v>
+      </c>
+      <c r="L65" t="s">
+        <v>100</v>
+      </c>
+      <c r="M65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1862</v>
       </c>
@@ -1391,8 +2237,20 @@
       <c r="C66" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>99</v>
+      </c>
+      <c r="K66">
+        <v>47</v>
+      </c>
+      <c r="L66" t="s">
+        <v>100</v>
+      </c>
+      <c r="M66" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1863</v>
       </c>
@@ -1402,8 +2260,20 @@
       <c r="C67" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>99</v>
+      </c>
+      <c r="K67">
+        <v>47</v>
+      </c>
+      <c r="L67" t="s">
+        <v>100</v>
+      </c>
+      <c r="M67" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1863</v>
       </c>
@@ -1413,8 +2283,20 @@
       <c r="C68" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>99</v>
+      </c>
+      <c r="K68">
+        <v>47</v>
+      </c>
+      <c r="L68" t="s">
+        <v>100</v>
+      </c>
+      <c r="M68" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1863</v>
       </c>
@@ -1424,8 +2306,20 @@
       <c r="C69" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>99</v>
+      </c>
+      <c r="K69">
+        <v>47</v>
+      </c>
+      <c r="L69" t="s">
+        <v>100</v>
+      </c>
+      <c r="M69" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1863</v>
       </c>
@@ -1435,8 +2329,20 @@
       <c r="C70" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>99</v>
+      </c>
+      <c r="K70">
+        <v>47</v>
+      </c>
+      <c r="L70" t="s">
+        <v>100</v>
+      </c>
+      <c r="M70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1863</v>
       </c>
@@ -1446,8 +2352,20 @@
       <c r="C71" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>99</v>
+      </c>
+      <c r="K71">
+        <v>47</v>
+      </c>
+      <c r="L71" t="s">
+        <v>100</v>
+      </c>
+      <c r="M71" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1863</v>
       </c>
@@ -1457,8 +2375,20 @@
       <c r="C72" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>99</v>
+      </c>
+      <c r="K72">
+        <v>47</v>
+      </c>
+      <c r="L72" t="s">
+        <v>100</v>
+      </c>
+      <c r="M72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1863</v>
       </c>
@@ -1468,8 +2398,20 @@
       <c r="C73" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>99</v>
+      </c>
+      <c r="K73">
+        <v>47</v>
+      </c>
+      <c r="L73" t="s">
+        <v>100</v>
+      </c>
+      <c r="M73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1863</v>
       </c>
@@ -1479,8 +2421,20 @@
       <c r="C74" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>99</v>
+      </c>
+      <c r="K74">
+        <v>47</v>
+      </c>
+      <c r="L74" t="s">
+        <v>100</v>
+      </c>
+      <c r="M74" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1863</v>
       </c>
@@ -1490,8 +2444,20 @@
       <c r="C75" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>99</v>
+      </c>
+      <c r="K75">
+        <v>47</v>
+      </c>
+      <c r="L75" t="s">
+        <v>100</v>
+      </c>
+      <c r="M75" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1863</v>
       </c>
@@ -1501,8 +2467,20 @@
       <c r="C76" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>99</v>
+      </c>
+      <c r="K76">
+        <v>47</v>
+      </c>
+      <c r="L76" t="s">
+        <v>100</v>
+      </c>
+      <c r="M76" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1863</v>
       </c>
@@ -1512,8 +2490,20 @@
       <c r="C77" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>99</v>
+      </c>
+      <c r="K77">
+        <v>47</v>
+      </c>
+      <c r="L77" t="s">
+        <v>100</v>
+      </c>
+      <c r="M77" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1863</v>
       </c>
@@ -1523,8 +2513,20 @@
       <c r="C78" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>99</v>
+      </c>
+      <c r="K78">
+        <v>47</v>
+      </c>
+      <c r="L78" t="s">
+        <v>100</v>
+      </c>
+      <c r="M78" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1863</v>
       </c>
@@ -1534,8 +2536,20 @@
       <c r="C79" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
+        <v>99</v>
+      </c>
+      <c r="K79">
+        <v>47</v>
+      </c>
+      <c r="L79" t="s">
+        <v>100</v>
+      </c>
+      <c r="M79" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1863</v>
       </c>
@@ -1545,8 +2559,366 @@
       <c r="C80" t="s">
         <v>80</v>
       </c>
+      <c r="J80" t="s">
+        <v>99</v>
+      </c>
+      <c r="K80">
+        <v>47</v>
+      </c>
+      <c r="L80" t="s">
+        <v>100</v>
+      </c>
+      <c r="M80" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1864</v>
+      </c>
+      <c r="B81">
+        <v>56</v>
+      </c>
+      <c r="C81" t="s">
+        <v>81</v>
+      </c>
+      <c r="J81" t="s">
+        <v>99</v>
+      </c>
+      <c r="K81">
+        <v>47</v>
+      </c>
+      <c r="L81" t="s">
+        <v>100</v>
+      </c>
+      <c r="M81" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>1864</v>
+      </c>
+      <c r="B82">
+        <v>56</v>
+      </c>
+      <c r="C82" t="s">
+        <v>67</v>
+      </c>
+      <c r="J82" t="s">
+        <v>99</v>
+      </c>
+      <c r="K82">
+        <v>47</v>
+      </c>
+      <c r="L82" t="s">
+        <v>100</v>
+      </c>
+      <c r="M82" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>1864</v>
+      </c>
+      <c r="B83">
+        <v>56</v>
+      </c>
+      <c r="C83" t="s">
+        <v>82</v>
+      </c>
+      <c r="J83" t="s">
+        <v>99</v>
+      </c>
+      <c r="K83">
+        <v>47</v>
+      </c>
+      <c r="L83" t="s">
+        <v>100</v>
+      </c>
+      <c r="M83" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>1864</v>
+      </c>
+      <c r="B84">
+        <v>56</v>
+      </c>
+      <c r="C84" t="s">
+        <v>83</v>
+      </c>
+      <c r="J84" t="s">
+        <v>99</v>
+      </c>
+      <c r="K84">
+        <v>47</v>
+      </c>
+      <c r="L84" t="s">
+        <v>100</v>
+      </c>
+      <c r="M84" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>1864</v>
+      </c>
+      <c r="B85">
+        <v>57</v>
+      </c>
+      <c r="C85" t="s">
+        <v>84</v>
+      </c>
+      <c r="J85" t="s">
+        <v>99</v>
+      </c>
+      <c r="K85">
+        <v>47</v>
+      </c>
+      <c r="L85" t="s">
+        <v>100</v>
+      </c>
+      <c r="M85" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>1865</v>
+      </c>
+      <c r="B86">
+        <v>57</v>
+      </c>
+      <c r="C86" t="s">
+        <v>85</v>
+      </c>
+      <c r="J86" t="s">
+        <v>99</v>
+      </c>
+      <c r="K86">
+        <v>47</v>
+      </c>
+      <c r="L86" t="s">
+        <v>100</v>
+      </c>
+      <c r="M86" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1865</v>
+      </c>
+      <c r="B87">
+        <v>57</v>
+      </c>
+      <c r="C87" t="s">
+        <v>86</v>
+      </c>
+      <c r="J87" t="s">
+        <v>99</v>
+      </c>
+      <c r="K87">
+        <v>47</v>
+      </c>
+      <c r="L87" t="s">
+        <v>100</v>
+      </c>
+      <c r="M87" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>1865</v>
+      </c>
+      <c r="B88">
+        <v>58</v>
+      </c>
+      <c r="C88" t="s">
+        <v>87</v>
+      </c>
+      <c r="J88" t="s">
+        <v>99</v>
+      </c>
+      <c r="K88">
+        <v>47</v>
+      </c>
+      <c r="L88" t="s">
+        <v>100</v>
+      </c>
+      <c r="M88" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1865</v>
+      </c>
+      <c r="B89">
+        <v>58</v>
+      </c>
+      <c r="C89" t="s">
+        <v>88</v>
+      </c>
+      <c r="J89" t="s">
+        <v>99</v>
+      </c>
+      <c r="K89">
+        <v>47</v>
+      </c>
+      <c r="L89" t="s">
+        <v>100</v>
+      </c>
+      <c r="M89" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>1865</v>
+      </c>
+      <c r="B90">
+        <v>58</v>
+      </c>
+      <c r="C90" t="s">
+        <v>89</v>
+      </c>
+      <c r="J90" t="s">
+        <v>99</v>
+      </c>
+      <c r="K90">
+        <v>47</v>
+      </c>
+      <c r="L90" t="s">
+        <v>100</v>
+      </c>
+      <c r="M90" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1865</v>
+      </c>
+      <c r="B91">
+        <v>58</v>
+      </c>
+      <c r="C91" t="s">
+        <v>90</v>
+      </c>
+      <c r="J91" t="s">
+        <v>99</v>
+      </c>
+      <c r="K91">
+        <v>47</v>
+      </c>
+      <c r="L91" t="s">
+        <v>100</v>
+      </c>
+      <c r="M91" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1865</v>
+      </c>
+      <c r="B92">
+        <v>59</v>
+      </c>
+      <c r="C92" t="s">
+        <v>91</v>
+      </c>
+      <c r="J92" t="s">
+        <v>99</v>
+      </c>
+      <c r="K92">
+        <v>47</v>
+      </c>
+      <c r="L92" t="s">
+        <v>100</v>
+      </c>
+      <c r="M92" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1865</v>
+      </c>
+      <c r="B93">
+        <v>59</v>
+      </c>
+      <c r="C93" t="s">
+        <v>92</v>
+      </c>
+      <c r="J93" t="s">
+        <v>99</v>
+      </c>
+      <c r="K93">
+        <v>47</v>
+      </c>
+      <c r="L93" t="s">
+        <v>100</v>
+      </c>
+      <c r="M93" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1865</v>
+      </c>
+      <c r="B94">
+        <v>59</v>
+      </c>
+      <c r="C94" t="s">
+        <v>93</v>
+      </c>
+      <c r="J94" t="s">
+        <v>99</v>
+      </c>
+      <c r="K94">
+        <v>47</v>
+      </c>
+      <c r="L94" t="s">
+        <v>100</v>
+      </c>
+      <c r="M94" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>1865</v>
+      </c>
+      <c r="B95">
+        <v>59</v>
+      </c>
+      <c r="C95" t="s">
+        <v>94</v>
+      </c>
+      <c r="J95" t="s">
+        <v>99</v>
+      </c>
+      <c r="K95">
+        <v>47</v>
+      </c>
+      <c r="L95" t="s">
+        <v>100</v>
+      </c>
+      <c r="M95" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M1" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
indexació de cognoms del llibre de matrimonis Linyola anys 1852-1856 completa
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Matrimonis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D62E6C1-D24D-4B95-A520-310B65D37F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA04F7E8-D9D8-4B59-8594-7E59023EEBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C34A0C26-324D-4E17-B7B1-6D7DB0FCFBF8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="150">
   <si>
     <t>Cognoms Familia</t>
   </si>
@@ -345,6 +345,150 @@
   </si>
   <si>
     <t>1857-1865</t>
+  </si>
+  <si>
+    <t>1852-1856</t>
+  </si>
+  <si>
+    <t>A,5</t>
+  </si>
+  <si>
+    <t>Pasqual Gilavert</t>
+  </si>
+  <si>
+    <t>Majoral Fiquera</t>
+  </si>
+  <si>
+    <t>Majoral Vergé</t>
+  </si>
+  <si>
+    <t>Gormiguera Ginestà</t>
+  </si>
+  <si>
+    <t>Formiguera Martí</t>
+  </si>
+  <si>
+    <t>Varniol Castelló</t>
+  </si>
+  <si>
+    <t>Prenafeta Torres</t>
+  </si>
+  <si>
+    <t>Gomà Galceran</t>
+  </si>
+  <si>
+    <t>Cava Codina</t>
+  </si>
+  <si>
+    <t>Oliva Trepat</t>
+  </si>
+  <si>
+    <t>Cercós Martí</t>
+  </si>
+  <si>
+    <t>Centena Mata</t>
+  </si>
+  <si>
+    <t>Ribes Martí</t>
+  </si>
+  <si>
+    <t>Palou Mas</t>
+  </si>
+  <si>
+    <t>Palou Mosset</t>
+  </si>
+  <si>
+    <t>Bellet Pedrós</t>
+  </si>
+  <si>
+    <t>Labaquial Figuera</t>
+  </si>
+  <si>
+    <t>Roma Civit</t>
+  </si>
+  <si>
+    <t>Binefa Martí</t>
+  </si>
+  <si>
+    <t>Formiiguera Bellet</t>
+  </si>
+  <si>
+    <t>Fabregat Mosset</t>
+  </si>
+  <si>
+    <t>Cascallo Mosset</t>
+  </si>
+  <si>
+    <t>Cisteró Nabau</t>
+  </si>
+  <si>
+    <t>Riart Rosell</t>
+  </si>
+  <si>
+    <t>Roige Pasqual</t>
+  </si>
+  <si>
+    <t>Solsona Majoral</t>
+  </si>
+  <si>
+    <t>Gili Pujol</t>
+  </si>
+  <si>
+    <t>Martí Fradevia</t>
+  </si>
+  <si>
+    <t>Moset Mas</t>
+  </si>
+  <si>
+    <t>Martí Gené</t>
+  </si>
+  <si>
+    <t>Pallerola Solé</t>
+  </si>
+  <si>
+    <t>Pedrós Mas</t>
+  </si>
+  <si>
+    <t>Cascalló Vallés</t>
+  </si>
+  <si>
+    <t>Llovera Sales</t>
+  </si>
+  <si>
+    <t>Niubó Mas</t>
+  </si>
+  <si>
+    <t>Fabregat Arderiu</t>
+  </si>
+  <si>
+    <t>Colell Farré</t>
+  </si>
+  <si>
+    <t>Martí Gene</t>
+  </si>
+  <si>
+    <t>Bellet Escolà</t>
+  </si>
+  <si>
+    <t>Renyé Pujol</t>
+  </si>
+  <si>
+    <t>Pasqual Ribes</t>
+  </si>
+  <si>
+    <t>Mas Riart</t>
+  </si>
+  <si>
+    <t>Planes Agulló</t>
+  </si>
+  <si>
+    <t>Pedrós Bonet</t>
+  </si>
+  <si>
+    <t>Simó Mata</t>
+  </si>
+  <si>
+    <t>Torra Civit</t>
   </si>
 </sst>
 </file>
@@ -696,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}">
-  <dimension ref="A1:M95"/>
+  <dimension ref="A1:M143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2917,6 +3061,1110 @@
         <v>101</v>
       </c>
     </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>1852</v>
+      </c>
+      <c r="B96">
+        <v>4</v>
+      </c>
+      <c r="C96" t="s">
+        <v>104</v>
+      </c>
+      <c r="J96" t="s">
+        <v>99</v>
+      </c>
+      <c r="K96">
+        <v>47</v>
+      </c>
+      <c r="L96" t="s">
+        <v>103</v>
+      </c>
+      <c r="M96" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>1852</v>
+      </c>
+      <c r="B97">
+        <v>5</v>
+      </c>
+      <c r="C97" t="s">
+        <v>105</v>
+      </c>
+      <c r="J97" t="s">
+        <v>99</v>
+      </c>
+      <c r="K97">
+        <v>47</v>
+      </c>
+      <c r="L97" t="s">
+        <v>103</v>
+      </c>
+      <c r="M97" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>1852</v>
+      </c>
+      <c r="B98">
+        <v>6</v>
+      </c>
+      <c r="C98" t="s">
+        <v>106</v>
+      </c>
+      <c r="J98" t="s">
+        <v>99</v>
+      </c>
+      <c r="K98">
+        <v>47</v>
+      </c>
+      <c r="L98" t="s">
+        <v>103</v>
+      </c>
+      <c r="M98" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>1852</v>
+      </c>
+      <c r="B99">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s">
+        <v>107</v>
+      </c>
+      <c r="J99" t="s">
+        <v>99</v>
+      </c>
+      <c r="K99">
+        <v>47</v>
+      </c>
+      <c r="L99" t="s">
+        <v>103</v>
+      </c>
+      <c r="M99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1852</v>
+      </c>
+      <c r="B100">
+        <v>8</v>
+      </c>
+      <c r="C100" t="s">
+        <v>108</v>
+      </c>
+      <c r="J100" t="s">
+        <v>99</v>
+      </c>
+      <c r="K100">
+        <v>47</v>
+      </c>
+      <c r="L100" t="s">
+        <v>103</v>
+      </c>
+      <c r="M100" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>1852</v>
+      </c>
+      <c r="B101">
+        <v>9</v>
+      </c>
+      <c r="C101" t="s">
+        <v>109</v>
+      </c>
+      <c r="J101" t="s">
+        <v>99</v>
+      </c>
+      <c r="K101">
+        <v>47</v>
+      </c>
+      <c r="L101" t="s">
+        <v>103</v>
+      </c>
+      <c r="M101" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>1852</v>
+      </c>
+      <c r="B102">
+        <v>10</v>
+      </c>
+      <c r="C102" t="s">
+        <v>110</v>
+      </c>
+      <c r="J102" t="s">
+        <v>99</v>
+      </c>
+      <c r="K102">
+        <v>47</v>
+      </c>
+      <c r="L102" t="s">
+        <v>103</v>
+      </c>
+      <c r="M102" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1852</v>
+      </c>
+      <c r="B103">
+        <v>11</v>
+      </c>
+      <c r="C103" t="s">
+        <v>111</v>
+      </c>
+      <c r="J103" t="s">
+        <v>99</v>
+      </c>
+      <c r="K103">
+        <v>47</v>
+      </c>
+      <c r="L103" t="s">
+        <v>103</v>
+      </c>
+      <c r="M103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1853</v>
+      </c>
+      <c r="B104">
+        <v>12</v>
+      </c>
+      <c r="C104" t="s">
+        <v>112</v>
+      </c>
+      <c r="J104" t="s">
+        <v>99</v>
+      </c>
+      <c r="K104">
+        <v>47</v>
+      </c>
+      <c r="L104" t="s">
+        <v>103</v>
+      </c>
+      <c r="M104" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>1853</v>
+      </c>
+      <c r="B105">
+        <v>13</v>
+      </c>
+      <c r="C105" t="s">
+        <v>10</v>
+      </c>
+      <c r="J105" t="s">
+        <v>99</v>
+      </c>
+      <c r="K105">
+        <v>47</v>
+      </c>
+      <c r="L105" t="s">
+        <v>103</v>
+      </c>
+      <c r="M105" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>1853</v>
+      </c>
+      <c r="B106">
+        <v>14</v>
+      </c>
+      <c r="C106" t="s">
+        <v>113</v>
+      </c>
+      <c r="J106" t="s">
+        <v>99</v>
+      </c>
+      <c r="K106">
+        <v>47</v>
+      </c>
+      <c r="L106" t="s">
+        <v>103</v>
+      </c>
+      <c r="M106" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1853</v>
+      </c>
+      <c r="B107">
+        <v>15</v>
+      </c>
+      <c r="C107" t="s">
+        <v>114</v>
+      </c>
+      <c r="J107" t="s">
+        <v>99</v>
+      </c>
+      <c r="K107">
+        <v>47</v>
+      </c>
+      <c r="L107" t="s">
+        <v>103</v>
+      </c>
+      <c r="M107" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>1853</v>
+      </c>
+      <c r="B108">
+        <v>16</v>
+      </c>
+      <c r="C108" t="s">
+        <v>115</v>
+      </c>
+      <c r="J108" t="s">
+        <v>99</v>
+      </c>
+      <c r="K108">
+        <v>47</v>
+      </c>
+      <c r="L108" t="s">
+        <v>103</v>
+      </c>
+      <c r="M108" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1853</v>
+      </c>
+      <c r="B109">
+        <v>17</v>
+      </c>
+      <c r="C109" t="s">
+        <v>116</v>
+      </c>
+      <c r="J109" t="s">
+        <v>99</v>
+      </c>
+      <c r="K109">
+        <v>47</v>
+      </c>
+      <c r="L109" t="s">
+        <v>103</v>
+      </c>
+      <c r="M109" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1854</v>
+      </c>
+      <c r="B110">
+        <v>19</v>
+      </c>
+      <c r="C110" t="s">
+        <v>117</v>
+      </c>
+      <c r="J110" t="s">
+        <v>99</v>
+      </c>
+      <c r="K110">
+        <v>47</v>
+      </c>
+      <c r="L110" t="s">
+        <v>103</v>
+      </c>
+      <c r="M110" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1854</v>
+      </c>
+      <c r="B111">
+        <v>20</v>
+      </c>
+      <c r="C111" t="s">
+        <v>118</v>
+      </c>
+      <c r="J111" t="s">
+        <v>99</v>
+      </c>
+      <c r="K111">
+        <v>47</v>
+      </c>
+      <c r="L111" t="s">
+        <v>103</v>
+      </c>
+      <c r="M111" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1854</v>
+      </c>
+      <c r="B112">
+        <v>21</v>
+      </c>
+      <c r="C112" t="s">
+        <v>119</v>
+      </c>
+      <c r="J112" t="s">
+        <v>99</v>
+      </c>
+      <c r="K112">
+        <v>47</v>
+      </c>
+      <c r="L112" t="s">
+        <v>103</v>
+      </c>
+      <c r="M112" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>1854</v>
+      </c>
+      <c r="B113">
+        <v>22</v>
+      </c>
+      <c r="C113" t="s">
+        <v>120</v>
+      </c>
+      <c r="J113" t="s">
+        <v>99</v>
+      </c>
+      <c r="K113">
+        <v>47</v>
+      </c>
+      <c r="L113" t="s">
+        <v>103</v>
+      </c>
+      <c r="M113" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>1854</v>
+      </c>
+      <c r="B114">
+        <v>23</v>
+      </c>
+      <c r="C114" t="s">
+        <v>121</v>
+      </c>
+      <c r="J114" t="s">
+        <v>99</v>
+      </c>
+      <c r="K114">
+        <v>47</v>
+      </c>
+      <c r="L114" t="s">
+        <v>103</v>
+      </c>
+      <c r="M114" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>1854</v>
+      </c>
+      <c r="B115">
+        <v>24</v>
+      </c>
+      <c r="C115" t="s">
+        <v>122</v>
+      </c>
+      <c r="J115" t="s">
+        <v>99</v>
+      </c>
+      <c r="K115">
+        <v>47</v>
+      </c>
+      <c r="L115" t="s">
+        <v>103</v>
+      </c>
+      <c r="M115" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>1854</v>
+      </c>
+      <c r="B116">
+        <v>25</v>
+      </c>
+      <c r="C116" t="s">
+        <v>123</v>
+      </c>
+      <c r="J116" t="s">
+        <v>99</v>
+      </c>
+      <c r="K116">
+        <v>47</v>
+      </c>
+      <c r="L116" t="s">
+        <v>103</v>
+      </c>
+      <c r="M116" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>1854</v>
+      </c>
+      <c r="B117">
+        <v>26</v>
+      </c>
+      <c r="C117" t="s">
+        <v>124</v>
+      </c>
+      <c r="J117" t="s">
+        <v>99</v>
+      </c>
+      <c r="K117">
+        <v>47</v>
+      </c>
+      <c r="L117" t="s">
+        <v>103</v>
+      </c>
+      <c r="M117" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>1854</v>
+      </c>
+      <c r="B118">
+        <v>27</v>
+      </c>
+      <c r="C118" t="s">
+        <v>125</v>
+      </c>
+      <c r="J118" t="s">
+        <v>99</v>
+      </c>
+      <c r="K118">
+        <v>47</v>
+      </c>
+      <c r="L118" t="s">
+        <v>103</v>
+      </c>
+      <c r="M118" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>1855</v>
+      </c>
+      <c r="B119">
+        <v>28</v>
+      </c>
+      <c r="C119" t="s">
+        <v>126</v>
+      </c>
+      <c r="J119" t="s">
+        <v>99</v>
+      </c>
+      <c r="K119">
+        <v>47</v>
+      </c>
+      <c r="L119" t="s">
+        <v>103</v>
+      </c>
+      <c r="M119" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>1855</v>
+      </c>
+      <c r="B120">
+        <v>29</v>
+      </c>
+      <c r="C120" t="s">
+        <v>127</v>
+      </c>
+      <c r="J120" t="s">
+        <v>99</v>
+      </c>
+      <c r="K120">
+        <v>47</v>
+      </c>
+      <c r="L120" t="s">
+        <v>103</v>
+      </c>
+      <c r="M120" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1855</v>
+      </c>
+      <c r="B121">
+        <v>30</v>
+      </c>
+      <c r="C121" t="s">
+        <v>128</v>
+      </c>
+      <c r="J121" t="s">
+        <v>99</v>
+      </c>
+      <c r="K121">
+        <v>47</v>
+      </c>
+      <c r="L121" t="s">
+        <v>103</v>
+      </c>
+      <c r="M121" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>1855</v>
+      </c>
+      <c r="B122">
+        <v>31</v>
+      </c>
+      <c r="C122" t="s">
+        <v>129</v>
+      </c>
+      <c r="J122" t="s">
+        <v>99</v>
+      </c>
+      <c r="K122">
+        <v>47</v>
+      </c>
+      <c r="L122" t="s">
+        <v>103</v>
+      </c>
+      <c r="M122" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>1855</v>
+      </c>
+      <c r="B123">
+        <v>32</v>
+      </c>
+      <c r="C123" t="s">
+        <v>130</v>
+      </c>
+      <c r="J123" t="s">
+        <v>99</v>
+      </c>
+      <c r="K123">
+        <v>47</v>
+      </c>
+      <c r="L123" t="s">
+        <v>103</v>
+      </c>
+      <c r="M123" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>1855</v>
+      </c>
+      <c r="B124">
+        <v>33</v>
+      </c>
+      <c r="C124" t="s">
+        <v>131</v>
+      </c>
+      <c r="J124" t="s">
+        <v>99</v>
+      </c>
+      <c r="K124">
+        <v>47</v>
+      </c>
+      <c r="L124" t="s">
+        <v>103</v>
+      </c>
+      <c r="M124" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>1855</v>
+      </c>
+      <c r="B125">
+        <v>34</v>
+      </c>
+      <c r="C125" t="s">
+        <v>132</v>
+      </c>
+      <c r="J125" t="s">
+        <v>99</v>
+      </c>
+      <c r="K125">
+        <v>47</v>
+      </c>
+      <c r="L125" t="s">
+        <v>103</v>
+      </c>
+      <c r="M125" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>1855</v>
+      </c>
+      <c r="B126">
+        <v>35</v>
+      </c>
+      <c r="C126" t="s">
+        <v>133</v>
+      </c>
+      <c r="J126" t="s">
+        <v>99</v>
+      </c>
+      <c r="K126">
+        <v>47</v>
+      </c>
+      <c r="L126" t="s">
+        <v>103</v>
+      </c>
+      <c r="M126" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>1855</v>
+      </c>
+      <c r="B127">
+        <v>36</v>
+      </c>
+      <c r="C127" t="s">
+        <v>134</v>
+      </c>
+      <c r="J127" t="s">
+        <v>99</v>
+      </c>
+      <c r="K127">
+        <v>47</v>
+      </c>
+      <c r="L127" t="s">
+        <v>103</v>
+      </c>
+      <c r="M127" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>1855</v>
+      </c>
+      <c r="B128">
+        <v>37</v>
+      </c>
+      <c r="C128" t="s">
+        <v>135</v>
+      </c>
+      <c r="J128" t="s">
+        <v>99</v>
+      </c>
+      <c r="K128">
+        <v>47</v>
+      </c>
+      <c r="L128" t="s">
+        <v>103</v>
+      </c>
+      <c r="M128" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>1855</v>
+      </c>
+      <c r="B129">
+        <v>38</v>
+      </c>
+      <c r="C129" t="s">
+        <v>136</v>
+      </c>
+      <c r="J129" t="s">
+        <v>99</v>
+      </c>
+      <c r="K129">
+        <v>47</v>
+      </c>
+      <c r="L129" t="s">
+        <v>103</v>
+      </c>
+      <c r="M129" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>1855</v>
+      </c>
+      <c r="B130">
+        <v>39</v>
+      </c>
+      <c r="C130" t="s">
+        <v>137</v>
+      </c>
+      <c r="J130" t="s">
+        <v>99</v>
+      </c>
+      <c r="K130">
+        <v>47</v>
+      </c>
+      <c r="L130" t="s">
+        <v>103</v>
+      </c>
+      <c r="M130" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>1856</v>
+      </c>
+      <c r="B131">
+        <v>40</v>
+      </c>
+      <c r="C131" t="s">
+        <v>138</v>
+      </c>
+      <c r="J131" t="s">
+        <v>99</v>
+      </c>
+      <c r="K131">
+        <v>47</v>
+      </c>
+      <c r="L131" t="s">
+        <v>103</v>
+      </c>
+      <c r="M131" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>1856</v>
+      </c>
+      <c r="B132">
+        <v>41</v>
+      </c>
+      <c r="C132" t="s">
+        <v>139</v>
+      </c>
+      <c r="J132" t="s">
+        <v>99</v>
+      </c>
+      <c r="K132">
+        <v>47</v>
+      </c>
+      <c r="L132" t="s">
+        <v>103</v>
+      </c>
+      <c r="M132" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>1856</v>
+      </c>
+      <c r="B133">
+        <v>41</v>
+      </c>
+      <c r="C133" t="s">
+        <v>140</v>
+      </c>
+      <c r="J133" t="s">
+        <v>99</v>
+      </c>
+      <c r="K133">
+        <v>47</v>
+      </c>
+      <c r="L133" t="s">
+        <v>103</v>
+      </c>
+      <c r="M133" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>1856</v>
+      </c>
+      <c r="B134">
+        <v>42</v>
+      </c>
+      <c r="C134" t="s">
+        <v>141</v>
+      </c>
+      <c r="J134" t="s">
+        <v>99</v>
+      </c>
+      <c r="K134">
+        <v>47</v>
+      </c>
+      <c r="L134" t="s">
+        <v>103</v>
+      </c>
+      <c r="M134" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>1856</v>
+      </c>
+      <c r="B135">
+        <v>42</v>
+      </c>
+      <c r="C135" t="s">
+        <v>87</v>
+      </c>
+      <c r="J135" t="s">
+        <v>99</v>
+      </c>
+      <c r="K135">
+        <v>47</v>
+      </c>
+      <c r="L135" t="s">
+        <v>103</v>
+      </c>
+      <c r="M135" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>1856</v>
+      </c>
+      <c r="B136">
+        <v>43</v>
+      </c>
+      <c r="C136" t="s">
+        <v>142</v>
+      </c>
+      <c r="J136" t="s">
+        <v>99</v>
+      </c>
+      <c r="K136">
+        <v>47</v>
+      </c>
+      <c r="L136" t="s">
+        <v>103</v>
+      </c>
+      <c r="M136" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>1856</v>
+      </c>
+      <c r="B137">
+        <v>43</v>
+      </c>
+      <c r="C137" t="s">
+        <v>143</v>
+      </c>
+      <c r="J137" t="s">
+        <v>99</v>
+      </c>
+      <c r="K137">
+        <v>47</v>
+      </c>
+      <c r="L137" t="s">
+        <v>103</v>
+      </c>
+      <c r="M137" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>1856</v>
+      </c>
+      <c r="B138">
+        <v>44</v>
+      </c>
+      <c r="C138" t="s">
+        <v>144</v>
+      </c>
+      <c r="J138" t="s">
+        <v>99</v>
+      </c>
+      <c r="K138">
+        <v>47</v>
+      </c>
+      <c r="L138" t="s">
+        <v>103</v>
+      </c>
+      <c r="M138" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>1856</v>
+      </c>
+      <c r="B139">
+        <v>44</v>
+      </c>
+      <c r="C139" t="s">
+        <v>145</v>
+      </c>
+      <c r="J139" t="s">
+        <v>99</v>
+      </c>
+      <c r="K139">
+        <v>47</v>
+      </c>
+      <c r="L139" t="s">
+        <v>103</v>
+      </c>
+      <c r="M139" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>1856</v>
+      </c>
+      <c r="B140">
+        <v>45</v>
+      </c>
+      <c r="C140" t="s">
+        <v>146</v>
+      </c>
+      <c r="J140" t="s">
+        <v>99</v>
+      </c>
+      <c r="K140">
+        <v>47</v>
+      </c>
+      <c r="L140" t="s">
+        <v>103</v>
+      </c>
+      <c r="M140" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>1856</v>
+      </c>
+      <c r="B141">
+        <v>45</v>
+      </c>
+      <c r="C141" t="s">
+        <v>147</v>
+      </c>
+      <c r="J141" t="s">
+        <v>99</v>
+      </c>
+      <c r="K141">
+        <v>47</v>
+      </c>
+      <c r="L141" t="s">
+        <v>103</v>
+      </c>
+      <c r="M141" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>1856</v>
+      </c>
+      <c r="B142">
+        <v>46</v>
+      </c>
+      <c r="C142" t="s">
+        <v>148</v>
+      </c>
+      <c r="J142" t="s">
+        <v>99</v>
+      </c>
+      <c r="K142">
+        <v>47</v>
+      </c>
+      <c r="L142" t="s">
+        <v>103</v>
+      </c>
+      <c r="M142" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>1856</v>
+      </c>
+      <c r="B143">
+        <v>46</v>
+      </c>
+      <c r="C143" t="s">
+        <v>149</v>
+      </c>
+      <c r="J143" t="s">
+        <v>99</v>
+      </c>
+      <c r="K143">
+        <v>47</v>
+      </c>
+      <c r="L143" t="s">
+        <v>103</v>
+      </c>
+      <c r="M143" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
indexació de cognoms del llibre de matrimonis Linyola anys 1814-1851 fins al fotograma 20 de 109
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Matrimonis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA04F7E8-D9D8-4B59-8594-7E59023EEBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAEBA10-D168-4956-87CA-99B2B95D9B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C34A0C26-324D-4E17-B7B1-6D7DB0FCFBF8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="195">
   <si>
     <t>Cognoms Familia</t>
   </si>
@@ -489,6 +489,141 @@
   </si>
   <si>
     <t>Torra Civit</t>
+  </si>
+  <si>
+    <t>1814-1851</t>
+  </si>
+  <si>
+    <t>A,4</t>
+  </si>
+  <si>
+    <t>Margall Busquets</t>
+  </si>
+  <si>
+    <t>Vilamajor Civit</t>
+  </si>
+  <si>
+    <t>Vilamajor Codina</t>
+  </si>
+  <si>
+    <t>Vinaixa Cascalló</t>
+  </si>
+  <si>
+    <t>Batlle Asqueró</t>
+  </si>
+  <si>
+    <t>Bellet Martí</t>
+  </si>
+  <si>
+    <t>Solsona Jovells</t>
+  </si>
+  <si>
+    <t>Vilaplana Civit</t>
+  </si>
+  <si>
+    <t>Ariatós Giné</t>
+  </si>
+  <si>
+    <t>Roiger Caelles</t>
+  </si>
+  <si>
+    <t>Lamarca Vergé</t>
+  </si>
+  <si>
+    <t>Bertran Farré</t>
+  </si>
+  <si>
+    <t>Ponsarnau Torrent</t>
+  </si>
+  <si>
+    <t>Novell Soler</t>
+  </si>
+  <si>
+    <t>Civit Carrera</t>
+  </si>
+  <si>
+    <t>Boldú Violant</t>
+  </si>
+  <si>
+    <t>Soler Giné</t>
+  </si>
+  <si>
+    <t>Bresolí Cascalló</t>
+  </si>
+  <si>
+    <t>Trepat Giner</t>
+  </si>
+  <si>
+    <t>Giné Pedrós</t>
+  </si>
+  <si>
+    <t>Novell Torrent</t>
+  </si>
+  <si>
+    <t>Berniell Gené</t>
+  </si>
+  <si>
+    <t>Niubó Martí</t>
+  </si>
+  <si>
+    <t>Llas Espervé</t>
+  </si>
+  <si>
+    <t>Sucarrat Mirassó</t>
+  </si>
+  <si>
+    <t>Torrent Cascalló</t>
+  </si>
+  <si>
+    <t>Font Coll</t>
+  </si>
+  <si>
+    <t>Capdevila Mas</t>
+  </si>
+  <si>
+    <t>Soler Mas</t>
+  </si>
+  <si>
+    <t>Rossell Agulló</t>
+  </si>
+  <si>
+    <t>Ginestà Mosset</t>
+  </si>
+  <si>
+    <t>Oromi Roma</t>
+  </si>
+  <si>
+    <t>Mas Viladebait</t>
+  </si>
+  <si>
+    <t>Martí Batlle</t>
+  </si>
+  <si>
+    <t>Cisteré Mosset</t>
+  </si>
+  <si>
+    <t>Planes Pallaas</t>
+  </si>
+  <si>
+    <t>Roig Coll</t>
+  </si>
+  <si>
+    <t>Monyart Bellera</t>
+  </si>
+  <si>
+    <t>Agulló Calderó</t>
+  </si>
+  <si>
+    <t>Civit Mas</t>
+  </si>
+  <si>
+    <t>Batlle Pujol</t>
+  </si>
+  <si>
+    <t>Caelles Mata</t>
+  </si>
+  <si>
+    <t>Mas Bobé</t>
   </si>
 </sst>
 </file>
@@ -840,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}">
-  <dimension ref="A1:M143"/>
+  <dimension ref="A1:M187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="A188" sqref="A188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4165,6 +4300,1018 @@
         <v>102</v>
       </c>
     </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>1814</v>
+      </c>
+      <c r="B144">
+        <v>3</v>
+      </c>
+      <c r="C144" t="s">
+        <v>152</v>
+      </c>
+      <c r="J144" t="s">
+        <v>99</v>
+      </c>
+      <c r="K144">
+        <v>47</v>
+      </c>
+      <c r="L144" t="s">
+        <v>151</v>
+      </c>
+      <c r="M144" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>1814</v>
+      </c>
+      <c r="B145">
+        <v>3</v>
+      </c>
+      <c r="C145" t="s">
+        <v>153</v>
+      </c>
+      <c r="J145" t="s">
+        <v>99</v>
+      </c>
+      <c r="K145">
+        <v>47</v>
+      </c>
+      <c r="L145" t="s">
+        <v>151</v>
+      </c>
+      <c r="M145" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>1814</v>
+      </c>
+      <c r="B146">
+        <v>4</v>
+      </c>
+      <c r="C146" t="s">
+        <v>154</v>
+      </c>
+      <c r="J146" t="s">
+        <v>99</v>
+      </c>
+      <c r="K146">
+        <v>47</v>
+      </c>
+      <c r="L146" t="s">
+        <v>151</v>
+      </c>
+      <c r="M146" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>1814</v>
+      </c>
+      <c r="B147">
+        <v>4</v>
+      </c>
+      <c r="C147" t="s">
+        <v>155</v>
+      </c>
+      <c r="J147" t="s">
+        <v>99</v>
+      </c>
+      <c r="K147">
+        <v>47</v>
+      </c>
+      <c r="L147" t="s">
+        <v>151</v>
+      </c>
+      <c r="M147" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>1814</v>
+      </c>
+      <c r="B148">
+        <v>4</v>
+      </c>
+      <c r="C148" t="s">
+        <v>156</v>
+      </c>
+      <c r="J148" t="s">
+        <v>99</v>
+      </c>
+      <c r="K148">
+        <v>47</v>
+      </c>
+      <c r="L148" t="s">
+        <v>151</v>
+      </c>
+      <c r="M148" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>1814</v>
+      </c>
+      <c r="B149">
+        <v>5</v>
+      </c>
+      <c r="C149" t="s">
+        <v>157</v>
+      </c>
+      <c r="J149" t="s">
+        <v>99</v>
+      </c>
+      <c r="K149">
+        <v>47</v>
+      </c>
+      <c r="L149" t="s">
+        <v>151</v>
+      </c>
+      <c r="M149" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>1814</v>
+      </c>
+      <c r="B150">
+        <v>5</v>
+      </c>
+      <c r="C150" t="s">
+        <v>158</v>
+      </c>
+      <c r="J150" t="s">
+        <v>99</v>
+      </c>
+      <c r="K150">
+        <v>47</v>
+      </c>
+      <c r="L150" t="s">
+        <v>151</v>
+      </c>
+      <c r="M150" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>1814</v>
+      </c>
+      <c r="B151">
+        <v>5</v>
+      </c>
+      <c r="C151" t="s">
+        <v>159</v>
+      </c>
+      <c r="J151" t="s">
+        <v>99</v>
+      </c>
+      <c r="K151">
+        <v>47</v>
+      </c>
+      <c r="L151" t="s">
+        <v>151</v>
+      </c>
+      <c r="M151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>1814</v>
+      </c>
+      <c r="B152">
+        <v>6</v>
+      </c>
+      <c r="C152" t="s">
+        <v>160</v>
+      </c>
+      <c r="J152" t="s">
+        <v>99</v>
+      </c>
+      <c r="K152">
+        <v>47</v>
+      </c>
+      <c r="L152" t="s">
+        <v>151</v>
+      </c>
+      <c r="M152" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>1815</v>
+      </c>
+      <c r="B153">
+        <v>6</v>
+      </c>
+      <c r="C153" t="s">
+        <v>161</v>
+      </c>
+      <c r="J153" t="s">
+        <v>99</v>
+      </c>
+      <c r="K153">
+        <v>47</v>
+      </c>
+      <c r="L153" t="s">
+        <v>151</v>
+      </c>
+      <c r="M153" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>1815</v>
+      </c>
+      <c r="B154">
+        <v>6</v>
+      </c>
+      <c r="C154" t="s">
+        <v>162</v>
+      </c>
+      <c r="J154" t="s">
+        <v>99</v>
+      </c>
+      <c r="K154">
+        <v>47</v>
+      </c>
+      <c r="L154" t="s">
+        <v>151</v>
+      </c>
+      <c r="M154" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>1815</v>
+      </c>
+      <c r="B155">
+        <v>7</v>
+      </c>
+      <c r="C155" t="s">
+        <v>163</v>
+      </c>
+      <c r="J155" t="s">
+        <v>99</v>
+      </c>
+      <c r="K155">
+        <v>47</v>
+      </c>
+      <c r="L155" t="s">
+        <v>151</v>
+      </c>
+      <c r="M155" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>1816</v>
+      </c>
+      <c r="B156">
+        <v>7</v>
+      </c>
+      <c r="C156" t="s">
+        <v>164</v>
+      </c>
+      <c r="J156" t="s">
+        <v>99</v>
+      </c>
+      <c r="K156">
+        <v>47</v>
+      </c>
+      <c r="L156" t="s">
+        <v>151</v>
+      </c>
+      <c r="M156" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>1816</v>
+      </c>
+      <c r="B157">
+        <v>8</v>
+      </c>
+      <c r="C157" t="s">
+        <v>165</v>
+      </c>
+      <c r="J157" t="s">
+        <v>99</v>
+      </c>
+      <c r="K157">
+        <v>47</v>
+      </c>
+      <c r="L157" t="s">
+        <v>151</v>
+      </c>
+      <c r="M157" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>1816</v>
+      </c>
+      <c r="B158">
+        <v>8</v>
+      </c>
+      <c r="C158" t="s">
+        <v>166</v>
+      </c>
+      <c r="J158" t="s">
+        <v>99</v>
+      </c>
+      <c r="K158">
+        <v>47</v>
+      </c>
+      <c r="L158" t="s">
+        <v>151</v>
+      </c>
+      <c r="M158" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>1816</v>
+      </c>
+      <c r="B159">
+        <v>8</v>
+      </c>
+      <c r="C159" t="s">
+        <v>167</v>
+      </c>
+      <c r="J159" t="s">
+        <v>99</v>
+      </c>
+      <c r="K159">
+        <v>47</v>
+      </c>
+      <c r="L159" t="s">
+        <v>151</v>
+      </c>
+      <c r="M159" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>1816</v>
+      </c>
+      <c r="B160">
+        <v>9</v>
+      </c>
+      <c r="C160" t="s">
+        <v>168</v>
+      </c>
+      <c r="J160" t="s">
+        <v>99</v>
+      </c>
+      <c r="K160">
+        <v>47</v>
+      </c>
+      <c r="L160" t="s">
+        <v>151</v>
+      </c>
+      <c r="M160" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>1816</v>
+      </c>
+      <c r="B161">
+        <v>9</v>
+      </c>
+      <c r="C161" t="s">
+        <v>169</v>
+      </c>
+      <c r="J161" t="s">
+        <v>99</v>
+      </c>
+      <c r="K161">
+        <v>47</v>
+      </c>
+      <c r="L161" t="s">
+        <v>151</v>
+      </c>
+      <c r="M161" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>1816</v>
+      </c>
+      <c r="B162">
+        <v>10</v>
+      </c>
+      <c r="C162" t="s">
+        <v>170</v>
+      </c>
+      <c r="J162" t="s">
+        <v>99</v>
+      </c>
+      <c r="K162">
+        <v>47</v>
+      </c>
+      <c r="L162" t="s">
+        <v>151</v>
+      </c>
+      <c r="M162" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>1816</v>
+      </c>
+      <c r="B163">
+        <v>10</v>
+      </c>
+      <c r="C163" t="s">
+        <v>171</v>
+      </c>
+      <c r="J163" t="s">
+        <v>99</v>
+      </c>
+      <c r="K163">
+        <v>47</v>
+      </c>
+      <c r="L163" t="s">
+        <v>151</v>
+      </c>
+      <c r="M163" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>1816</v>
+      </c>
+      <c r="B164">
+        <v>11</v>
+      </c>
+      <c r="C164" t="s">
+        <v>172</v>
+      </c>
+      <c r="J164" t="s">
+        <v>99</v>
+      </c>
+      <c r="K164">
+        <v>47</v>
+      </c>
+      <c r="L164" t="s">
+        <v>151</v>
+      </c>
+      <c r="M164" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>1817</v>
+      </c>
+      <c r="B165">
+        <v>11</v>
+      </c>
+      <c r="C165" t="s">
+        <v>75</v>
+      </c>
+      <c r="J165" t="s">
+        <v>99</v>
+      </c>
+      <c r="K165">
+        <v>47</v>
+      </c>
+      <c r="L165" t="s">
+        <v>151</v>
+      </c>
+      <c r="M165" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>1817</v>
+      </c>
+      <c r="B166">
+        <v>11</v>
+      </c>
+      <c r="C166" t="s">
+        <v>173</v>
+      </c>
+      <c r="J166" t="s">
+        <v>99</v>
+      </c>
+      <c r="K166">
+        <v>47</v>
+      </c>
+      <c r="L166" t="s">
+        <v>151</v>
+      </c>
+      <c r="M166" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>1817</v>
+      </c>
+      <c r="B167">
+        <v>12</v>
+      </c>
+      <c r="C167" t="s">
+        <v>174</v>
+      </c>
+      <c r="J167" t="s">
+        <v>99</v>
+      </c>
+      <c r="K167">
+        <v>47</v>
+      </c>
+      <c r="L167" t="s">
+        <v>151</v>
+      </c>
+      <c r="M167" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>1817</v>
+      </c>
+      <c r="B168">
+        <v>12</v>
+      </c>
+      <c r="C168" t="s">
+        <v>175</v>
+      </c>
+      <c r="J168" t="s">
+        <v>99</v>
+      </c>
+      <c r="K168">
+        <v>47</v>
+      </c>
+      <c r="L168" t="s">
+        <v>151</v>
+      </c>
+      <c r="M168" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>1817</v>
+      </c>
+      <c r="B169">
+        <v>13</v>
+      </c>
+      <c r="C169" t="s">
+        <v>176</v>
+      </c>
+      <c r="J169" t="s">
+        <v>99</v>
+      </c>
+      <c r="K169">
+        <v>47</v>
+      </c>
+      <c r="L169" t="s">
+        <v>151</v>
+      </c>
+      <c r="M169" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>1817</v>
+      </c>
+      <c r="B170">
+        <v>13</v>
+      </c>
+      <c r="C170" t="s">
+        <v>177</v>
+      </c>
+      <c r="J170" t="s">
+        <v>99</v>
+      </c>
+      <c r="K170">
+        <v>47</v>
+      </c>
+      <c r="L170" t="s">
+        <v>151</v>
+      </c>
+      <c r="M170" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>1817</v>
+      </c>
+      <c r="B171">
+        <v>14</v>
+      </c>
+      <c r="C171" t="s">
+        <v>178</v>
+      </c>
+      <c r="J171" t="s">
+        <v>99</v>
+      </c>
+      <c r="K171">
+        <v>47</v>
+      </c>
+      <c r="L171" t="s">
+        <v>151</v>
+      </c>
+      <c r="M171" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>1818</v>
+      </c>
+      <c r="B172">
+        <v>14</v>
+      </c>
+      <c r="C172" t="s">
+        <v>179</v>
+      </c>
+      <c r="J172" t="s">
+        <v>99</v>
+      </c>
+      <c r="K172">
+        <v>47</v>
+      </c>
+      <c r="L172" t="s">
+        <v>151</v>
+      </c>
+      <c r="M172" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>1818</v>
+      </c>
+      <c r="B173">
+        <v>14</v>
+      </c>
+      <c r="C173" t="s">
+        <v>180</v>
+      </c>
+      <c r="J173" t="s">
+        <v>99</v>
+      </c>
+      <c r="K173">
+        <v>47</v>
+      </c>
+      <c r="L173" t="s">
+        <v>151</v>
+      </c>
+      <c r="M173" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>1818</v>
+      </c>
+      <c r="B174">
+        <v>15</v>
+      </c>
+      <c r="C174" t="s">
+        <v>181</v>
+      </c>
+      <c r="J174" t="s">
+        <v>99</v>
+      </c>
+      <c r="K174">
+        <v>47</v>
+      </c>
+      <c r="L174" t="s">
+        <v>151</v>
+      </c>
+      <c r="M174" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>1818</v>
+      </c>
+      <c r="B175">
+        <v>15</v>
+      </c>
+      <c r="C175" t="s">
+        <v>182</v>
+      </c>
+      <c r="J175" t="s">
+        <v>99</v>
+      </c>
+      <c r="K175">
+        <v>47</v>
+      </c>
+      <c r="L175" t="s">
+        <v>151</v>
+      </c>
+      <c r="M175" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>1819</v>
+      </c>
+      <c r="B176">
+        <v>16</v>
+      </c>
+      <c r="C176" t="s">
+        <v>183</v>
+      </c>
+      <c r="J176" t="s">
+        <v>99</v>
+      </c>
+      <c r="K176">
+        <v>47</v>
+      </c>
+      <c r="L176" t="s">
+        <v>151</v>
+      </c>
+      <c r="M176" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>1819</v>
+      </c>
+      <c r="B177">
+        <v>16</v>
+      </c>
+      <c r="C177" t="s">
+        <v>184</v>
+      </c>
+      <c r="J177" t="s">
+        <v>99</v>
+      </c>
+      <c r="K177">
+        <v>47</v>
+      </c>
+      <c r="L177" t="s">
+        <v>151</v>
+      </c>
+      <c r="M177" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>1819</v>
+      </c>
+      <c r="B178">
+        <v>17</v>
+      </c>
+      <c r="C178" t="s">
+        <v>185</v>
+      </c>
+      <c r="J178" t="s">
+        <v>99</v>
+      </c>
+      <c r="K178">
+        <v>47</v>
+      </c>
+      <c r="L178" t="s">
+        <v>151</v>
+      </c>
+      <c r="M178" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>1819</v>
+      </c>
+      <c r="B179">
+        <v>17</v>
+      </c>
+      <c r="C179" t="s">
+        <v>186</v>
+      </c>
+      <c r="J179" t="s">
+        <v>99</v>
+      </c>
+      <c r="K179">
+        <v>47</v>
+      </c>
+      <c r="L179" t="s">
+        <v>151</v>
+      </c>
+      <c r="M179" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>1819</v>
+      </c>
+      <c r="B180">
+        <v>17</v>
+      </c>
+      <c r="C180" t="s">
+        <v>187</v>
+      </c>
+      <c r="J180" t="s">
+        <v>99</v>
+      </c>
+      <c r="K180">
+        <v>47</v>
+      </c>
+      <c r="L180" t="s">
+        <v>151</v>
+      </c>
+      <c r="M180" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>1819</v>
+      </c>
+      <c r="B181">
+        <v>18</v>
+      </c>
+      <c r="C181" t="s">
+        <v>188</v>
+      </c>
+      <c r="J181" t="s">
+        <v>99</v>
+      </c>
+      <c r="K181">
+        <v>47</v>
+      </c>
+      <c r="L181" t="s">
+        <v>151</v>
+      </c>
+      <c r="M181" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>1819</v>
+      </c>
+      <c r="B182">
+        <v>18</v>
+      </c>
+      <c r="C182" t="s">
+        <v>189</v>
+      </c>
+      <c r="J182" t="s">
+        <v>99</v>
+      </c>
+      <c r="K182">
+        <v>47</v>
+      </c>
+      <c r="L182" t="s">
+        <v>151</v>
+      </c>
+      <c r="M182" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>1820</v>
+      </c>
+      <c r="B183">
+        <v>19</v>
+      </c>
+      <c r="C183" t="s">
+        <v>190</v>
+      </c>
+      <c r="J183" t="s">
+        <v>99</v>
+      </c>
+      <c r="K183">
+        <v>47</v>
+      </c>
+      <c r="L183" t="s">
+        <v>151</v>
+      </c>
+      <c r="M183" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>1820</v>
+      </c>
+      <c r="B184">
+        <v>19</v>
+      </c>
+      <c r="C184" t="s">
+        <v>191</v>
+      </c>
+      <c r="J184" t="s">
+        <v>99</v>
+      </c>
+      <c r="K184">
+        <v>47</v>
+      </c>
+      <c r="L184" t="s">
+        <v>151</v>
+      </c>
+      <c r="M184" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>1820</v>
+      </c>
+      <c r="B185">
+        <v>19</v>
+      </c>
+      <c r="C185" t="s">
+        <v>192</v>
+      </c>
+      <c r="J185" t="s">
+        <v>99</v>
+      </c>
+      <c r="K185">
+        <v>47</v>
+      </c>
+      <c r="L185" t="s">
+        <v>151</v>
+      </c>
+      <c r="M185" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>1820</v>
+      </c>
+      <c r="B186">
+        <v>20</v>
+      </c>
+      <c r="C186" t="s">
+        <v>193</v>
+      </c>
+      <c r="J186" t="s">
+        <v>99</v>
+      </c>
+      <c r="K186">
+        <v>47</v>
+      </c>
+      <c r="L186" t="s">
+        <v>151</v>
+      </c>
+      <c r="M186" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>1820</v>
+      </c>
+      <c r="B187">
+        <v>20</v>
+      </c>
+      <c r="C187" t="s">
+        <v>194</v>
+      </c>
+      <c r="J187" t="s">
+        <v>99</v>
+      </c>
+      <c r="K187">
+        <v>47</v>
+      </c>
+      <c r="L187" t="s">
+        <v>151</v>
+      </c>
+      <c r="M187" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
indexant llibre matrimonis 1749-1770 fins pag 30
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Matrimonis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1925F9D1-2D61-455C-9867-2F7D198529FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F52D168-28E9-47C2-B92B-E40790628FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C34A0C26-324D-4E17-B7B1-6D7DB0FCFBF8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$M$646</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$M$715</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2892" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="769">
   <si>
     <t>Cognoms Familia</t>
   </si>
@@ -2181,6 +2181,171 @@
   </si>
   <si>
     <t>Llorens Pujol</t>
+  </si>
+  <si>
+    <t>1749-1770</t>
+  </si>
+  <si>
+    <t>A,2</t>
+  </si>
+  <si>
+    <t>Mas Martí</t>
+  </si>
+  <si>
+    <t>Incognit Planes</t>
+  </si>
+  <si>
+    <t>Civit Incognit</t>
+  </si>
+  <si>
+    <t>Marti Ginesta</t>
+  </si>
+  <si>
+    <t>Pedrós Rey</t>
+  </si>
+  <si>
+    <t>Puig Valles</t>
+  </si>
+  <si>
+    <t>Martí Solé</t>
+  </si>
+  <si>
+    <t>Corberó Thomas</t>
+  </si>
+  <si>
+    <t>Mas Planes</t>
+  </si>
+  <si>
+    <t>Tarragó Solà</t>
+  </si>
+  <si>
+    <t>Gene Arrufat</t>
+  </si>
+  <si>
+    <t>Martí Mas</t>
+  </si>
+  <si>
+    <t>Batlle Vergè</t>
+  </si>
+  <si>
+    <t>Civit Rossell</t>
+  </si>
+  <si>
+    <t>Senallosa Domingo</t>
+  </si>
+  <si>
+    <t>Vilaplana Vergé</t>
+  </si>
+  <si>
+    <t>Solà Mas</t>
+  </si>
+  <si>
+    <t>Cascalló Corberó</t>
+  </si>
+  <si>
+    <t>Duch Sucarrat</t>
+  </si>
+  <si>
+    <t>Gene Palou</t>
+  </si>
+  <si>
+    <t>Pedrós Felip</t>
+  </si>
+  <si>
+    <t>Trepat Valles</t>
+  </si>
+  <si>
+    <t>Martí Roma</t>
+  </si>
+  <si>
+    <t>Agulló Cases</t>
+  </si>
+  <si>
+    <t>Font Fortuny</t>
+  </si>
+  <si>
+    <t>Cascalló Ribes</t>
+  </si>
+  <si>
+    <t>Queral Vergé</t>
+  </si>
+  <si>
+    <t>Mata Senallosa</t>
+  </si>
+  <si>
+    <t>Cuberes Solsona</t>
+  </si>
+  <si>
+    <t>Tarroja Pujades</t>
+  </si>
+  <si>
+    <t>Falcó Mas</t>
+  </si>
+  <si>
+    <t>Falcó Torruella</t>
+  </si>
+  <si>
+    <t>Vergé Galceran</t>
+  </si>
+  <si>
+    <t>Pallas Pujal</t>
+  </si>
+  <si>
+    <t>Mas Torren</t>
+  </si>
+  <si>
+    <t>Dalmau Vallés</t>
+  </si>
+  <si>
+    <t>Coll Fabregat</t>
+  </si>
+  <si>
+    <t>Mosset Rubiol</t>
+  </si>
+  <si>
+    <t>Vergé Tapies</t>
+  </si>
+  <si>
+    <t>Civit Serra</t>
+  </si>
+  <si>
+    <t>Vergé Mas</t>
+  </si>
+  <si>
+    <t>Curcó Pujol</t>
+  </si>
+  <si>
+    <t>Pujol Roigé</t>
+  </si>
+  <si>
+    <t>Cascalló Druet</t>
+  </si>
+  <si>
+    <t>Mas Roige</t>
+  </si>
+  <si>
+    <t>Pujol Prats</t>
+  </si>
+  <si>
+    <t>Salvat Bonjorn</t>
+  </si>
+  <si>
+    <t>Torra Balagué</t>
+  </si>
+  <si>
+    <t>Sucarrat Pera</t>
+  </si>
+  <si>
+    <t>Mosset Codina</t>
+  </si>
+  <si>
+    <t>Ponsarnau Palou</t>
+  </si>
+  <si>
+    <t>Batalla Tarroja</t>
+  </si>
+  <si>
+    <t>vergé Mas</t>
   </si>
 </sst>
 </file>
@@ -2535,11 +2700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}">
-  <dimension ref="A1:N713"/>
+  <dimension ref="A1:N767"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A681" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A714" sqref="A714"/>
+      <pane ySplit="1" topLeftCell="A743" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A768" sqref="A768"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19055,8 +19220,1250 @@
         <v>398</v>
       </c>
     </row>
+    <row r="714" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A714">
+        <v>1749</v>
+      </c>
+      <c r="B714">
+        <v>3</v>
+      </c>
+      <c r="C714" t="s">
+        <v>716</v>
+      </c>
+      <c r="J714" t="s">
+        <v>99</v>
+      </c>
+      <c r="K714">
+        <v>47</v>
+      </c>
+      <c r="L714" t="s">
+        <v>715</v>
+      </c>
+      <c r="M714" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="715" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A715">
+        <v>1750</v>
+      </c>
+      <c r="B715">
+        <v>3</v>
+      </c>
+      <c r="C715" t="s">
+        <v>717</v>
+      </c>
+      <c r="J715" t="s">
+        <v>99</v>
+      </c>
+      <c r="K715">
+        <v>47</v>
+      </c>
+      <c r="L715" t="s">
+        <v>715</v>
+      </c>
+      <c r="M715" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="716" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A716">
+        <v>1750</v>
+      </c>
+      <c r="B716">
+        <v>4</v>
+      </c>
+      <c r="C716" t="s">
+        <v>718</v>
+      </c>
+      <c r="J716" t="s">
+        <v>99</v>
+      </c>
+      <c r="K716">
+        <v>47</v>
+      </c>
+      <c r="L716" t="s">
+        <v>715</v>
+      </c>
+      <c r="M716" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="717" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A717">
+        <v>1750</v>
+      </c>
+      <c r="B717">
+        <v>4</v>
+      </c>
+      <c r="C717" t="s">
+        <v>719</v>
+      </c>
+      <c r="J717" t="s">
+        <v>99</v>
+      </c>
+      <c r="K717">
+        <v>47</v>
+      </c>
+      <c r="L717" t="s">
+        <v>715</v>
+      </c>
+      <c r="M717" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="718" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A718">
+        <v>1751</v>
+      </c>
+      <c r="B718">
+        <v>5</v>
+      </c>
+      <c r="C718" t="s">
+        <v>720</v>
+      </c>
+      <c r="J718" t="s">
+        <v>99</v>
+      </c>
+      <c r="K718">
+        <v>47</v>
+      </c>
+      <c r="L718" t="s">
+        <v>715</v>
+      </c>
+      <c r="M718" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="719" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A719">
+        <v>1751</v>
+      </c>
+      <c r="B719">
+        <v>5</v>
+      </c>
+      <c r="C719" t="s">
+        <v>724</v>
+      </c>
+      <c r="J719" t="s">
+        <v>99</v>
+      </c>
+      <c r="K719">
+        <v>47</v>
+      </c>
+      <c r="L719" t="s">
+        <v>715</v>
+      </c>
+      <c r="M719" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="720" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A720">
+        <v>1751</v>
+      </c>
+      <c r="B720">
+        <v>5</v>
+      </c>
+      <c r="C720" t="s">
+        <v>721</v>
+      </c>
+      <c r="J720" t="s">
+        <v>99</v>
+      </c>
+      <c r="K720">
+        <v>47</v>
+      </c>
+      <c r="L720" t="s">
+        <v>715</v>
+      </c>
+      <c r="M720" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="721" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A721">
+        <v>1753</v>
+      </c>
+      <c r="B721">
+        <v>6</v>
+      </c>
+      <c r="C721" t="s">
+        <v>722</v>
+      </c>
+      <c r="J721" t="s">
+        <v>99</v>
+      </c>
+      <c r="K721">
+        <v>47</v>
+      </c>
+      <c r="L721" t="s">
+        <v>715</v>
+      </c>
+      <c r="M721" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="722" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A722">
+        <v>1753</v>
+      </c>
+      <c r="B722">
+        <v>6</v>
+      </c>
+      <c r="C722" t="s">
+        <v>723</v>
+      </c>
+      <c r="J722" t="s">
+        <v>99</v>
+      </c>
+      <c r="K722">
+        <v>47</v>
+      </c>
+      <c r="L722" t="s">
+        <v>715</v>
+      </c>
+      <c r="M722" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="723" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A723">
+        <v>1753</v>
+      </c>
+      <c r="B723">
+        <v>7</v>
+      </c>
+      <c r="C723" t="s">
+        <v>725</v>
+      </c>
+      <c r="J723" t="s">
+        <v>99</v>
+      </c>
+      <c r="K723">
+        <v>47</v>
+      </c>
+      <c r="L723" t="s">
+        <v>715</v>
+      </c>
+      <c r="M723" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="724" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A724">
+        <v>1753</v>
+      </c>
+      <c r="B724">
+        <v>7</v>
+      </c>
+      <c r="C724" t="s">
+        <v>726</v>
+      </c>
+      <c r="J724" t="s">
+        <v>99</v>
+      </c>
+      <c r="K724">
+        <v>47</v>
+      </c>
+      <c r="L724" t="s">
+        <v>715</v>
+      </c>
+      <c r="M724" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="725" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A725">
+        <v>1754</v>
+      </c>
+      <c r="B725">
+        <v>7</v>
+      </c>
+      <c r="C725" t="s">
+        <v>727</v>
+      </c>
+      <c r="J725" t="s">
+        <v>99</v>
+      </c>
+      <c r="K725">
+        <v>47</v>
+      </c>
+      <c r="L725" t="s">
+        <v>715</v>
+      </c>
+      <c r="M725" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="726" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A726">
+        <v>1754</v>
+      </c>
+      <c r="B726">
+        <v>8</v>
+      </c>
+      <c r="C726" t="s">
+        <v>728</v>
+      </c>
+      <c r="J726" t="s">
+        <v>99</v>
+      </c>
+      <c r="K726">
+        <v>47</v>
+      </c>
+      <c r="L726" t="s">
+        <v>715</v>
+      </c>
+      <c r="M726" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="727" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A727">
+        <v>1755</v>
+      </c>
+      <c r="B727">
+        <v>9</v>
+      </c>
+      <c r="C727" t="s">
+        <v>729</v>
+      </c>
+      <c r="J727" t="s">
+        <v>99</v>
+      </c>
+      <c r="K727">
+        <v>47</v>
+      </c>
+      <c r="L727" t="s">
+        <v>715</v>
+      </c>
+      <c r="M727" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="728" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A728">
+        <v>1755</v>
+      </c>
+      <c r="B728">
+        <v>9</v>
+      </c>
+      <c r="C728" t="s">
+        <v>730</v>
+      </c>
+      <c r="J728" t="s">
+        <v>99</v>
+      </c>
+      <c r="K728">
+        <v>47</v>
+      </c>
+      <c r="L728" t="s">
+        <v>715</v>
+      </c>
+      <c r="M728" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="729" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A729">
+        <v>1755</v>
+      </c>
+      <c r="B729">
+        <v>9</v>
+      </c>
+      <c r="C729" t="s">
+        <v>731</v>
+      </c>
+      <c r="J729" t="s">
+        <v>99</v>
+      </c>
+      <c r="K729">
+        <v>47</v>
+      </c>
+      <c r="L729" t="s">
+        <v>715</v>
+      </c>
+      <c r="M729" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="730" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A730">
+        <v>1755</v>
+      </c>
+      <c r="B730">
+        <v>10</v>
+      </c>
+      <c r="C730" t="s">
+        <v>732</v>
+      </c>
+      <c r="J730" t="s">
+        <v>99</v>
+      </c>
+      <c r="K730">
+        <v>47</v>
+      </c>
+      <c r="L730" t="s">
+        <v>715</v>
+      </c>
+      <c r="M730" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="731" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A731">
+        <v>1755</v>
+      </c>
+      <c r="B731">
+        <v>10</v>
+      </c>
+      <c r="C731" t="s">
+        <v>733</v>
+      </c>
+      <c r="J731" t="s">
+        <v>99</v>
+      </c>
+      <c r="K731">
+        <v>47</v>
+      </c>
+      <c r="L731" t="s">
+        <v>715</v>
+      </c>
+      <c r="M731" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="732" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A732">
+        <v>1756</v>
+      </c>
+      <c r="B732">
+        <v>10</v>
+      </c>
+      <c r="C732" t="s">
+        <v>734</v>
+      </c>
+      <c r="J732" t="s">
+        <v>99</v>
+      </c>
+      <c r="K732">
+        <v>47</v>
+      </c>
+      <c r="L732" t="s">
+        <v>715</v>
+      </c>
+      <c r="M732" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="733" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A733">
+        <v>1756</v>
+      </c>
+      <c r="B733">
+        <v>11</v>
+      </c>
+      <c r="C733" t="s">
+        <v>735</v>
+      </c>
+      <c r="J733" t="s">
+        <v>99</v>
+      </c>
+      <c r="K733">
+        <v>47</v>
+      </c>
+      <c r="L733" t="s">
+        <v>715</v>
+      </c>
+      <c r="M733" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="734" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A734">
+        <v>1756</v>
+      </c>
+      <c r="B734">
+        <v>11</v>
+      </c>
+      <c r="C734" t="s">
+        <v>736</v>
+      </c>
+      <c r="J734" t="s">
+        <v>99</v>
+      </c>
+      <c r="K734">
+        <v>47</v>
+      </c>
+      <c r="L734" t="s">
+        <v>715</v>
+      </c>
+      <c r="M734" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="735" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A735">
+        <v>1756</v>
+      </c>
+      <c r="B735">
+        <v>12</v>
+      </c>
+      <c r="C735" t="s">
+        <v>737</v>
+      </c>
+      <c r="J735" t="s">
+        <v>99</v>
+      </c>
+      <c r="K735">
+        <v>47</v>
+      </c>
+      <c r="L735" t="s">
+        <v>715</v>
+      </c>
+      <c r="M735" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="736" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A736">
+        <v>1756</v>
+      </c>
+      <c r="B736">
+        <v>12</v>
+      </c>
+      <c r="C736" t="s">
+        <v>738</v>
+      </c>
+      <c r="J736" t="s">
+        <v>99</v>
+      </c>
+      <c r="K736">
+        <v>47</v>
+      </c>
+      <c r="L736" t="s">
+        <v>715</v>
+      </c>
+      <c r="M736" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="737" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A737">
+        <v>1756</v>
+      </c>
+      <c r="B737">
+        <v>13</v>
+      </c>
+      <c r="C737" t="s">
+        <v>739</v>
+      </c>
+      <c r="J737" t="s">
+        <v>99</v>
+      </c>
+      <c r="K737">
+        <v>47</v>
+      </c>
+      <c r="L737" t="s">
+        <v>715</v>
+      </c>
+      <c r="M737" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="738" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A738">
+        <v>1756</v>
+      </c>
+      <c r="B738">
+        <v>13</v>
+      </c>
+      <c r="C738" t="s">
+        <v>740</v>
+      </c>
+      <c r="J738" t="s">
+        <v>99</v>
+      </c>
+      <c r="K738">
+        <v>47</v>
+      </c>
+      <c r="L738" t="s">
+        <v>715</v>
+      </c>
+      <c r="M738" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="739" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A739">
+        <v>1756</v>
+      </c>
+      <c r="B739">
+        <v>14</v>
+      </c>
+      <c r="C739" t="s">
+        <v>741</v>
+      </c>
+      <c r="J739" t="s">
+        <v>99</v>
+      </c>
+      <c r="K739">
+        <v>47</v>
+      </c>
+      <c r="L739" t="s">
+        <v>715</v>
+      </c>
+      <c r="M739" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="740" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A740">
+        <v>1757</v>
+      </c>
+      <c r="B740">
+        <v>14</v>
+      </c>
+      <c r="C740" t="s">
+        <v>742</v>
+      </c>
+      <c r="J740" t="s">
+        <v>99</v>
+      </c>
+      <c r="K740">
+        <v>47</v>
+      </c>
+      <c r="L740" t="s">
+        <v>715</v>
+      </c>
+      <c r="M740" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="741" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A741">
+        <v>1757</v>
+      </c>
+      <c r="B741">
+        <v>15</v>
+      </c>
+      <c r="C741" t="s">
+        <v>743</v>
+      </c>
+      <c r="J741" t="s">
+        <v>99</v>
+      </c>
+      <c r="K741">
+        <v>47</v>
+      </c>
+      <c r="L741" t="s">
+        <v>715</v>
+      </c>
+      <c r="M741" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="742" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A742">
+        <v>1757</v>
+      </c>
+      <c r="B742">
+        <v>15</v>
+      </c>
+      <c r="C742" t="s">
+        <v>744</v>
+      </c>
+      <c r="J742" t="s">
+        <v>99</v>
+      </c>
+      <c r="K742">
+        <v>47</v>
+      </c>
+      <c r="L742" t="s">
+        <v>715</v>
+      </c>
+      <c r="M742" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="743" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A743">
+        <v>1757</v>
+      </c>
+      <c r="B743">
+        <v>16</v>
+      </c>
+      <c r="C743" t="s">
+        <v>745</v>
+      </c>
+      <c r="J743" t="s">
+        <v>99</v>
+      </c>
+      <c r="K743">
+        <v>47</v>
+      </c>
+      <c r="L743" t="s">
+        <v>715</v>
+      </c>
+      <c r="M743" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="744" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A744">
+        <v>1757</v>
+      </c>
+      <c r="B744">
+        <v>16</v>
+      </c>
+      <c r="C744" t="s">
+        <v>746</v>
+      </c>
+      <c r="J744" t="s">
+        <v>99</v>
+      </c>
+      <c r="K744">
+        <v>47</v>
+      </c>
+      <c r="L744" t="s">
+        <v>715</v>
+      </c>
+      <c r="M744" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="745" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A745">
+        <v>1758</v>
+      </c>
+      <c r="B745">
+        <v>17</v>
+      </c>
+      <c r="C745" t="s">
+        <v>747</v>
+      </c>
+      <c r="J745" t="s">
+        <v>99</v>
+      </c>
+      <c r="K745">
+        <v>47</v>
+      </c>
+      <c r="L745" t="s">
+        <v>715</v>
+      </c>
+      <c r="M745" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="746" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A746">
+        <v>1758</v>
+      </c>
+      <c r="B746">
+        <v>17</v>
+      </c>
+      <c r="C746" t="s">
+        <v>748</v>
+      </c>
+      <c r="J746" t="s">
+        <v>99</v>
+      </c>
+      <c r="K746">
+        <v>47</v>
+      </c>
+      <c r="L746" t="s">
+        <v>715</v>
+      </c>
+      <c r="M746" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="747" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A747">
+        <v>1758</v>
+      </c>
+      <c r="B747">
+        <v>18</v>
+      </c>
+      <c r="C747" t="s">
+        <v>135</v>
+      </c>
+      <c r="J747" t="s">
+        <v>99</v>
+      </c>
+      <c r="K747">
+        <v>47</v>
+      </c>
+      <c r="L747" t="s">
+        <v>715</v>
+      </c>
+      <c r="M747" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="748" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A748">
+        <v>1758</v>
+      </c>
+      <c r="B748">
+        <v>18</v>
+      </c>
+      <c r="C748" t="s">
+        <v>749</v>
+      </c>
+      <c r="J748" t="s">
+        <v>99</v>
+      </c>
+      <c r="K748">
+        <v>47</v>
+      </c>
+      <c r="L748" t="s">
+        <v>715</v>
+      </c>
+      <c r="M748" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="749" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A749">
+        <v>1758</v>
+      </c>
+      <c r="B749">
+        <v>19</v>
+      </c>
+      <c r="C749" t="s">
+        <v>750</v>
+      </c>
+      <c r="J749" t="s">
+        <v>99</v>
+      </c>
+      <c r="K749">
+        <v>47</v>
+      </c>
+      <c r="L749" t="s">
+        <v>715</v>
+      </c>
+      <c r="M749" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="750" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A750">
+        <v>1758</v>
+      </c>
+      <c r="B750">
+        <v>19</v>
+      </c>
+      <c r="C750" t="s">
+        <v>751</v>
+      </c>
+      <c r="J750" t="s">
+        <v>99</v>
+      </c>
+      <c r="K750">
+        <v>47</v>
+      </c>
+      <c r="L750" t="s">
+        <v>715</v>
+      </c>
+      <c r="M750" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="751" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A751">
+        <v>1758</v>
+      </c>
+      <c r="B751">
+        <v>20</v>
+      </c>
+      <c r="C751" t="s">
+        <v>752</v>
+      </c>
+      <c r="J751" t="s">
+        <v>99</v>
+      </c>
+      <c r="K751">
+        <v>47</v>
+      </c>
+      <c r="L751" t="s">
+        <v>715</v>
+      </c>
+      <c r="M751" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="752" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A752">
+        <v>1758</v>
+      </c>
+      <c r="B752">
+        <v>20</v>
+      </c>
+      <c r="C752" t="s">
+        <v>753</v>
+      </c>
+      <c r="J752" t="s">
+        <v>99</v>
+      </c>
+      <c r="K752">
+        <v>47</v>
+      </c>
+      <c r="L752" t="s">
+        <v>715</v>
+      </c>
+      <c r="M752" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="753" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A753">
+        <v>1758</v>
+      </c>
+      <c r="B753">
+        <v>21</v>
+      </c>
+      <c r="C753" t="s">
+        <v>754</v>
+      </c>
+      <c r="J753" t="s">
+        <v>99</v>
+      </c>
+      <c r="K753">
+        <v>47</v>
+      </c>
+      <c r="L753" t="s">
+        <v>715</v>
+      </c>
+      <c r="M753" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="754" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A754">
+        <v>1759</v>
+      </c>
+      <c r="B754">
+        <v>22</v>
+      </c>
+      <c r="C754" t="s">
+        <v>755</v>
+      </c>
+      <c r="J754" t="s">
+        <v>99</v>
+      </c>
+      <c r="K754">
+        <v>47</v>
+      </c>
+      <c r="L754" t="s">
+        <v>715</v>
+      </c>
+      <c r="M754" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="755" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A755">
+        <v>1759</v>
+      </c>
+      <c r="B755">
+        <v>22</v>
+      </c>
+      <c r="C755" t="s">
+        <v>756</v>
+      </c>
+      <c r="J755" t="s">
+        <v>99</v>
+      </c>
+      <c r="K755">
+        <v>47</v>
+      </c>
+      <c r="L755" t="s">
+        <v>715</v>
+      </c>
+      <c r="M755" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="756" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A756">
+        <v>1759</v>
+      </c>
+      <c r="B756">
+        <v>23</v>
+      </c>
+      <c r="C756" t="s">
+        <v>757</v>
+      </c>
+      <c r="J756" t="s">
+        <v>99</v>
+      </c>
+      <c r="K756">
+        <v>47</v>
+      </c>
+      <c r="L756" t="s">
+        <v>715</v>
+      </c>
+      <c r="M756" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="757" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A757">
+        <v>1759</v>
+      </c>
+      <c r="B757">
+        <v>23</v>
+      </c>
+      <c r="C757" t="s">
+        <v>758</v>
+      </c>
+      <c r="J757" t="s">
+        <v>99</v>
+      </c>
+      <c r="K757">
+        <v>47</v>
+      </c>
+      <c r="L757" t="s">
+        <v>715</v>
+      </c>
+      <c r="M757" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="758" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A758">
+        <v>1759</v>
+      </c>
+      <c r="B758">
+        <v>24</v>
+      </c>
+      <c r="C758" t="s">
+        <v>759</v>
+      </c>
+      <c r="J758" t="s">
+        <v>99</v>
+      </c>
+      <c r="K758">
+        <v>47</v>
+      </c>
+      <c r="L758" t="s">
+        <v>715</v>
+      </c>
+      <c r="M758" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="759" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A759">
+        <v>1759</v>
+      </c>
+      <c r="B759">
+        <v>24</v>
+      </c>
+      <c r="C759" t="s">
+        <v>760</v>
+      </c>
+      <c r="J759" t="s">
+        <v>99</v>
+      </c>
+      <c r="K759">
+        <v>47</v>
+      </c>
+      <c r="L759" t="s">
+        <v>715</v>
+      </c>
+      <c r="M759" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="760" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A760">
+        <v>1759</v>
+      </c>
+      <c r="B760">
+        <v>25</v>
+      </c>
+      <c r="C760" t="s">
+        <v>761</v>
+      </c>
+      <c r="J760" t="s">
+        <v>99</v>
+      </c>
+      <c r="K760">
+        <v>47</v>
+      </c>
+      <c r="L760" t="s">
+        <v>715</v>
+      </c>
+      <c r="M760" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="761" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A761">
+        <v>1759</v>
+      </c>
+      <c r="B761">
+        <v>25</v>
+      </c>
+      <c r="C761" t="s">
+        <v>762</v>
+      </c>
+      <c r="J761" t="s">
+        <v>99</v>
+      </c>
+      <c r="K761">
+        <v>47</v>
+      </c>
+      <c r="L761" t="s">
+        <v>715</v>
+      </c>
+      <c r="M761" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="762" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A762">
+        <v>1760</v>
+      </c>
+      <c r="B762">
+        <v>26</v>
+      </c>
+      <c r="C762" t="s">
+        <v>763</v>
+      </c>
+      <c r="J762" t="s">
+        <v>99</v>
+      </c>
+      <c r="K762">
+        <v>47</v>
+      </c>
+      <c r="L762" t="s">
+        <v>715</v>
+      </c>
+      <c r="M762" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="763" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A763">
+        <v>1761</v>
+      </c>
+      <c r="B763">
+        <v>28</v>
+      </c>
+      <c r="C763" t="s">
+        <v>764</v>
+      </c>
+      <c r="J763" t="s">
+        <v>99</v>
+      </c>
+      <c r="K763">
+        <v>47</v>
+      </c>
+      <c r="L763" t="s">
+        <v>715</v>
+      </c>
+      <c r="M763" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="764" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A764">
+        <v>1761</v>
+      </c>
+      <c r="B764">
+        <v>28</v>
+      </c>
+      <c r="C764" t="s">
+        <v>765</v>
+      </c>
+      <c r="J764" t="s">
+        <v>99</v>
+      </c>
+      <c r="K764">
+        <v>47</v>
+      </c>
+      <c r="L764" t="s">
+        <v>715</v>
+      </c>
+      <c r="M764" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="765" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A765">
+        <v>1761</v>
+      </c>
+      <c r="B765">
+        <v>29</v>
+      </c>
+      <c r="C765" t="s">
+        <v>766</v>
+      </c>
+      <c r="J765" t="s">
+        <v>99</v>
+      </c>
+      <c r="K765">
+        <v>47</v>
+      </c>
+      <c r="L765" t="s">
+        <v>715</v>
+      </c>
+      <c r="M765" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="766" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A766">
+        <v>1761</v>
+      </c>
+      <c r="B766">
+        <v>29</v>
+      </c>
+      <c r="C766" t="s">
+        <v>767</v>
+      </c>
+      <c r="J766" t="s">
+        <v>99</v>
+      </c>
+      <c r="K766">
+        <v>47</v>
+      </c>
+      <c r="L766" t="s">
+        <v>715</v>
+      </c>
+      <c r="M766" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="767" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A767">
+        <v>1761</v>
+      </c>
+      <c r="B767">
+        <v>30</v>
+      </c>
+      <c r="C767" t="s">
+        <v>768</v>
+      </c>
+      <c r="J767" t="s">
+        <v>99</v>
+      </c>
+      <c r="K767">
+        <v>47</v>
+      </c>
+      <c r="L767" t="s">
+        <v>715</v>
+      </c>
+      <c r="M767" t="s">
+        <v>714</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M646" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}"/>
+  <autoFilter ref="A1:M715" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
afegint indexacio matrimonis Linyola
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Matrimonis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F52D168-28E9-47C2-B92B-E40790628FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C876939-D1A2-46E3-B291-769FF02088BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C34A0C26-324D-4E17-B7B1-6D7DB0FCFBF8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3280" uniqueCount="807">
   <si>
     <t>Cognoms Familia</t>
   </si>
@@ -2346,6 +2346,120 @@
   </si>
   <si>
     <t>vergé Mas</t>
+  </si>
+  <si>
+    <t>Roige Pons</t>
+  </si>
+  <si>
+    <t>Repetit</t>
+  </si>
+  <si>
+    <t>Valles Massot</t>
+  </si>
+  <si>
+    <t>Segura Palou</t>
+  </si>
+  <si>
+    <t>Druet Pujades</t>
+  </si>
+  <si>
+    <t>Domingo Pera</t>
+  </si>
+  <si>
+    <t>Solsona Melé</t>
+  </si>
+  <si>
+    <t>Roma Redon</t>
+  </si>
+  <si>
+    <t>Vallés Fabregat</t>
+  </si>
+  <si>
+    <t>Pujol Pedrós</t>
+  </si>
+  <si>
+    <t>Batalla Margall</t>
+  </si>
+  <si>
+    <t>Cascalló Pujades</t>
+  </si>
+  <si>
+    <t>Manyach Mas</t>
+  </si>
+  <si>
+    <t>Torrà Eroles</t>
+  </si>
+  <si>
+    <t>Vergé Codina</t>
+  </si>
+  <si>
+    <t>Viladebaix Solà</t>
+  </si>
+  <si>
+    <t>Claverol Siriols</t>
+  </si>
+  <si>
+    <t>Palou Vergé</t>
+  </si>
+  <si>
+    <t>Sabater Valles</t>
+  </si>
+  <si>
+    <t>Mas Thomas</t>
+  </si>
+  <si>
+    <t>Roma Oriola</t>
+  </si>
+  <si>
+    <t>Duart Alexandre</t>
+  </si>
+  <si>
+    <t>Homs Cascalló</t>
+  </si>
+  <si>
+    <t>Navau Santesmases</t>
+  </si>
+  <si>
+    <t>Galceran Rodon</t>
+  </si>
+  <si>
+    <t>Vergé Thomas</t>
+  </si>
+  <si>
+    <t>Roma Vallés</t>
+  </si>
+  <si>
+    <t>Bonjorn Domenech</t>
+  </si>
+  <si>
+    <t>Gine Serra</t>
+  </si>
+  <si>
+    <t>Claverol Roca</t>
+  </si>
+  <si>
+    <t>Carrera Galceran</t>
+  </si>
+  <si>
+    <t>Cases Mas</t>
+  </si>
+  <si>
+    <t>Gispert Agulló</t>
+  </si>
+  <si>
+    <t>Pilfort Teixidó</t>
+  </si>
+  <si>
+    <t>Sunyé Fabregat</t>
+  </si>
+  <si>
+    <t>Mas Giné</t>
+  </si>
+  <si>
+    <t>Pujades Porta</t>
+  </si>
+  <si>
+    <t>Codol ?</t>
   </si>
 </sst>
 </file>
@@ -2700,11 +2814,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}">
-  <dimension ref="A1:N767"/>
+  <dimension ref="A1:N810"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A743" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A768" sqref="A768"/>
+      <pane ySplit="1" topLeftCell="A794" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A811" sqref="A811"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20462,6 +20576,995 @@
         <v>714</v>
       </c>
     </row>
+    <row r="768" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A768">
+        <v>1761</v>
+      </c>
+      <c r="B768">
+        <v>31</v>
+      </c>
+      <c r="C768" t="s">
+        <v>769</v>
+      </c>
+      <c r="J768" t="s">
+        <v>99</v>
+      </c>
+      <c r="K768">
+        <v>47</v>
+      </c>
+      <c r="L768" t="s">
+        <v>715</v>
+      </c>
+      <c r="M768" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="769" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A769">
+        <v>1761</v>
+      </c>
+      <c r="B769">
+        <v>31</v>
+      </c>
+      <c r="C769" t="s">
+        <v>724</v>
+      </c>
+      <c r="J769" t="s">
+        <v>99</v>
+      </c>
+      <c r="K769">
+        <v>47</v>
+      </c>
+      <c r="L769" t="s">
+        <v>715</v>
+      </c>
+      <c r="M769" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="770" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A770">
+        <v>1761</v>
+      </c>
+      <c r="B770">
+        <v>32</v>
+      </c>
+      <c r="C770" t="s">
+        <v>770</v>
+      </c>
+      <c r="J770" t="s">
+        <v>99</v>
+      </c>
+      <c r="K770">
+        <v>47</v>
+      </c>
+      <c r="L770" t="s">
+        <v>715</v>
+      </c>
+      <c r="M770" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="771" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A771">
+        <v>1761</v>
+      </c>
+      <c r="B771">
+        <v>33</v>
+      </c>
+      <c r="C771" t="s">
+        <v>771</v>
+      </c>
+      <c r="J771" t="s">
+        <v>99</v>
+      </c>
+      <c r="K771">
+        <v>47</v>
+      </c>
+      <c r="L771" t="s">
+        <v>715</v>
+      </c>
+      <c r="M771" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="772" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A772">
+        <v>1761</v>
+      </c>
+      <c r="B772">
+        <v>33</v>
+      </c>
+      <c r="C772" t="s">
+        <v>772</v>
+      </c>
+      <c r="J772" t="s">
+        <v>99</v>
+      </c>
+      <c r="K772">
+        <v>47</v>
+      </c>
+      <c r="L772" t="s">
+        <v>715</v>
+      </c>
+      <c r="M772" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="773" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A773">
+        <v>1761</v>
+      </c>
+      <c r="B773">
+        <v>34</v>
+      </c>
+      <c r="C773" t="s">
+        <v>773</v>
+      </c>
+      <c r="J773" t="s">
+        <v>99</v>
+      </c>
+      <c r="K773">
+        <v>47</v>
+      </c>
+      <c r="L773" t="s">
+        <v>715</v>
+      </c>
+      <c r="M773" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="774" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A774">
+        <v>1762</v>
+      </c>
+      <c r="B774">
+        <v>34</v>
+      </c>
+      <c r="C774" t="s">
+        <v>774</v>
+      </c>
+      <c r="J774" t="s">
+        <v>99</v>
+      </c>
+      <c r="K774">
+        <v>47</v>
+      </c>
+      <c r="L774" t="s">
+        <v>715</v>
+      </c>
+      <c r="M774" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="775" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A775">
+        <v>1762</v>
+      </c>
+      <c r="B775">
+        <v>35</v>
+      </c>
+      <c r="C775" t="s">
+        <v>775</v>
+      </c>
+      <c r="J775" t="s">
+        <v>99</v>
+      </c>
+      <c r="K775">
+        <v>47</v>
+      </c>
+      <c r="L775" t="s">
+        <v>715</v>
+      </c>
+      <c r="M775" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="776" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A776">
+        <v>1762</v>
+      </c>
+      <c r="B776">
+        <v>35</v>
+      </c>
+      <c r="C776" t="s">
+        <v>776</v>
+      </c>
+      <c r="J776" t="s">
+        <v>99</v>
+      </c>
+      <c r="K776">
+        <v>47</v>
+      </c>
+      <c r="L776" t="s">
+        <v>715</v>
+      </c>
+      <c r="M776" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="777" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A777">
+        <v>1762</v>
+      </c>
+      <c r="B777">
+        <v>35</v>
+      </c>
+      <c r="C777" t="s">
+        <v>777</v>
+      </c>
+      <c r="J777" t="s">
+        <v>99</v>
+      </c>
+      <c r="K777">
+        <v>47</v>
+      </c>
+      <c r="L777" t="s">
+        <v>715</v>
+      </c>
+      <c r="M777" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="778" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A778">
+        <v>1763</v>
+      </c>
+      <c r="B778">
+        <v>36</v>
+      </c>
+      <c r="C778" t="s">
+        <v>778</v>
+      </c>
+      <c r="J778" t="s">
+        <v>99</v>
+      </c>
+      <c r="K778">
+        <v>47</v>
+      </c>
+      <c r="L778" t="s">
+        <v>715</v>
+      </c>
+      <c r="M778" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="779" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A779">
+        <v>1763</v>
+      </c>
+      <c r="B779">
+        <v>36</v>
+      </c>
+      <c r="C779" t="s">
+        <v>779</v>
+      </c>
+      <c r="J779" t="s">
+        <v>99</v>
+      </c>
+      <c r="K779">
+        <v>47</v>
+      </c>
+      <c r="L779" t="s">
+        <v>715</v>
+      </c>
+      <c r="M779" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="780" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A780">
+        <v>1763</v>
+      </c>
+      <c r="B780">
+        <v>37</v>
+      </c>
+      <c r="C780" t="s">
+        <v>780</v>
+      </c>
+      <c r="J780" t="s">
+        <v>99</v>
+      </c>
+      <c r="K780">
+        <v>47</v>
+      </c>
+      <c r="L780" t="s">
+        <v>715</v>
+      </c>
+      <c r="M780" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="781" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A781">
+        <v>1763</v>
+      </c>
+      <c r="B781">
+        <v>37</v>
+      </c>
+      <c r="C781" t="s">
+        <v>781</v>
+      </c>
+      <c r="J781" t="s">
+        <v>99</v>
+      </c>
+      <c r="K781">
+        <v>47</v>
+      </c>
+      <c r="L781" t="s">
+        <v>715</v>
+      </c>
+      <c r="M781" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="782" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A782">
+        <v>1763</v>
+      </c>
+      <c r="B782">
+        <v>38</v>
+      </c>
+      <c r="C782" t="s">
+        <v>782</v>
+      </c>
+      <c r="J782" t="s">
+        <v>99</v>
+      </c>
+      <c r="K782">
+        <v>47</v>
+      </c>
+      <c r="L782" t="s">
+        <v>715</v>
+      </c>
+      <c r="M782" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="783" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A783">
+        <v>1763</v>
+      </c>
+      <c r="B783">
+        <v>38</v>
+      </c>
+      <c r="C783" t="s">
+        <v>783</v>
+      </c>
+      <c r="J783" t="s">
+        <v>99</v>
+      </c>
+      <c r="K783">
+        <v>47</v>
+      </c>
+      <c r="L783" t="s">
+        <v>715</v>
+      </c>
+      <c r="M783" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="784" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A784">
+        <v>1763</v>
+      </c>
+      <c r="B784">
+        <v>39</v>
+      </c>
+      <c r="C784" t="s">
+        <v>784</v>
+      </c>
+      <c r="J784" t="s">
+        <v>99</v>
+      </c>
+      <c r="K784">
+        <v>47</v>
+      </c>
+      <c r="L784" t="s">
+        <v>715</v>
+      </c>
+      <c r="M784" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="785" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A785">
+        <v>1763</v>
+      </c>
+      <c r="B785">
+        <v>39</v>
+      </c>
+      <c r="C785" t="s">
+        <v>783</v>
+      </c>
+      <c r="J785" t="s">
+        <v>99</v>
+      </c>
+      <c r="K785">
+        <v>47</v>
+      </c>
+      <c r="L785" t="s">
+        <v>715</v>
+      </c>
+      <c r="M785" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="786" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A786">
+        <v>1764</v>
+      </c>
+      <c r="B786">
+        <v>40</v>
+      </c>
+      <c r="C786" t="s">
+        <v>785</v>
+      </c>
+      <c r="J786" t="s">
+        <v>99</v>
+      </c>
+      <c r="K786">
+        <v>47</v>
+      </c>
+      <c r="L786" t="s">
+        <v>715</v>
+      </c>
+      <c r="M786" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="787" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A787">
+        <v>1764</v>
+      </c>
+      <c r="B787">
+        <v>40</v>
+      </c>
+      <c r="C787" t="s">
+        <v>725</v>
+      </c>
+      <c r="J787" t="s">
+        <v>99</v>
+      </c>
+      <c r="K787">
+        <v>47</v>
+      </c>
+      <c r="L787" t="s">
+        <v>715</v>
+      </c>
+      <c r="M787" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="788" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A788">
+        <v>1764</v>
+      </c>
+      <c r="B788">
+        <v>40</v>
+      </c>
+      <c r="C788" t="s">
+        <v>786</v>
+      </c>
+      <c r="J788" t="s">
+        <v>99</v>
+      </c>
+      <c r="K788">
+        <v>47</v>
+      </c>
+      <c r="L788" t="s">
+        <v>715</v>
+      </c>
+      <c r="M788" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="789" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A789">
+        <v>1764</v>
+      </c>
+      <c r="B789">
+        <v>41</v>
+      </c>
+      <c r="C789" t="s">
+        <v>787</v>
+      </c>
+      <c r="J789" t="s">
+        <v>99</v>
+      </c>
+      <c r="K789">
+        <v>47</v>
+      </c>
+      <c r="L789" t="s">
+        <v>715</v>
+      </c>
+      <c r="M789" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="790" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A790">
+        <v>1764</v>
+      </c>
+      <c r="B790">
+        <v>41</v>
+      </c>
+      <c r="C790" t="s">
+        <v>788</v>
+      </c>
+      <c r="J790" t="s">
+        <v>99</v>
+      </c>
+      <c r="K790">
+        <v>47</v>
+      </c>
+      <c r="L790" t="s">
+        <v>715</v>
+      </c>
+      <c r="M790" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="791" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A791">
+        <v>1764</v>
+      </c>
+      <c r="B791">
+        <v>42</v>
+      </c>
+      <c r="C791" t="s">
+        <v>789</v>
+      </c>
+      <c r="J791" t="s">
+        <v>99</v>
+      </c>
+      <c r="K791">
+        <v>47</v>
+      </c>
+      <c r="L791" t="s">
+        <v>715</v>
+      </c>
+      <c r="M791" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="792" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A792">
+        <v>1764</v>
+      </c>
+      <c r="B792">
+        <v>42</v>
+      </c>
+      <c r="C792" t="s">
+        <v>327</v>
+      </c>
+      <c r="J792" t="s">
+        <v>99</v>
+      </c>
+      <c r="K792">
+        <v>47</v>
+      </c>
+      <c r="L792" t="s">
+        <v>715</v>
+      </c>
+      <c r="M792" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="793" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A793">
+        <v>1764</v>
+      </c>
+      <c r="B793">
+        <v>43</v>
+      </c>
+      <c r="C793" t="s">
+        <v>790</v>
+      </c>
+      <c r="J793" t="s">
+        <v>99</v>
+      </c>
+      <c r="K793">
+        <v>47</v>
+      </c>
+      <c r="L793" t="s">
+        <v>715</v>
+      </c>
+      <c r="M793" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="794" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A794">
+        <v>1764</v>
+      </c>
+      <c r="B794">
+        <v>43</v>
+      </c>
+      <c r="C794" t="s">
+        <v>791</v>
+      </c>
+      <c r="J794" t="s">
+        <v>99</v>
+      </c>
+      <c r="K794">
+        <v>47</v>
+      </c>
+      <c r="L794" t="s">
+        <v>715</v>
+      </c>
+      <c r="M794" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="795" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A795">
+        <v>1764</v>
+      </c>
+      <c r="B795">
+        <v>44</v>
+      </c>
+      <c r="C795" t="s">
+        <v>76</v>
+      </c>
+      <c r="J795" t="s">
+        <v>99</v>
+      </c>
+      <c r="K795">
+        <v>47</v>
+      </c>
+      <c r="L795" t="s">
+        <v>715</v>
+      </c>
+      <c r="M795" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="796" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A796">
+        <v>1765</v>
+      </c>
+      <c r="B796">
+        <v>44</v>
+      </c>
+      <c r="C796" t="s">
+        <v>792</v>
+      </c>
+      <c r="J796" t="s">
+        <v>99</v>
+      </c>
+      <c r="K796">
+        <v>47</v>
+      </c>
+      <c r="L796" t="s">
+        <v>715</v>
+      </c>
+      <c r="M796" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="797" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A797">
+        <v>1765</v>
+      </c>
+      <c r="B797">
+        <v>44</v>
+      </c>
+      <c r="C797" t="s">
+        <v>793</v>
+      </c>
+      <c r="J797" t="s">
+        <v>99</v>
+      </c>
+      <c r="K797">
+        <v>47</v>
+      </c>
+      <c r="L797" t="s">
+        <v>715</v>
+      </c>
+      <c r="M797" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="798" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A798">
+        <v>1765</v>
+      </c>
+      <c r="B798">
+        <v>45</v>
+      </c>
+      <c r="C798" t="s">
+        <v>794</v>
+      </c>
+      <c r="J798" t="s">
+        <v>99</v>
+      </c>
+      <c r="K798">
+        <v>47</v>
+      </c>
+      <c r="L798" t="s">
+        <v>715</v>
+      </c>
+      <c r="M798" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="799" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A799">
+        <v>1765</v>
+      </c>
+      <c r="B799">
+        <v>45</v>
+      </c>
+      <c r="C799" t="s">
+        <v>795</v>
+      </c>
+      <c r="J799" t="s">
+        <v>99</v>
+      </c>
+      <c r="K799">
+        <v>47</v>
+      </c>
+      <c r="L799" t="s">
+        <v>715</v>
+      </c>
+      <c r="M799" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="800" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A800">
+        <v>1765</v>
+      </c>
+      <c r="B800">
+        <v>46</v>
+      </c>
+      <c r="C800" t="s">
+        <v>796</v>
+      </c>
+      <c r="J800" t="s">
+        <v>99</v>
+      </c>
+      <c r="K800">
+        <v>47</v>
+      </c>
+      <c r="L800" t="s">
+        <v>715</v>
+      </c>
+      <c r="M800" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="801" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A801">
+        <v>1765</v>
+      </c>
+      <c r="B801">
+        <v>46</v>
+      </c>
+      <c r="C801" t="s">
+        <v>797</v>
+      </c>
+      <c r="J801" t="s">
+        <v>99</v>
+      </c>
+      <c r="K801">
+        <v>47</v>
+      </c>
+      <c r="L801" t="s">
+        <v>715</v>
+      </c>
+      <c r="M801" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="802" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A802">
+        <v>1765</v>
+      </c>
+      <c r="B802">
+        <v>46</v>
+      </c>
+      <c r="C802" t="s">
+        <v>798</v>
+      </c>
+      <c r="J802" t="s">
+        <v>99</v>
+      </c>
+      <c r="K802">
+        <v>47</v>
+      </c>
+      <c r="L802" t="s">
+        <v>715</v>
+      </c>
+      <c r="M802" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="803" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A803">
+        <v>1765</v>
+      </c>
+      <c r="B803">
+        <v>47</v>
+      </c>
+      <c r="C803" t="s">
+        <v>799</v>
+      </c>
+      <c r="J803" t="s">
+        <v>99</v>
+      </c>
+      <c r="K803">
+        <v>47</v>
+      </c>
+      <c r="L803" t="s">
+        <v>715</v>
+      </c>
+      <c r="M803" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="804" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A804">
+        <v>1765</v>
+      </c>
+      <c r="B804">
+        <v>47</v>
+      </c>
+      <c r="C804" t="s">
+        <v>800</v>
+      </c>
+      <c r="J804" t="s">
+        <v>99</v>
+      </c>
+      <c r="K804">
+        <v>47</v>
+      </c>
+      <c r="L804" t="s">
+        <v>715</v>
+      </c>
+      <c r="M804" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="805" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A805">
+        <v>1765</v>
+      </c>
+      <c r="B805">
+        <v>48</v>
+      </c>
+      <c r="C805" t="s">
+        <v>801</v>
+      </c>
+      <c r="J805" t="s">
+        <v>99</v>
+      </c>
+      <c r="K805">
+        <v>47</v>
+      </c>
+      <c r="L805" t="s">
+        <v>715</v>
+      </c>
+      <c r="M805" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="806" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A806">
+        <v>1761</v>
+      </c>
+      <c r="B806">
+        <v>48</v>
+      </c>
+      <c r="C806" t="s">
+        <v>802</v>
+      </c>
+      <c r="J806" t="s">
+        <v>99</v>
+      </c>
+      <c r="K806">
+        <v>47</v>
+      </c>
+      <c r="L806" t="s">
+        <v>715</v>
+      </c>
+      <c r="M806" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="807" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A807">
+        <v>1761</v>
+      </c>
+      <c r="B807">
+        <v>48</v>
+      </c>
+      <c r="C807" t="s">
+        <v>803</v>
+      </c>
+      <c r="J807" t="s">
+        <v>99</v>
+      </c>
+      <c r="K807">
+        <v>47</v>
+      </c>
+      <c r="L807" t="s">
+        <v>715</v>
+      </c>
+      <c r="M807" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="808" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A808">
+        <v>1761</v>
+      </c>
+      <c r="B808">
+        <v>49</v>
+      </c>
+      <c r="C808" t="s">
+        <v>804</v>
+      </c>
+      <c r="J808" t="s">
+        <v>99</v>
+      </c>
+      <c r="K808">
+        <v>47</v>
+      </c>
+      <c r="L808" t="s">
+        <v>715</v>
+      </c>
+      <c r="M808" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="809" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A809">
+        <v>1761</v>
+      </c>
+      <c r="B809">
+        <v>49</v>
+      </c>
+      <c r="C809" t="s">
+        <v>805</v>
+      </c>
+      <c r="J809" t="s">
+        <v>99</v>
+      </c>
+      <c r="K809">
+        <v>47</v>
+      </c>
+      <c r="L809" t="s">
+        <v>715</v>
+      </c>
+      <c r="M809" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="810" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A810">
+        <v>1761</v>
+      </c>
+      <c r="B810">
+        <v>49</v>
+      </c>
+      <c r="C810" t="s">
+        <v>806</v>
+      </c>
+      <c r="J810" t="s">
+        <v>99</v>
+      </c>
+      <c r="K810">
+        <v>47</v>
+      </c>
+      <c r="L810" t="s">
+        <v>715</v>
+      </c>
+      <c r="M810" t="s">
+        <v>714</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M715" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
afegint dades matrimonis 1693-1749 fins pàg 14
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Matrimonis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C876939-D1A2-46E3-B291-769FF02088BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5004A1-8031-4D3D-AF1D-F057D16B394E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C34A0C26-324D-4E17-B7B1-6D7DB0FCFBF8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3280" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3616" uniqueCount="890">
   <si>
     <t>Cognoms Familia</t>
   </si>
@@ -2459,7 +2459,256 @@
     <t>Pujades Porta</t>
   </si>
   <si>
-    <t>Codol ?</t>
+    <t>Codol Esquius</t>
+  </si>
+  <si>
+    <t>Margall Mas</t>
+  </si>
+  <si>
+    <t>Batlle Sunyé</t>
+  </si>
+  <si>
+    <t>Cadena Agulló</t>
+  </si>
+  <si>
+    <t>Civit Boladeres</t>
+  </si>
+  <si>
+    <t>Gine Cascallo</t>
+  </si>
+  <si>
+    <t>Fabregat Roige</t>
+  </si>
+  <si>
+    <t>Torra Duch</t>
+  </si>
+  <si>
+    <t>Falcó Sunyé</t>
+  </si>
+  <si>
+    <t>Roige Massana</t>
+  </si>
+  <si>
+    <t>Gassó Torrent</t>
+  </si>
+  <si>
+    <t>Duart Bosch</t>
+  </si>
+  <si>
+    <t>Pedrós Carles</t>
+  </si>
+  <si>
+    <t>Boldú Badia</t>
+  </si>
+  <si>
+    <t>Serra Tarragó</t>
+  </si>
+  <si>
+    <t>1693-1749</t>
+  </si>
+  <si>
+    <t>A, 1</t>
+  </si>
+  <si>
+    <t>Ortiz Muntaner</t>
+  </si>
+  <si>
+    <t>Castelló Roma</t>
+  </si>
+  <si>
+    <t>Aldabo Borràs</t>
+  </si>
+  <si>
+    <t>Barrill Boria</t>
+  </si>
+  <si>
+    <t>Mirassó Balaguer</t>
+  </si>
+  <si>
+    <t>Cuberes Mirassó</t>
+  </si>
+  <si>
+    <t>Amargall Codina</t>
+  </si>
+  <si>
+    <t>Fabrigues Fontanals</t>
+  </si>
+  <si>
+    <t>Mas Mata</t>
+  </si>
+  <si>
+    <t>Roiger Capdevila</t>
+  </si>
+  <si>
+    <t>Castellà Bosch</t>
+  </si>
+  <si>
+    <t>Figat Monserrat</t>
+  </si>
+  <si>
+    <t>Martí Agulló</t>
+  </si>
+  <si>
+    <t>Lamarca Montaner</t>
+  </si>
+  <si>
+    <t>Batlle Paris</t>
+  </si>
+  <si>
+    <t>Corbi Claret</t>
+  </si>
+  <si>
+    <t>Niubó Gine</t>
+  </si>
+  <si>
+    <t>Casadella Berga</t>
+  </si>
+  <si>
+    <t>Torres Cases</t>
+  </si>
+  <si>
+    <t>Capdevila Agulló</t>
+  </si>
+  <si>
+    <t>Pinies Bosch</t>
+  </si>
+  <si>
+    <t>Farrerich Giné</t>
+  </si>
+  <si>
+    <t>Torruella Alies</t>
+  </si>
+  <si>
+    <t>Fa Amargall</t>
+  </si>
+  <si>
+    <t>Serra Garcia</t>
+  </si>
+  <si>
+    <t>Galitó Cuberes</t>
+  </si>
+  <si>
+    <t>Pallàs Giné</t>
+  </si>
+  <si>
+    <t>Capdevila Borràs</t>
+  </si>
+  <si>
+    <t>Fontalans Farrerich</t>
+  </si>
+  <si>
+    <t>Balaguer Farrer</t>
+  </si>
+  <si>
+    <t>Cava Borràs</t>
+  </si>
+  <si>
+    <t>Verni Pollina</t>
+  </si>
+  <si>
+    <t>Colell Agulló</t>
+  </si>
+  <si>
+    <t>Botet Ganyet</t>
+  </si>
+  <si>
+    <t>Martí Pons</t>
+  </si>
+  <si>
+    <t>Carbonell Cava</t>
+  </si>
+  <si>
+    <t>Serra Casals</t>
+  </si>
+  <si>
+    <t>Ricart Calbis</t>
+  </si>
+  <si>
+    <t>Mora Agulló</t>
+  </si>
+  <si>
+    <t>Martí Soler</t>
+  </si>
+  <si>
+    <t>Agulló Pedrós</t>
+  </si>
+  <si>
+    <t>Giné Moset</t>
+  </si>
+  <si>
+    <t>Mor Marti</t>
+  </si>
+  <si>
+    <t>Oriola Fenoll</t>
+  </si>
+  <si>
+    <t>Curcó Gasol</t>
+  </si>
+  <si>
+    <t>Torres Capdevila</t>
+  </si>
+  <si>
+    <t>Corberó Torrent</t>
+  </si>
+  <si>
+    <t>Folguera Mirassó</t>
+  </si>
+  <si>
+    <t>Balaguer Mas</t>
+  </si>
+  <si>
+    <t>Amargall Formiguera</t>
+  </si>
+  <si>
+    <t>Cluet Mata</t>
+  </si>
+  <si>
+    <t>Capdevila Vilagines</t>
+  </si>
+  <si>
+    <t>Civit Ballverdú</t>
+  </si>
+  <si>
+    <t>Tarabes Cases</t>
+  </si>
+  <si>
+    <t>Bonjorn Rodon</t>
+  </si>
+  <si>
+    <t>Lapera Farrer</t>
+  </si>
+  <si>
+    <t>Roma Gila</t>
+  </si>
+  <si>
+    <t>Novell Galceran</t>
+  </si>
+  <si>
+    <t>Larroja Huguet</t>
+  </si>
+  <si>
+    <t>Torrent Forés</t>
+  </si>
+  <si>
+    <t>Fontanals Palou</t>
+  </si>
+  <si>
+    <t>Serra Cahueres</t>
+  </si>
+  <si>
+    <t>Roiger Fenoll</t>
+  </si>
+  <si>
+    <t>Riuvert Ortiz</t>
+  </si>
+  <si>
+    <t>Morell Fleis</t>
+  </si>
+  <si>
+    <t>Mosset Vergé</t>
+  </si>
+  <si>
+    <t>Capdevila Bondal</t>
   </si>
 </sst>
 </file>
@@ -2814,11 +3063,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}">
-  <dimension ref="A1:N810"/>
+  <dimension ref="A1:N894"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A794" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A811" sqref="A811"/>
+      <pane ySplit="1" topLeftCell="A861" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A895" sqref="A895"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21429,7 +21678,7 @@
     </row>
     <row r="805" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A805">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="B805">
         <v>48</v>
@@ -21452,7 +21701,7 @@
     </row>
     <row r="806" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A806">
-        <v>1761</v>
+        <v>1767</v>
       </c>
       <c r="B806">
         <v>48</v>
@@ -21475,7 +21724,7 @@
     </row>
     <row r="807" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A807">
-        <v>1761</v>
+        <v>1767</v>
       </c>
       <c r="B807">
         <v>48</v>
@@ -21498,7 +21747,7 @@
     </row>
     <row r="808" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A808">
-        <v>1761</v>
+        <v>1767</v>
       </c>
       <c r="B808">
         <v>49</v>
@@ -21521,7 +21770,7 @@
     </row>
     <row r="809" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A809">
-        <v>1761</v>
+        <v>1767</v>
       </c>
       <c r="B809">
         <v>49</v>
@@ -21544,7 +21793,7 @@
     </row>
     <row r="810" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A810">
-        <v>1761</v>
+        <v>1767</v>
       </c>
       <c r="B810">
         <v>49</v>
@@ -21563,6 +21812,1938 @@
       </c>
       <c r="M810" t="s">
         <v>714</v>
+      </c>
+    </row>
+    <row r="811" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A811">
+        <v>1767</v>
+      </c>
+      <c r="B811">
+        <v>50</v>
+      </c>
+      <c r="C811" t="s">
+        <v>807</v>
+      </c>
+      <c r="J811" t="s">
+        <v>99</v>
+      </c>
+      <c r="K811">
+        <v>47</v>
+      </c>
+      <c r="L811" t="s">
+        <v>715</v>
+      </c>
+      <c r="M811" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="812" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A812">
+        <v>1767</v>
+      </c>
+      <c r="B812">
+        <v>50</v>
+      </c>
+      <c r="C812" t="s">
+        <v>808</v>
+      </c>
+      <c r="J812" t="s">
+        <v>99</v>
+      </c>
+      <c r="K812">
+        <v>47</v>
+      </c>
+      <c r="L812" t="s">
+        <v>715</v>
+      </c>
+      <c r="M812" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="813" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A813">
+        <v>1767</v>
+      </c>
+      <c r="B813">
+        <v>50</v>
+      </c>
+      <c r="C813" t="s">
+        <v>809</v>
+      </c>
+      <c r="J813" t="s">
+        <v>99</v>
+      </c>
+      <c r="K813">
+        <v>47</v>
+      </c>
+      <c r="L813" t="s">
+        <v>715</v>
+      </c>
+      <c r="M813" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="814" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A814">
+        <v>1767</v>
+      </c>
+      <c r="B814">
+        <v>51</v>
+      </c>
+      <c r="C814" t="s">
+        <v>810</v>
+      </c>
+      <c r="J814" t="s">
+        <v>99</v>
+      </c>
+      <c r="K814">
+        <v>47</v>
+      </c>
+      <c r="L814" t="s">
+        <v>715</v>
+      </c>
+      <c r="M814" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="815" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A815">
+        <v>1768</v>
+      </c>
+      <c r="B815">
+        <v>51</v>
+      </c>
+      <c r="C815" t="s">
+        <v>525</v>
+      </c>
+      <c r="J815" t="s">
+        <v>99</v>
+      </c>
+      <c r="K815">
+        <v>47</v>
+      </c>
+      <c r="L815" t="s">
+        <v>715</v>
+      </c>
+      <c r="M815" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="816" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A816">
+        <v>1768</v>
+      </c>
+      <c r="B816">
+        <v>51</v>
+      </c>
+      <c r="C816" t="s">
+        <v>811</v>
+      </c>
+      <c r="J816" t="s">
+        <v>99</v>
+      </c>
+      <c r="K816">
+        <v>47</v>
+      </c>
+      <c r="L816" t="s">
+        <v>715</v>
+      </c>
+      <c r="M816" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="817" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A817">
+        <v>1768</v>
+      </c>
+      <c r="B817">
+        <v>52</v>
+      </c>
+      <c r="C817" t="s">
+        <v>812</v>
+      </c>
+      <c r="J817" t="s">
+        <v>99</v>
+      </c>
+      <c r="K817">
+        <v>47</v>
+      </c>
+      <c r="L817" t="s">
+        <v>715</v>
+      </c>
+      <c r="M817" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="818" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A818">
+        <v>1768</v>
+      </c>
+      <c r="B818">
+        <v>52</v>
+      </c>
+      <c r="C818" t="s">
+        <v>813</v>
+      </c>
+      <c r="J818" t="s">
+        <v>99</v>
+      </c>
+      <c r="K818">
+        <v>47</v>
+      </c>
+      <c r="L818" t="s">
+        <v>715</v>
+      </c>
+      <c r="M818" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="819" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A819">
+        <v>1768</v>
+      </c>
+      <c r="B819">
+        <v>53</v>
+      </c>
+      <c r="C819" t="s">
+        <v>814</v>
+      </c>
+      <c r="J819" t="s">
+        <v>99</v>
+      </c>
+      <c r="K819">
+        <v>47</v>
+      </c>
+      <c r="L819" t="s">
+        <v>715</v>
+      </c>
+      <c r="M819" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="820" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A820">
+        <v>1768</v>
+      </c>
+      <c r="B820">
+        <v>53</v>
+      </c>
+      <c r="C820" t="s">
+        <v>815</v>
+      </c>
+      <c r="J820" t="s">
+        <v>99</v>
+      </c>
+      <c r="K820">
+        <v>47</v>
+      </c>
+      <c r="L820" t="s">
+        <v>715</v>
+      </c>
+      <c r="M820" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="821" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A821">
+        <v>1768</v>
+      </c>
+      <c r="B821">
+        <v>54</v>
+      </c>
+      <c r="C821" t="s">
+        <v>816</v>
+      </c>
+      <c r="J821" t="s">
+        <v>99</v>
+      </c>
+      <c r="K821">
+        <v>47</v>
+      </c>
+      <c r="L821" t="s">
+        <v>715</v>
+      </c>
+      <c r="M821" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="822" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A822">
+        <v>1768</v>
+      </c>
+      <c r="B822">
+        <v>54</v>
+      </c>
+      <c r="C822" t="s">
+        <v>817</v>
+      </c>
+      <c r="J822" t="s">
+        <v>99</v>
+      </c>
+      <c r="K822">
+        <v>47</v>
+      </c>
+      <c r="L822" t="s">
+        <v>715</v>
+      </c>
+      <c r="M822" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="823" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A823">
+        <v>1769</v>
+      </c>
+      <c r="B823">
+        <v>55</v>
+      </c>
+      <c r="C823" t="s">
+        <v>818</v>
+      </c>
+      <c r="J823" t="s">
+        <v>99</v>
+      </c>
+      <c r="K823">
+        <v>47</v>
+      </c>
+      <c r="L823" t="s">
+        <v>715</v>
+      </c>
+      <c r="M823" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="824" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A824">
+        <v>1769</v>
+      </c>
+      <c r="B824">
+        <v>55</v>
+      </c>
+      <c r="C824" t="s">
+        <v>819</v>
+      </c>
+      <c r="J824" t="s">
+        <v>99</v>
+      </c>
+      <c r="K824">
+        <v>47</v>
+      </c>
+      <c r="L824" t="s">
+        <v>715</v>
+      </c>
+      <c r="M824" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="825" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A825">
+        <v>1769</v>
+      </c>
+      <c r="B825">
+        <v>56</v>
+      </c>
+      <c r="C825" t="s">
+        <v>820</v>
+      </c>
+      <c r="J825" t="s">
+        <v>99</v>
+      </c>
+      <c r="K825">
+        <v>47</v>
+      </c>
+      <c r="L825" t="s">
+        <v>715</v>
+      </c>
+      <c r="M825" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="826" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A826">
+        <v>1693</v>
+      </c>
+      <c r="B826">
+        <v>3</v>
+      </c>
+      <c r="C826" t="s">
+        <v>823</v>
+      </c>
+      <c r="J826" t="s">
+        <v>99</v>
+      </c>
+      <c r="K826">
+        <v>47</v>
+      </c>
+      <c r="L826" t="s">
+        <v>822</v>
+      </c>
+      <c r="M826" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="827" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A827">
+        <v>1693</v>
+      </c>
+      <c r="B827">
+        <v>3</v>
+      </c>
+      <c r="C827" t="s">
+        <v>824</v>
+      </c>
+      <c r="J827" t="s">
+        <v>99</v>
+      </c>
+      <c r="K827">
+        <v>47</v>
+      </c>
+      <c r="L827" t="s">
+        <v>822</v>
+      </c>
+      <c r="M827" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="828" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A828">
+        <v>1693</v>
+      </c>
+      <c r="B828">
+        <v>3</v>
+      </c>
+      <c r="C828" t="s">
+        <v>825</v>
+      </c>
+      <c r="J828" t="s">
+        <v>99</v>
+      </c>
+      <c r="K828">
+        <v>47</v>
+      </c>
+      <c r="L828" t="s">
+        <v>822</v>
+      </c>
+      <c r="M828" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="829" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A829">
+        <v>1694</v>
+      </c>
+      <c r="B829">
+        <v>4</v>
+      </c>
+      <c r="C829" t="s">
+        <v>826</v>
+      </c>
+      <c r="J829" t="s">
+        <v>99</v>
+      </c>
+      <c r="K829">
+        <v>47</v>
+      </c>
+      <c r="L829" t="s">
+        <v>822</v>
+      </c>
+      <c r="M829" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="830" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A830">
+        <v>1694</v>
+      </c>
+      <c r="B830">
+        <v>4</v>
+      </c>
+      <c r="C830" t="s">
+        <v>827</v>
+      </c>
+      <c r="J830" t="s">
+        <v>99</v>
+      </c>
+      <c r="K830">
+        <v>47</v>
+      </c>
+      <c r="L830" t="s">
+        <v>822</v>
+      </c>
+      <c r="M830" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="831" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A831">
+        <v>1694</v>
+      </c>
+      <c r="B831">
+        <v>4</v>
+      </c>
+      <c r="C831" t="s">
+        <v>828</v>
+      </c>
+      <c r="J831" t="s">
+        <v>99</v>
+      </c>
+      <c r="K831">
+        <v>47</v>
+      </c>
+      <c r="L831" t="s">
+        <v>822</v>
+      </c>
+      <c r="M831" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="832" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A832">
+        <v>1694</v>
+      </c>
+      <c r="B832">
+        <v>4</v>
+      </c>
+      <c r="C832" t="s">
+        <v>829</v>
+      </c>
+      <c r="J832" t="s">
+        <v>99</v>
+      </c>
+      <c r="K832">
+        <v>47</v>
+      </c>
+      <c r="L832" t="s">
+        <v>822</v>
+      </c>
+      <c r="M832" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="833" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A833">
+        <v>1694</v>
+      </c>
+      <c r="B833">
+        <v>4</v>
+      </c>
+      <c r="C833" t="s">
+        <v>830</v>
+      </c>
+      <c r="J833" t="s">
+        <v>99</v>
+      </c>
+      <c r="K833">
+        <v>47</v>
+      </c>
+      <c r="L833" t="s">
+        <v>822</v>
+      </c>
+      <c r="M833" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="834" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A834">
+        <v>1694</v>
+      </c>
+      <c r="B834">
+        <v>4</v>
+      </c>
+      <c r="C834" t="s">
+        <v>831</v>
+      </c>
+      <c r="J834" t="s">
+        <v>99</v>
+      </c>
+      <c r="K834">
+        <v>47</v>
+      </c>
+      <c r="L834" t="s">
+        <v>822</v>
+      </c>
+      <c r="M834" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="835" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A835">
+        <v>1694</v>
+      </c>
+      <c r="B835">
+        <v>5</v>
+      </c>
+      <c r="C835" t="s">
+        <v>832</v>
+      </c>
+      <c r="J835" t="s">
+        <v>99</v>
+      </c>
+      <c r="K835">
+        <v>47</v>
+      </c>
+      <c r="L835" t="s">
+        <v>822</v>
+      </c>
+      <c r="M835" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="836" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A836">
+        <v>1694</v>
+      </c>
+      <c r="B836">
+        <v>5</v>
+      </c>
+      <c r="C836" t="s">
+        <v>833</v>
+      </c>
+      <c r="J836" t="s">
+        <v>99</v>
+      </c>
+      <c r="K836">
+        <v>47</v>
+      </c>
+      <c r="L836" t="s">
+        <v>822</v>
+      </c>
+      <c r="M836" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="837" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A837">
+        <v>1694</v>
+      </c>
+      <c r="B837">
+        <v>5</v>
+      </c>
+      <c r="C837" t="s">
+        <v>834</v>
+      </c>
+      <c r="J837" t="s">
+        <v>99</v>
+      </c>
+      <c r="K837">
+        <v>47</v>
+      </c>
+      <c r="L837" t="s">
+        <v>822</v>
+      </c>
+      <c r="M837" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="838" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A838">
+        <v>1694</v>
+      </c>
+      <c r="B838">
+        <v>5</v>
+      </c>
+      <c r="C838" t="s">
+        <v>835</v>
+      </c>
+      <c r="J838" t="s">
+        <v>99</v>
+      </c>
+      <c r="K838">
+        <v>47</v>
+      </c>
+      <c r="L838" t="s">
+        <v>822</v>
+      </c>
+      <c r="M838" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="839" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A839">
+        <v>1694</v>
+      </c>
+      <c r="B839">
+        <v>5</v>
+      </c>
+      <c r="C839" t="s">
+        <v>836</v>
+      </c>
+      <c r="J839" t="s">
+        <v>99</v>
+      </c>
+      <c r="K839">
+        <v>47</v>
+      </c>
+      <c r="L839" t="s">
+        <v>822</v>
+      </c>
+      <c r="M839" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="840" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A840">
+        <v>1694</v>
+      </c>
+      <c r="B840">
+        <v>5</v>
+      </c>
+      <c r="C840" t="s">
+        <v>837</v>
+      </c>
+      <c r="J840" t="s">
+        <v>99</v>
+      </c>
+      <c r="K840">
+        <v>47</v>
+      </c>
+      <c r="L840" t="s">
+        <v>822</v>
+      </c>
+      <c r="M840" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="841" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A841">
+        <v>1695</v>
+      </c>
+      <c r="B841">
+        <v>6</v>
+      </c>
+      <c r="C841" t="s">
+        <v>838</v>
+      </c>
+      <c r="J841" t="s">
+        <v>99</v>
+      </c>
+      <c r="K841">
+        <v>47</v>
+      </c>
+      <c r="L841" t="s">
+        <v>822</v>
+      </c>
+      <c r="M841" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="842" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A842">
+        <v>1695</v>
+      </c>
+      <c r="B842">
+        <v>6</v>
+      </c>
+      <c r="C842" t="s">
+        <v>839</v>
+      </c>
+      <c r="J842" t="s">
+        <v>99</v>
+      </c>
+      <c r="K842">
+        <v>47</v>
+      </c>
+      <c r="L842" t="s">
+        <v>822</v>
+      </c>
+      <c r="M842" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="843" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A843">
+        <v>1696</v>
+      </c>
+      <c r="B843">
+        <v>6</v>
+      </c>
+      <c r="C843" t="s">
+        <v>840</v>
+      </c>
+      <c r="J843" t="s">
+        <v>99</v>
+      </c>
+      <c r="K843">
+        <v>47</v>
+      </c>
+      <c r="L843" t="s">
+        <v>822</v>
+      </c>
+      <c r="M843" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="844" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A844">
+        <v>1696</v>
+      </c>
+      <c r="B844">
+        <v>6</v>
+      </c>
+      <c r="C844" t="s">
+        <v>841</v>
+      </c>
+      <c r="J844" t="s">
+        <v>99</v>
+      </c>
+      <c r="K844">
+        <v>47</v>
+      </c>
+      <c r="L844" t="s">
+        <v>822</v>
+      </c>
+      <c r="M844" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="845" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A845">
+        <v>1696</v>
+      </c>
+      <c r="B845">
+        <v>6</v>
+      </c>
+      <c r="C845" t="s">
+        <v>842</v>
+      </c>
+      <c r="J845" t="s">
+        <v>99</v>
+      </c>
+      <c r="K845">
+        <v>47</v>
+      </c>
+      <c r="L845" t="s">
+        <v>822</v>
+      </c>
+      <c r="M845" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="846" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A846">
+        <v>1696</v>
+      </c>
+      <c r="B846">
+        <v>6</v>
+      </c>
+      <c r="C846" t="s">
+        <v>843</v>
+      </c>
+      <c r="J846" t="s">
+        <v>99</v>
+      </c>
+      <c r="K846">
+        <v>47</v>
+      </c>
+      <c r="L846" t="s">
+        <v>822</v>
+      </c>
+      <c r="M846" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="847" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A847">
+        <v>1697</v>
+      </c>
+      <c r="B847">
+        <v>7</v>
+      </c>
+      <c r="C847" t="s">
+        <v>844</v>
+      </c>
+      <c r="J847" t="s">
+        <v>99</v>
+      </c>
+      <c r="K847">
+        <v>47</v>
+      </c>
+      <c r="L847" t="s">
+        <v>822</v>
+      </c>
+      <c r="M847" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="848" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A848">
+        <v>1697</v>
+      </c>
+      <c r="B848">
+        <v>7</v>
+      </c>
+      <c r="C848" t="s">
+        <v>845</v>
+      </c>
+      <c r="J848" t="s">
+        <v>99</v>
+      </c>
+      <c r="K848">
+        <v>47</v>
+      </c>
+      <c r="L848" t="s">
+        <v>822</v>
+      </c>
+      <c r="M848" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="849" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A849">
+        <v>1697</v>
+      </c>
+      <c r="B849">
+        <v>7</v>
+      </c>
+      <c r="C849" t="s">
+        <v>846</v>
+      </c>
+      <c r="J849" t="s">
+        <v>99</v>
+      </c>
+      <c r="K849">
+        <v>47</v>
+      </c>
+      <c r="L849" t="s">
+        <v>822</v>
+      </c>
+      <c r="M849" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="850" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A850">
+        <v>1697</v>
+      </c>
+      <c r="B850">
+        <v>7</v>
+      </c>
+      <c r="C850" t="s">
+        <v>847</v>
+      </c>
+      <c r="J850" t="s">
+        <v>99</v>
+      </c>
+      <c r="K850">
+        <v>47</v>
+      </c>
+      <c r="L850" t="s">
+        <v>822</v>
+      </c>
+      <c r="M850" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="851" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A851">
+        <v>1697</v>
+      </c>
+      <c r="B851">
+        <v>7</v>
+      </c>
+      <c r="C851" t="s">
+        <v>848</v>
+      </c>
+      <c r="J851" t="s">
+        <v>99</v>
+      </c>
+      <c r="K851">
+        <v>47</v>
+      </c>
+      <c r="L851" t="s">
+        <v>822</v>
+      </c>
+      <c r="M851" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="852" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A852">
+        <v>1697</v>
+      </c>
+      <c r="B852">
+        <v>7</v>
+      </c>
+      <c r="C852" t="s">
+        <v>849</v>
+      </c>
+      <c r="J852" t="s">
+        <v>99</v>
+      </c>
+      <c r="K852">
+        <v>47</v>
+      </c>
+      <c r="L852" t="s">
+        <v>822</v>
+      </c>
+      <c r="M852" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="853" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A853">
+        <v>1697</v>
+      </c>
+      <c r="B853">
+        <v>8</v>
+      </c>
+      <c r="C853" t="s">
+        <v>850</v>
+      </c>
+      <c r="J853" t="s">
+        <v>99</v>
+      </c>
+      <c r="K853">
+        <v>47</v>
+      </c>
+      <c r="L853" t="s">
+        <v>822</v>
+      </c>
+      <c r="M853" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="854" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A854">
+        <v>1698</v>
+      </c>
+      <c r="B854">
+        <v>8</v>
+      </c>
+      <c r="C854" t="s">
+        <v>851</v>
+      </c>
+      <c r="J854" t="s">
+        <v>99</v>
+      </c>
+      <c r="K854">
+        <v>47</v>
+      </c>
+      <c r="L854" t="s">
+        <v>822</v>
+      </c>
+      <c r="M854" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="855" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A855">
+        <v>1698</v>
+      </c>
+      <c r="B855">
+        <v>8</v>
+      </c>
+      <c r="C855" t="s">
+        <v>852</v>
+      </c>
+      <c r="J855" t="s">
+        <v>99</v>
+      </c>
+      <c r="K855">
+        <v>47</v>
+      </c>
+      <c r="L855" t="s">
+        <v>822</v>
+      </c>
+      <c r="M855" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="856" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A856">
+        <v>1698</v>
+      </c>
+      <c r="B856">
+        <v>8</v>
+      </c>
+      <c r="C856" t="s">
+        <v>853</v>
+      </c>
+      <c r="J856" t="s">
+        <v>99</v>
+      </c>
+      <c r="K856">
+        <v>47</v>
+      </c>
+      <c r="L856" t="s">
+        <v>822</v>
+      </c>
+      <c r="M856" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="857" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A857">
+        <v>1699</v>
+      </c>
+      <c r="B857">
+        <v>8</v>
+      </c>
+      <c r="C857" t="s">
+        <v>854</v>
+      </c>
+      <c r="J857" t="s">
+        <v>99</v>
+      </c>
+      <c r="K857">
+        <v>47</v>
+      </c>
+      <c r="L857" t="s">
+        <v>822</v>
+      </c>
+      <c r="M857" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="858" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A858">
+        <v>1699</v>
+      </c>
+      <c r="B858">
+        <v>8</v>
+      </c>
+      <c r="C858" t="s">
+        <v>797</v>
+      </c>
+      <c r="J858" t="s">
+        <v>99</v>
+      </c>
+      <c r="K858">
+        <v>47</v>
+      </c>
+      <c r="L858" t="s">
+        <v>822</v>
+      </c>
+      <c r="M858" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="859" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A859">
+        <v>1699</v>
+      </c>
+      <c r="B859">
+        <v>9</v>
+      </c>
+      <c r="C859" t="s">
+        <v>855</v>
+      </c>
+      <c r="J859" t="s">
+        <v>99</v>
+      </c>
+      <c r="K859">
+        <v>47</v>
+      </c>
+      <c r="L859" t="s">
+        <v>822</v>
+      </c>
+      <c r="M859" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="860" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A860">
+        <v>1700</v>
+      </c>
+      <c r="B860">
+        <v>9</v>
+      </c>
+      <c r="C860" t="s">
+        <v>856</v>
+      </c>
+      <c r="J860" t="s">
+        <v>99</v>
+      </c>
+      <c r="K860">
+        <v>47</v>
+      </c>
+      <c r="L860" t="s">
+        <v>822</v>
+      </c>
+      <c r="M860" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="861" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A861">
+        <v>1700</v>
+      </c>
+      <c r="B861">
+        <v>9</v>
+      </c>
+      <c r="C861" t="s">
+        <v>857</v>
+      </c>
+      <c r="J861" t="s">
+        <v>99</v>
+      </c>
+      <c r="K861">
+        <v>47</v>
+      </c>
+      <c r="L861" t="s">
+        <v>822</v>
+      </c>
+      <c r="M861" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="862" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A862">
+        <v>1700</v>
+      </c>
+      <c r="B862">
+        <v>9</v>
+      </c>
+      <c r="C862" t="s">
+        <v>858</v>
+      </c>
+      <c r="J862" t="s">
+        <v>99</v>
+      </c>
+      <c r="K862">
+        <v>47</v>
+      </c>
+      <c r="L862" t="s">
+        <v>822</v>
+      </c>
+      <c r="M862" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="863" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A863">
+        <v>1702</v>
+      </c>
+      <c r="B863">
+        <v>9</v>
+      </c>
+      <c r="C863" t="s">
+        <v>859</v>
+      </c>
+      <c r="J863" t="s">
+        <v>99</v>
+      </c>
+      <c r="K863">
+        <v>47</v>
+      </c>
+      <c r="L863" t="s">
+        <v>822</v>
+      </c>
+      <c r="M863" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="864" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A864">
+        <v>1702</v>
+      </c>
+      <c r="B864">
+        <v>9</v>
+      </c>
+      <c r="C864" t="s">
+        <v>860</v>
+      </c>
+      <c r="J864" t="s">
+        <v>99</v>
+      </c>
+      <c r="K864">
+        <v>47</v>
+      </c>
+      <c r="L864" t="s">
+        <v>822</v>
+      </c>
+      <c r="M864" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="865" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A865">
+        <v>1703</v>
+      </c>
+      <c r="B865">
+        <v>10</v>
+      </c>
+      <c r="C865" t="s">
+        <v>861</v>
+      </c>
+      <c r="J865" t="s">
+        <v>99</v>
+      </c>
+      <c r="K865">
+        <v>47</v>
+      </c>
+      <c r="L865" t="s">
+        <v>822</v>
+      </c>
+      <c r="M865" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="866" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A866">
+        <v>1703</v>
+      </c>
+      <c r="B866">
+        <v>10</v>
+      </c>
+      <c r="C866" t="s">
+        <v>862</v>
+      </c>
+      <c r="J866" t="s">
+        <v>99</v>
+      </c>
+      <c r="K866">
+        <v>47</v>
+      </c>
+      <c r="L866" t="s">
+        <v>822</v>
+      </c>
+      <c r="M866" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="867" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A867">
+        <v>1704</v>
+      </c>
+      <c r="B867">
+        <v>10</v>
+      </c>
+      <c r="C867" t="s">
+        <v>664</v>
+      </c>
+      <c r="J867" t="s">
+        <v>99</v>
+      </c>
+      <c r="K867">
+        <v>47</v>
+      </c>
+      <c r="L867" t="s">
+        <v>822</v>
+      </c>
+      <c r="M867" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="868" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A868">
+        <v>1704</v>
+      </c>
+      <c r="B868">
+        <v>10</v>
+      </c>
+      <c r="C868" t="s">
+        <v>863</v>
+      </c>
+      <c r="J868" t="s">
+        <v>99</v>
+      </c>
+      <c r="K868">
+        <v>47</v>
+      </c>
+      <c r="L868" t="s">
+        <v>822</v>
+      </c>
+      <c r="M868" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="869" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A869">
+        <v>1704</v>
+      </c>
+      <c r="B869">
+        <v>10</v>
+      </c>
+      <c r="C869" t="s">
+        <v>864</v>
+      </c>
+      <c r="J869" t="s">
+        <v>99</v>
+      </c>
+      <c r="K869">
+        <v>47</v>
+      </c>
+      <c r="L869" t="s">
+        <v>822</v>
+      </c>
+      <c r="M869" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="870" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A870">
+        <v>1704</v>
+      </c>
+      <c r="B870">
+        <v>10</v>
+      </c>
+      <c r="C870" t="s">
+        <v>865</v>
+      </c>
+      <c r="J870" t="s">
+        <v>99</v>
+      </c>
+      <c r="K870">
+        <v>47</v>
+      </c>
+      <c r="L870" t="s">
+        <v>822</v>
+      </c>
+      <c r="M870" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="871" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A871">
+        <v>1704</v>
+      </c>
+      <c r="B871">
+        <v>11</v>
+      </c>
+      <c r="C871" t="s">
+        <v>866</v>
+      </c>
+      <c r="J871" t="s">
+        <v>99</v>
+      </c>
+      <c r="K871">
+        <v>47</v>
+      </c>
+      <c r="L871" t="s">
+        <v>822</v>
+      </c>
+      <c r="M871" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="872" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A872">
+        <v>1704</v>
+      </c>
+      <c r="B872">
+        <v>11</v>
+      </c>
+      <c r="C872" t="s">
+        <v>867</v>
+      </c>
+      <c r="J872" t="s">
+        <v>99</v>
+      </c>
+      <c r="K872">
+        <v>47</v>
+      </c>
+      <c r="L872" t="s">
+        <v>822</v>
+      </c>
+      <c r="M872" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="873" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A873">
+        <v>1704</v>
+      </c>
+      <c r="B873">
+        <v>11</v>
+      </c>
+      <c r="C873" t="s">
+        <v>868</v>
+      </c>
+      <c r="J873" t="s">
+        <v>99</v>
+      </c>
+      <c r="K873">
+        <v>47</v>
+      </c>
+      <c r="L873" t="s">
+        <v>822</v>
+      </c>
+      <c r="M873" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="874" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A874">
+        <v>1705</v>
+      </c>
+      <c r="B874">
+        <v>11</v>
+      </c>
+      <c r="C874" t="s">
+        <v>869</v>
+      </c>
+      <c r="J874" t="s">
+        <v>99</v>
+      </c>
+      <c r="K874">
+        <v>47</v>
+      </c>
+      <c r="L874" t="s">
+        <v>822</v>
+      </c>
+      <c r="M874" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="875" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A875">
+        <v>1705</v>
+      </c>
+      <c r="B875">
+        <v>11</v>
+      </c>
+      <c r="C875" t="s">
+        <v>870</v>
+      </c>
+      <c r="J875" t="s">
+        <v>99</v>
+      </c>
+      <c r="K875">
+        <v>47</v>
+      </c>
+      <c r="L875" t="s">
+        <v>822</v>
+      </c>
+      <c r="M875" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="876" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A876">
+        <v>1705</v>
+      </c>
+      <c r="B876">
+        <v>11</v>
+      </c>
+      <c r="C876" t="s">
+        <v>871</v>
+      </c>
+      <c r="J876" t="s">
+        <v>99</v>
+      </c>
+      <c r="K876">
+        <v>47</v>
+      </c>
+      <c r="L876" t="s">
+        <v>822</v>
+      </c>
+      <c r="M876" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="877" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A877">
+        <v>1705</v>
+      </c>
+      <c r="B877">
+        <v>12</v>
+      </c>
+      <c r="C877" t="s">
+        <v>872</v>
+      </c>
+      <c r="J877" t="s">
+        <v>99</v>
+      </c>
+      <c r="K877">
+        <v>47</v>
+      </c>
+      <c r="L877" t="s">
+        <v>822</v>
+      </c>
+      <c r="M877" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="878" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A878">
+        <v>1705</v>
+      </c>
+      <c r="B878">
+        <v>12</v>
+      </c>
+      <c r="C878" t="s">
+        <v>873</v>
+      </c>
+      <c r="J878" t="s">
+        <v>99</v>
+      </c>
+      <c r="K878">
+        <v>47</v>
+      </c>
+      <c r="L878" t="s">
+        <v>822</v>
+      </c>
+      <c r="M878" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="879" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A879">
+        <v>1706</v>
+      </c>
+      <c r="B879">
+        <v>12</v>
+      </c>
+      <c r="C879" t="s">
+        <v>874</v>
+      </c>
+      <c r="J879" t="s">
+        <v>99</v>
+      </c>
+      <c r="K879">
+        <v>47</v>
+      </c>
+      <c r="L879" t="s">
+        <v>822</v>
+      </c>
+      <c r="M879" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="880" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A880">
+        <v>1707</v>
+      </c>
+      <c r="B880">
+        <v>12</v>
+      </c>
+      <c r="C880" t="s">
+        <v>875</v>
+      </c>
+      <c r="J880" t="s">
+        <v>99</v>
+      </c>
+      <c r="K880">
+        <v>47</v>
+      </c>
+      <c r="L880" t="s">
+        <v>822</v>
+      </c>
+      <c r="M880" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="881" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A881">
+        <v>1707</v>
+      </c>
+      <c r="B881">
+        <v>12</v>
+      </c>
+      <c r="C881" t="s">
+        <v>876</v>
+      </c>
+      <c r="J881" t="s">
+        <v>99</v>
+      </c>
+      <c r="K881">
+        <v>47</v>
+      </c>
+      <c r="L881" t="s">
+        <v>822</v>
+      </c>
+      <c r="M881" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="882" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A882">
+        <v>1707</v>
+      </c>
+      <c r="B882">
+        <v>12</v>
+      </c>
+      <c r="C882" t="s">
+        <v>877</v>
+      </c>
+      <c r="J882" t="s">
+        <v>99</v>
+      </c>
+      <c r="K882">
+        <v>47</v>
+      </c>
+      <c r="L882" t="s">
+        <v>822</v>
+      </c>
+      <c r="M882" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="883" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A883">
+        <v>1707</v>
+      </c>
+      <c r="B883">
+        <v>13</v>
+      </c>
+      <c r="C883" t="s">
+        <v>878</v>
+      </c>
+      <c r="J883" t="s">
+        <v>99</v>
+      </c>
+      <c r="K883">
+        <v>47</v>
+      </c>
+      <c r="L883" t="s">
+        <v>822</v>
+      </c>
+      <c r="M883" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="884" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A884">
+        <v>1707</v>
+      </c>
+      <c r="B884">
+        <v>13</v>
+      </c>
+      <c r="C884" t="s">
+        <v>879</v>
+      </c>
+      <c r="J884" t="s">
+        <v>99</v>
+      </c>
+      <c r="K884">
+        <v>47</v>
+      </c>
+      <c r="L884" t="s">
+        <v>822</v>
+      </c>
+      <c r="M884" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="885" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A885">
+        <v>1707</v>
+      </c>
+      <c r="B885">
+        <v>13</v>
+      </c>
+      <c r="C885" t="s">
+        <v>880</v>
+      </c>
+      <c r="J885" t="s">
+        <v>99</v>
+      </c>
+      <c r="K885">
+        <v>47</v>
+      </c>
+      <c r="L885" t="s">
+        <v>822</v>
+      </c>
+      <c r="M885" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="886" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A886">
+        <v>1707</v>
+      </c>
+      <c r="B886">
+        <v>13</v>
+      </c>
+      <c r="C886" t="s">
+        <v>881</v>
+      </c>
+      <c r="J886" t="s">
+        <v>99</v>
+      </c>
+      <c r="K886">
+        <v>47</v>
+      </c>
+      <c r="L886" t="s">
+        <v>822</v>
+      </c>
+      <c r="M886" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="887" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A887">
+        <v>1707</v>
+      </c>
+      <c r="B887">
+        <v>13</v>
+      </c>
+      <c r="C887" t="s">
+        <v>882</v>
+      </c>
+      <c r="J887" t="s">
+        <v>99</v>
+      </c>
+      <c r="K887">
+        <v>47</v>
+      </c>
+      <c r="L887" t="s">
+        <v>822</v>
+      </c>
+      <c r="M887" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="888" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A888">
+        <v>1707</v>
+      </c>
+      <c r="B888">
+        <v>13</v>
+      </c>
+      <c r="C888" t="s">
+        <v>883</v>
+      </c>
+      <c r="J888" t="s">
+        <v>99</v>
+      </c>
+      <c r="K888">
+        <v>47</v>
+      </c>
+      <c r="L888" t="s">
+        <v>822</v>
+      </c>
+      <c r="M888" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="889" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A889">
+        <v>1707</v>
+      </c>
+      <c r="B889">
+        <v>14</v>
+      </c>
+      <c r="C889" t="s">
+        <v>884</v>
+      </c>
+      <c r="J889" t="s">
+        <v>99</v>
+      </c>
+      <c r="K889">
+        <v>47</v>
+      </c>
+      <c r="L889" t="s">
+        <v>822</v>
+      </c>
+      <c r="M889" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="890" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A890">
+        <v>1708</v>
+      </c>
+      <c r="B890">
+        <v>14</v>
+      </c>
+      <c r="C890" t="s">
+        <v>885</v>
+      </c>
+      <c r="J890" t="s">
+        <v>99</v>
+      </c>
+      <c r="K890">
+        <v>47</v>
+      </c>
+      <c r="L890" t="s">
+        <v>822</v>
+      </c>
+      <c r="M890" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="891" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A891">
+        <v>1709</v>
+      </c>
+      <c r="B891">
+        <v>14</v>
+      </c>
+      <c r="C891" t="s">
+        <v>886</v>
+      </c>
+      <c r="J891" t="s">
+        <v>99</v>
+      </c>
+      <c r="K891">
+        <v>47</v>
+      </c>
+      <c r="L891" t="s">
+        <v>822</v>
+      </c>
+      <c r="M891" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="892" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A892">
+        <v>1709</v>
+      </c>
+      <c r="B892">
+        <v>14</v>
+      </c>
+      <c r="C892" t="s">
+        <v>887</v>
+      </c>
+      <c r="J892" t="s">
+        <v>99</v>
+      </c>
+      <c r="K892">
+        <v>47</v>
+      </c>
+      <c r="L892" t="s">
+        <v>822</v>
+      </c>
+      <c r="M892" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="893" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A893">
+        <v>1709</v>
+      </c>
+      <c r="B893">
+        <v>14</v>
+      </c>
+      <c r="C893" t="s">
+        <v>888</v>
+      </c>
+      <c r="J893" t="s">
+        <v>99</v>
+      </c>
+      <c r="K893">
+        <v>47</v>
+      </c>
+      <c r="L893" t="s">
+        <v>822</v>
+      </c>
+      <c r="M893" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="894" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A894">
+        <v>1709</v>
+      </c>
+      <c r="B894">
+        <v>14</v>
+      </c>
+      <c r="C894" t="s">
+        <v>889</v>
+      </c>
+      <c r="J894" t="s">
+        <v>99</v>
+      </c>
+      <c r="K894">
+        <v>47</v>
+      </c>
+      <c r="L894" t="s">
+        <v>822</v>
+      </c>
+      <c r="M894" t="s">
+        <v>821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
indexació llibre 1693-1749 completa
</commit_message>
<xml_diff>
--- a/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
+++ b/Bisbats/Catalunya/Seu Urgell/Linyola/Sacraments/Matrimonis/Index_Llibres_Matrimonis_Linyola_Mormons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vstudio-code\repositorisArbre\DadesGenerals\Bisbats\Catalunya\Seu Urgell\Linyola\Sacraments\Matrimonis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5004A1-8031-4D3D-AF1D-F057D16B394E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2356D6E-6883-49EF-A620-F6D9DCB91930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C34A0C26-324D-4E17-B7B1-6D7DB0FCFBF8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3616" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4160" uniqueCount="1014">
   <si>
     <t>Cognoms Familia</t>
   </si>
@@ -2709,6 +2709,378 @@
   </si>
   <si>
     <t>Capdevila Bondal</t>
+  </si>
+  <si>
+    <t>Mosset Rialp</t>
+  </si>
+  <si>
+    <t>Torres Ballverdu</t>
+  </si>
+  <si>
+    <t>Guasch Macia</t>
+  </si>
+  <si>
+    <t>Batlle Mosset</t>
+  </si>
+  <si>
+    <t>Vallés Bonjorn</t>
+  </si>
+  <si>
+    <t>Curcó Giné</t>
+  </si>
+  <si>
+    <t>Trepat Martí</t>
+  </si>
+  <si>
+    <t>Domingo Mas</t>
+  </si>
+  <si>
+    <t>Palou Calaf</t>
+  </si>
+  <si>
+    <t>París Gene</t>
+  </si>
+  <si>
+    <t>Balaguer Martí</t>
+  </si>
+  <si>
+    <t>Pedrós Fabregat</t>
+  </si>
+  <si>
+    <t>Baga Fabregat</t>
+  </si>
+  <si>
+    <t>Pallas Pujades</t>
+  </si>
+  <si>
+    <t>Ques Carbí</t>
+  </si>
+  <si>
+    <t>Solà Vergé</t>
+  </si>
+  <si>
+    <t>Martí Torres</t>
+  </si>
+  <si>
+    <t>Tort Planes</t>
+  </si>
+  <si>
+    <t>Tarragó Roiger</t>
+  </si>
+  <si>
+    <t>Lluch Revert</t>
+  </si>
+  <si>
+    <t>Duch Capdevila</t>
+  </si>
+  <si>
+    <t>Felip Hospital</t>
+  </si>
+  <si>
+    <t>Queralt Agulló</t>
+  </si>
+  <si>
+    <t>Ganyet Fenoll</t>
+  </si>
+  <si>
+    <t>vidal Fontanals</t>
+  </si>
+  <si>
+    <t>Estruch Calaf</t>
+  </si>
+  <si>
+    <t>Saltó Solà</t>
+  </si>
+  <si>
+    <t>Valls Mas</t>
+  </si>
+  <si>
+    <t>Carrera Mosset</t>
+  </si>
+  <si>
+    <t>Ginestà Pallàs</t>
+  </si>
+  <si>
+    <t>Estradé Mosset</t>
+  </si>
+  <si>
+    <t>Batlle Mirassó</t>
+  </si>
+  <si>
+    <t>Mas Roma</t>
+  </si>
+  <si>
+    <t>Rubiol Cors</t>
+  </si>
+  <si>
+    <t>Bellet Roiger</t>
+  </si>
+  <si>
+    <t>Pujades Mas</t>
+  </si>
+  <si>
+    <t>Mata Mosset</t>
+  </si>
+  <si>
+    <t>Cuberes Pujades</t>
+  </si>
+  <si>
+    <t>Fenoll Planes</t>
+  </si>
+  <si>
+    <t>Mas Serra</t>
+  </si>
+  <si>
+    <t>Pujol Druet</t>
+  </si>
+  <si>
+    <t>Giné Mercé</t>
+  </si>
+  <si>
+    <t>Soler Martí</t>
+  </si>
+  <si>
+    <t>Mas Mas</t>
+  </si>
+  <si>
+    <t>Feres Cluet</t>
+  </si>
+  <si>
+    <t>Eroles Roigé</t>
+  </si>
+  <si>
+    <t>Miró Galceran</t>
+  </si>
+  <si>
+    <t>Vidal Lamarca</t>
+  </si>
+  <si>
+    <t>Mas Coll</t>
+  </si>
+  <si>
+    <t>Rosell Gasol</t>
+  </si>
+  <si>
+    <t>Cluet Cluet</t>
+  </si>
+  <si>
+    <t>Planes Roiger</t>
+  </si>
+  <si>
+    <t>Martí Civit</t>
+  </si>
+  <si>
+    <t>Roma Martí</t>
+  </si>
+  <si>
+    <t>Llaudet Marí</t>
+  </si>
+  <si>
+    <t>Mata Tonijoan</t>
+  </si>
+  <si>
+    <t>Fabregat Miraso</t>
+  </si>
+  <si>
+    <t>Roig Farrerich</t>
+  </si>
+  <si>
+    <t>Camrubí Pera</t>
+  </si>
+  <si>
+    <t>Mas Agulló</t>
+  </si>
+  <si>
+    <t>Gavarró Martí</t>
+  </si>
+  <si>
+    <t>Novell Solà</t>
+  </si>
+  <si>
+    <t>Solé Margall</t>
+  </si>
+  <si>
+    <t>Galceran Colell</t>
+  </si>
+  <si>
+    <t>Casals Pedrós</t>
+  </si>
+  <si>
+    <t>Agulló Arqullol</t>
+  </si>
+  <si>
+    <t>Mosset Agulló</t>
+  </si>
+  <si>
+    <t>Arrufat Monfà</t>
+  </si>
+  <si>
+    <t>Farrerich Plà</t>
+  </si>
+  <si>
+    <t>Mata Vinyes</t>
+  </si>
+  <si>
+    <t>Fabregat Soler</t>
+  </si>
+  <si>
+    <t>Torrent Fabregat</t>
+  </si>
+  <si>
+    <t>Oriola Mosset</t>
+  </si>
+  <si>
+    <t>Agulló Domingo</t>
+  </si>
+  <si>
+    <t>Almenar Gine</t>
+  </si>
+  <si>
+    <t>Torres Roma</t>
+  </si>
+  <si>
+    <t>Torrelles Corberó</t>
+  </si>
+  <si>
+    <t>Curcó Moragues</t>
+  </si>
+  <si>
+    <t>Xandre Pedrós</t>
+  </si>
+  <si>
+    <t>Pedrós Serra</t>
+  </si>
+  <si>
+    <t>Giné Mosset</t>
+  </si>
+  <si>
+    <t>Carulla Cuberes</t>
+  </si>
+  <si>
+    <t>Planes Giné</t>
+  </si>
+  <si>
+    <t>Rodón Graells</t>
+  </si>
+  <si>
+    <t>Vallés Serra</t>
+  </si>
+  <si>
+    <t>Farré Pallàs</t>
+  </si>
+  <si>
+    <t>Boladeres Trilla</t>
+  </si>
+  <si>
+    <t>Renyé Bagà</t>
+  </si>
+  <si>
+    <t>Planes Palou</t>
+  </si>
+  <si>
+    <t>Curcó Aspa</t>
+  </si>
+  <si>
+    <t>Folguera Feliu</t>
+  </si>
+  <si>
+    <t>Folguera Cuberes</t>
+  </si>
+  <si>
+    <t>Giné Faiges</t>
+  </si>
+  <si>
+    <t>Teixidó Palou</t>
+  </si>
+  <si>
+    <t>Guasch Bonjorn</t>
+  </si>
+  <si>
+    <t>Violant Vilaplana</t>
+  </si>
+  <si>
+    <t>Novell Huguet</t>
+  </si>
+  <si>
+    <t>Combes Mosset</t>
+  </si>
+  <si>
+    <t>Farreny Mas</t>
+  </si>
+  <si>
+    <t>Mir Solanes</t>
+  </si>
+  <si>
+    <t>Torrent Domingo</t>
+  </si>
+  <si>
+    <t>Fontich Mó</t>
+  </si>
+  <si>
+    <t>Mirassó Druet</t>
+  </si>
+  <si>
+    <t>Civit Torrent</t>
+  </si>
+  <si>
+    <t>Agulló Mó</t>
+  </si>
+  <si>
+    <t>Lluch Pujol</t>
+  </si>
+  <si>
+    <t>Ganyet Agulló</t>
+  </si>
+  <si>
+    <t>Perera Novell</t>
+  </si>
+  <si>
+    <t>Fontanals Camps</t>
+  </si>
+  <si>
+    <t>Garcia Gerené</t>
+  </si>
+  <si>
+    <t>Coll Bosch</t>
+  </si>
+  <si>
+    <t>Planes Amargall</t>
+  </si>
+  <si>
+    <t>Ganyet Soler</t>
+  </si>
+  <si>
+    <t>Oriola Fortuny</t>
+  </si>
+  <si>
+    <t>Gasol Partella</t>
+  </si>
+  <si>
+    <t>Mas Gené</t>
+  </si>
+  <si>
+    <t>Margall Bonjorn</t>
+  </si>
+  <si>
+    <t>Argilés Agulló</t>
+  </si>
+  <si>
+    <t>Torrent Mas</t>
+  </si>
+  <si>
+    <t>Eloi Amargall</t>
+  </si>
+  <si>
+    <t>Roig Pallás</t>
+  </si>
+  <si>
+    <t>Aldosa Roca</t>
+  </si>
+  <si>
+    <t>Martí Pedrós</t>
+  </si>
+  <si>
+    <t>Bellet Colell</t>
   </si>
 </sst>
 </file>
@@ -3063,11 +3435,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}">
-  <dimension ref="A1:N894"/>
+  <dimension ref="A1:N1030"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A861" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A895" sqref="A895"/>
+      <pane ySplit="1" topLeftCell="A808" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E984" sqref="E984"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23746,6 +24118,3134 @@
         <v>821</v>
       </c>
     </row>
+    <row r="895" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A895">
+        <v>1710</v>
+      </c>
+      <c r="B895">
+        <v>15</v>
+      </c>
+      <c r="C895" t="s">
+        <v>890</v>
+      </c>
+      <c r="J895" t="s">
+        <v>99</v>
+      </c>
+      <c r="K895">
+        <v>47</v>
+      </c>
+      <c r="L895" t="s">
+        <v>822</v>
+      </c>
+      <c r="M895" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="896" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A896">
+        <v>1711</v>
+      </c>
+      <c r="B896">
+        <v>15</v>
+      </c>
+      <c r="C896" t="s">
+        <v>891</v>
+      </c>
+      <c r="J896" t="s">
+        <v>99</v>
+      </c>
+      <c r="K896">
+        <v>47</v>
+      </c>
+      <c r="L896" t="s">
+        <v>822</v>
+      </c>
+      <c r="M896" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="897" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A897">
+        <v>1712</v>
+      </c>
+      <c r="B897">
+        <v>15</v>
+      </c>
+      <c r="C897" t="s">
+        <v>892</v>
+      </c>
+      <c r="J897" t="s">
+        <v>99</v>
+      </c>
+      <c r="K897">
+        <v>47</v>
+      </c>
+      <c r="L897" t="s">
+        <v>822</v>
+      </c>
+      <c r="M897" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="898" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A898">
+        <v>1712</v>
+      </c>
+      <c r="B898">
+        <v>15</v>
+      </c>
+      <c r="C898" t="s">
+        <v>125</v>
+      </c>
+      <c r="J898" t="s">
+        <v>99</v>
+      </c>
+      <c r="K898">
+        <v>47</v>
+      </c>
+      <c r="L898" t="s">
+        <v>822</v>
+      </c>
+      <c r="M898" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="899" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A899">
+        <v>1713</v>
+      </c>
+      <c r="B899">
+        <v>16</v>
+      </c>
+      <c r="C899" t="s">
+        <v>893</v>
+      </c>
+      <c r="J899" t="s">
+        <v>99</v>
+      </c>
+      <c r="K899">
+        <v>47</v>
+      </c>
+      <c r="L899" t="s">
+        <v>822</v>
+      </c>
+      <c r="M899" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="900" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A900">
+        <v>1713</v>
+      </c>
+      <c r="B900">
+        <v>16</v>
+      </c>
+      <c r="C900" t="s">
+        <v>894</v>
+      </c>
+      <c r="J900" t="s">
+        <v>99</v>
+      </c>
+      <c r="K900">
+        <v>47</v>
+      </c>
+      <c r="L900" t="s">
+        <v>822</v>
+      </c>
+      <c r="M900" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="901" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A901">
+        <v>1713</v>
+      </c>
+      <c r="B901">
+        <v>16</v>
+      </c>
+      <c r="C901" t="s">
+        <v>895</v>
+      </c>
+      <c r="J901" t="s">
+        <v>99</v>
+      </c>
+      <c r="K901">
+        <v>47</v>
+      </c>
+      <c r="L901" t="s">
+        <v>822</v>
+      </c>
+      <c r="M901" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="902" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A902">
+        <v>1713</v>
+      </c>
+      <c r="B902">
+        <v>17</v>
+      </c>
+      <c r="C902" t="s">
+        <v>896</v>
+      </c>
+      <c r="J902" t="s">
+        <v>99</v>
+      </c>
+      <c r="K902">
+        <v>47</v>
+      </c>
+      <c r="L902" t="s">
+        <v>822</v>
+      </c>
+      <c r="M902" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="903" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A903">
+        <v>1713</v>
+      </c>
+      <c r="B903">
+        <v>17</v>
+      </c>
+      <c r="C903" t="s">
+        <v>897</v>
+      </c>
+      <c r="J903" t="s">
+        <v>99</v>
+      </c>
+      <c r="K903">
+        <v>47</v>
+      </c>
+      <c r="L903" t="s">
+        <v>822</v>
+      </c>
+      <c r="M903" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="904" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A904">
+        <v>1714</v>
+      </c>
+      <c r="B904">
+        <v>17</v>
+      </c>
+      <c r="C904" t="s">
+        <v>898</v>
+      </c>
+      <c r="J904" t="s">
+        <v>99</v>
+      </c>
+      <c r="K904">
+        <v>47</v>
+      </c>
+      <c r="L904" t="s">
+        <v>822</v>
+      </c>
+      <c r="M904" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="905" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A905">
+        <v>1714</v>
+      </c>
+      <c r="B905">
+        <v>18</v>
+      </c>
+      <c r="C905" t="s">
+        <v>899</v>
+      </c>
+      <c r="J905" t="s">
+        <v>99</v>
+      </c>
+      <c r="K905">
+        <v>47</v>
+      </c>
+      <c r="L905" t="s">
+        <v>822</v>
+      </c>
+      <c r="M905" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="906" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A906">
+        <v>1714</v>
+      </c>
+      <c r="B906">
+        <v>18</v>
+      </c>
+      <c r="C906" t="s">
+        <v>900</v>
+      </c>
+      <c r="J906" t="s">
+        <v>99</v>
+      </c>
+      <c r="K906">
+        <v>47</v>
+      </c>
+      <c r="L906" t="s">
+        <v>822</v>
+      </c>
+      <c r="M906" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="907" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A907">
+        <v>1715</v>
+      </c>
+      <c r="B907">
+        <v>18</v>
+      </c>
+      <c r="C907" t="s">
+        <v>901</v>
+      </c>
+      <c r="J907" t="s">
+        <v>99</v>
+      </c>
+      <c r="K907">
+        <v>47</v>
+      </c>
+      <c r="L907" t="s">
+        <v>822</v>
+      </c>
+      <c r="M907" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="908" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A908">
+        <v>1715</v>
+      </c>
+      <c r="B908">
+        <v>18</v>
+      </c>
+      <c r="C908" t="s">
+        <v>902</v>
+      </c>
+      <c r="J908" t="s">
+        <v>99</v>
+      </c>
+      <c r="K908">
+        <v>47</v>
+      </c>
+      <c r="L908" t="s">
+        <v>822</v>
+      </c>
+      <c r="M908" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="909" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A909">
+        <v>1715</v>
+      </c>
+      <c r="B909">
+        <v>19</v>
+      </c>
+      <c r="C909" t="s">
+        <v>903</v>
+      </c>
+      <c r="J909" t="s">
+        <v>99</v>
+      </c>
+      <c r="K909">
+        <v>47</v>
+      </c>
+      <c r="L909" t="s">
+        <v>822</v>
+      </c>
+      <c r="M909" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="910" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A910">
+        <v>1716</v>
+      </c>
+      <c r="B910">
+        <v>19</v>
+      </c>
+      <c r="C910" t="s">
+        <v>904</v>
+      </c>
+      <c r="J910" t="s">
+        <v>99</v>
+      </c>
+      <c r="K910">
+        <v>47</v>
+      </c>
+      <c r="L910" t="s">
+        <v>822</v>
+      </c>
+      <c r="M910" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="911" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A911">
+        <v>1716</v>
+      </c>
+      <c r="B911">
+        <v>19</v>
+      </c>
+      <c r="C911" t="s">
+        <v>333</v>
+      </c>
+      <c r="J911" t="s">
+        <v>99</v>
+      </c>
+      <c r="K911">
+        <v>47</v>
+      </c>
+      <c r="L911" t="s">
+        <v>822</v>
+      </c>
+      <c r="M911" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="912" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A912">
+        <v>1716</v>
+      </c>
+      <c r="B912">
+        <v>19</v>
+      </c>
+      <c r="C912" t="s">
+        <v>905</v>
+      </c>
+      <c r="J912" t="s">
+        <v>99</v>
+      </c>
+      <c r="K912">
+        <v>47</v>
+      </c>
+      <c r="L912" t="s">
+        <v>822</v>
+      </c>
+      <c r="M912" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="913" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A913">
+        <v>1716</v>
+      </c>
+      <c r="B913">
+        <v>20</v>
+      </c>
+      <c r="C913" t="s">
+        <v>906</v>
+      </c>
+      <c r="J913" t="s">
+        <v>99</v>
+      </c>
+      <c r="K913">
+        <v>47</v>
+      </c>
+      <c r="L913" t="s">
+        <v>822</v>
+      </c>
+      <c r="M913" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="914" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A914">
+        <v>1716</v>
+      </c>
+      <c r="B914">
+        <v>20</v>
+      </c>
+      <c r="C914" t="s">
+        <v>907</v>
+      </c>
+      <c r="J914" t="s">
+        <v>99</v>
+      </c>
+      <c r="K914">
+        <v>47</v>
+      </c>
+      <c r="L914" t="s">
+        <v>822</v>
+      </c>
+      <c r="M914" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="915" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A915">
+        <v>1717</v>
+      </c>
+      <c r="B915">
+        <v>20</v>
+      </c>
+      <c r="C915" t="s">
+        <v>908</v>
+      </c>
+      <c r="J915" t="s">
+        <v>99</v>
+      </c>
+      <c r="K915">
+        <v>47</v>
+      </c>
+      <c r="L915" t="s">
+        <v>822</v>
+      </c>
+      <c r="M915" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="916" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A916">
+        <v>1717</v>
+      </c>
+      <c r="B916">
+        <v>21</v>
+      </c>
+      <c r="C916" t="s">
+        <v>909</v>
+      </c>
+      <c r="J916" t="s">
+        <v>99</v>
+      </c>
+      <c r="K916">
+        <v>47</v>
+      </c>
+      <c r="L916" t="s">
+        <v>822</v>
+      </c>
+      <c r="M916" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="917" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A917">
+        <v>1717</v>
+      </c>
+      <c r="B917">
+        <v>21</v>
+      </c>
+      <c r="C917" t="s">
+        <v>570</v>
+      </c>
+      <c r="J917" t="s">
+        <v>99</v>
+      </c>
+      <c r="K917">
+        <v>47</v>
+      </c>
+      <c r="L917" t="s">
+        <v>822</v>
+      </c>
+      <c r="M917" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="918" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A918">
+        <v>1717</v>
+      </c>
+      <c r="B918">
+        <v>21</v>
+      </c>
+      <c r="C918" t="s">
+        <v>910</v>
+      </c>
+      <c r="J918" t="s">
+        <v>99</v>
+      </c>
+      <c r="K918">
+        <v>47</v>
+      </c>
+      <c r="L918" t="s">
+        <v>822</v>
+      </c>
+      <c r="M918" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="919" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A919">
+        <v>1718</v>
+      </c>
+      <c r="B919">
+        <v>22</v>
+      </c>
+      <c r="C919" t="s">
+        <v>911</v>
+      </c>
+      <c r="J919" t="s">
+        <v>99</v>
+      </c>
+      <c r="K919">
+        <v>47</v>
+      </c>
+      <c r="L919" t="s">
+        <v>822</v>
+      </c>
+      <c r="M919" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="920" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A920">
+        <v>1718</v>
+      </c>
+      <c r="B920">
+        <v>22</v>
+      </c>
+      <c r="C920" t="s">
+        <v>912</v>
+      </c>
+      <c r="J920" t="s">
+        <v>99</v>
+      </c>
+      <c r="K920">
+        <v>47</v>
+      </c>
+      <c r="L920" t="s">
+        <v>822</v>
+      </c>
+      <c r="M920" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="921" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A921">
+        <v>1718</v>
+      </c>
+      <c r="B921">
+        <v>22</v>
+      </c>
+      <c r="C921" t="s">
+        <v>913</v>
+      </c>
+      <c r="J921" t="s">
+        <v>99</v>
+      </c>
+      <c r="K921">
+        <v>47</v>
+      </c>
+      <c r="L921" t="s">
+        <v>822</v>
+      </c>
+      <c r="M921" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="922" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A922">
+        <v>1718</v>
+      </c>
+      <c r="B922">
+        <v>22</v>
+      </c>
+      <c r="C922" t="s">
+        <v>914</v>
+      </c>
+      <c r="J922" t="s">
+        <v>99</v>
+      </c>
+      <c r="K922">
+        <v>47</v>
+      </c>
+      <c r="L922" t="s">
+        <v>822</v>
+      </c>
+      <c r="M922" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="923" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A923">
+        <v>1719</v>
+      </c>
+      <c r="B923">
+        <v>23</v>
+      </c>
+      <c r="C923" t="s">
+        <v>915</v>
+      </c>
+      <c r="J923" t="s">
+        <v>99</v>
+      </c>
+      <c r="K923">
+        <v>47</v>
+      </c>
+      <c r="L923" t="s">
+        <v>822</v>
+      </c>
+      <c r="M923" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="924" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A924">
+        <v>1719</v>
+      </c>
+      <c r="B924">
+        <v>23</v>
+      </c>
+      <c r="C924" t="s">
+        <v>916</v>
+      </c>
+      <c r="J924" t="s">
+        <v>99</v>
+      </c>
+      <c r="K924">
+        <v>47</v>
+      </c>
+      <c r="L924" t="s">
+        <v>822</v>
+      </c>
+      <c r="M924" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="925" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A925">
+        <v>1719</v>
+      </c>
+      <c r="B925">
+        <v>23</v>
+      </c>
+      <c r="C925" t="s">
+        <v>917</v>
+      </c>
+      <c r="J925" t="s">
+        <v>99</v>
+      </c>
+      <c r="K925">
+        <v>47</v>
+      </c>
+      <c r="L925" t="s">
+        <v>822</v>
+      </c>
+      <c r="M925" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="926" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A926">
+        <v>1720</v>
+      </c>
+      <c r="B926">
+        <v>24</v>
+      </c>
+      <c r="C926" t="s">
+        <v>918</v>
+      </c>
+      <c r="J926" t="s">
+        <v>99</v>
+      </c>
+      <c r="K926">
+        <v>47</v>
+      </c>
+      <c r="L926" t="s">
+        <v>822</v>
+      </c>
+      <c r="M926" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="927" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A927">
+        <v>1720</v>
+      </c>
+      <c r="B927">
+        <v>24</v>
+      </c>
+      <c r="C927" t="s">
+        <v>919</v>
+      </c>
+      <c r="J927" t="s">
+        <v>99</v>
+      </c>
+      <c r="K927">
+        <v>47</v>
+      </c>
+      <c r="L927" t="s">
+        <v>822</v>
+      </c>
+      <c r="M927" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="928" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A928">
+        <v>1720</v>
+      </c>
+      <c r="B928">
+        <v>24</v>
+      </c>
+      <c r="C928" t="s">
+        <v>920</v>
+      </c>
+      <c r="J928" t="s">
+        <v>99</v>
+      </c>
+      <c r="K928">
+        <v>47</v>
+      </c>
+      <c r="L928" t="s">
+        <v>822</v>
+      </c>
+      <c r="M928" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="929" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A929">
+        <v>1720</v>
+      </c>
+      <c r="B929">
+        <v>24</v>
+      </c>
+      <c r="C929" t="s">
+        <v>921</v>
+      </c>
+      <c r="J929" t="s">
+        <v>99</v>
+      </c>
+      <c r="K929">
+        <v>47</v>
+      </c>
+      <c r="L929" t="s">
+        <v>822</v>
+      </c>
+      <c r="M929" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="930" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A930">
+        <v>1720</v>
+      </c>
+      <c r="B930">
+        <v>25</v>
+      </c>
+      <c r="C930" t="s">
+        <v>922</v>
+      </c>
+      <c r="J930" t="s">
+        <v>99</v>
+      </c>
+      <c r="K930">
+        <v>47</v>
+      </c>
+      <c r="L930" t="s">
+        <v>822</v>
+      </c>
+      <c r="M930" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="931" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A931">
+        <v>1721</v>
+      </c>
+      <c r="B931">
+        <v>25</v>
+      </c>
+      <c r="C931" t="s">
+        <v>923</v>
+      </c>
+      <c r="J931" t="s">
+        <v>99</v>
+      </c>
+      <c r="K931">
+        <v>47</v>
+      </c>
+      <c r="L931" t="s">
+        <v>822</v>
+      </c>
+      <c r="M931" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="932" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A932">
+        <v>1721</v>
+      </c>
+      <c r="B932">
+        <v>25</v>
+      </c>
+      <c r="C932" t="s">
+        <v>558</v>
+      </c>
+      <c r="J932" t="s">
+        <v>99</v>
+      </c>
+      <c r="K932">
+        <v>47</v>
+      </c>
+      <c r="L932" t="s">
+        <v>822</v>
+      </c>
+      <c r="M932" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="933" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A933">
+        <v>1721</v>
+      </c>
+      <c r="B933">
+        <v>26</v>
+      </c>
+      <c r="C933" t="s">
+        <v>924</v>
+      </c>
+      <c r="J933" t="s">
+        <v>99</v>
+      </c>
+      <c r="K933">
+        <v>47</v>
+      </c>
+      <c r="L933" t="s">
+        <v>822</v>
+      </c>
+      <c r="M933" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="934" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A934">
+        <v>1722</v>
+      </c>
+      <c r="B934">
+        <v>26</v>
+      </c>
+      <c r="C934" t="s">
+        <v>925</v>
+      </c>
+      <c r="J934" t="s">
+        <v>99</v>
+      </c>
+      <c r="K934">
+        <v>47</v>
+      </c>
+      <c r="L934" t="s">
+        <v>822</v>
+      </c>
+      <c r="M934" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="935" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A935">
+        <v>1723</v>
+      </c>
+      <c r="B935">
+        <v>26</v>
+      </c>
+      <c r="C935" t="s">
+        <v>926</v>
+      </c>
+      <c r="J935" t="s">
+        <v>99</v>
+      </c>
+      <c r="K935">
+        <v>47</v>
+      </c>
+      <c r="L935" t="s">
+        <v>822</v>
+      </c>
+      <c r="M935" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="936" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A936">
+        <v>1724</v>
+      </c>
+      <c r="B936">
+        <v>26</v>
+      </c>
+      <c r="C936" t="s">
+        <v>927</v>
+      </c>
+      <c r="J936" t="s">
+        <v>99</v>
+      </c>
+      <c r="K936">
+        <v>47</v>
+      </c>
+      <c r="L936" t="s">
+        <v>822</v>
+      </c>
+      <c r="M936" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="937" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A937">
+        <v>1724</v>
+      </c>
+      <c r="B937">
+        <v>26</v>
+      </c>
+      <c r="C937" t="s">
+        <v>928</v>
+      </c>
+      <c r="J937" t="s">
+        <v>99</v>
+      </c>
+      <c r="K937">
+        <v>47</v>
+      </c>
+      <c r="L937" t="s">
+        <v>822</v>
+      </c>
+      <c r="M937" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="938" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A938">
+        <v>1725</v>
+      </c>
+      <c r="B938">
+        <v>27</v>
+      </c>
+      <c r="C938" t="s">
+        <v>281</v>
+      </c>
+      <c r="J938" t="s">
+        <v>99</v>
+      </c>
+      <c r="K938">
+        <v>47</v>
+      </c>
+      <c r="L938" t="s">
+        <v>822</v>
+      </c>
+      <c r="M938" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="939" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A939">
+        <v>1725</v>
+      </c>
+      <c r="B939">
+        <v>27</v>
+      </c>
+      <c r="C939" t="s">
+        <v>179</v>
+      </c>
+      <c r="J939" t="s">
+        <v>99</v>
+      </c>
+      <c r="K939">
+        <v>47</v>
+      </c>
+      <c r="L939" t="s">
+        <v>822</v>
+      </c>
+      <c r="M939" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="940" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A940">
+        <v>1725</v>
+      </c>
+      <c r="B940">
+        <v>27</v>
+      </c>
+      <c r="C940" t="s">
+        <v>929</v>
+      </c>
+      <c r="J940" t="s">
+        <v>99</v>
+      </c>
+      <c r="K940">
+        <v>47</v>
+      </c>
+      <c r="L940" t="s">
+        <v>822</v>
+      </c>
+      <c r="M940" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="941" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A941">
+        <v>1725</v>
+      </c>
+      <c r="B941">
+        <v>27</v>
+      </c>
+      <c r="C941" t="s">
+        <v>930</v>
+      </c>
+      <c r="J941" t="s">
+        <v>99</v>
+      </c>
+      <c r="K941">
+        <v>47</v>
+      </c>
+      <c r="L941" t="s">
+        <v>822</v>
+      </c>
+      <c r="M941" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="942" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A942">
+        <v>1725</v>
+      </c>
+      <c r="B942">
+        <v>28</v>
+      </c>
+      <c r="C942" t="s">
+        <v>325</v>
+      </c>
+      <c r="J942" t="s">
+        <v>99</v>
+      </c>
+      <c r="K942">
+        <v>47</v>
+      </c>
+      <c r="L942" t="s">
+        <v>822</v>
+      </c>
+      <c r="M942" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="943" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A943">
+        <v>1726</v>
+      </c>
+      <c r="B943">
+        <v>28</v>
+      </c>
+      <c r="C943" t="s">
+        <v>931</v>
+      </c>
+      <c r="J943" t="s">
+        <v>99</v>
+      </c>
+      <c r="K943">
+        <v>47</v>
+      </c>
+      <c r="L943" t="s">
+        <v>822</v>
+      </c>
+      <c r="M943" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="944" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A944">
+        <v>1726</v>
+      </c>
+      <c r="B944">
+        <v>28</v>
+      </c>
+      <c r="C944" t="s">
+        <v>932</v>
+      </c>
+      <c r="J944" t="s">
+        <v>99</v>
+      </c>
+      <c r="K944">
+        <v>47</v>
+      </c>
+      <c r="L944" t="s">
+        <v>822</v>
+      </c>
+      <c r="M944" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="945" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A945">
+        <v>1726</v>
+      </c>
+      <c r="B945">
+        <v>28</v>
+      </c>
+      <c r="C945" t="s">
+        <v>365</v>
+      </c>
+      <c r="J945" t="s">
+        <v>99</v>
+      </c>
+      <c r="K945">
+        <v>47</v>
+      </c>
+      <c r="L945" t="s">
+        <v>822</v>
+      </c>
+      <c r="M945" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="946" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A946">
+        <v>1726</v>
+      </c>
+      <c r="B946">
+        <v>28</v>
+      </c>
+      <c r="C946" t="s">
+        <v>933</v>
+      </c>
+      <c r="J946" t="s">
+        <v>99</v>
+      </c>
+      <c r="K946">
+        <v>47</v>
+      </c>
+      <c r="L946" t="s">
+        <v>822</v>
+      </c>
+      <c r="M946" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="947" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A947">
+        <v>1727</v>
+      </c>
+      <c r="B947">
+        <v>29</v>
+      </c>
+      <c r="C947" t="s">
+        <v>934</v>
+      </c>
+      <c r="J947" t="s">
+        <v>99</v>
+      </c>
+      <c r="K947">
+        <v>47</v>
+      </c>
+      <c r="L947" t="s">
+        <v>822</v>
+      </c>
+      <c r="M947" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="948" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A948">
+        <v>1727</v>
+      </c>
+      <c r="B948">
+        <v>29</v>
+      </c>
+      <c r="C948" t="s">
+        <v>935</v>
+      </c>
+      <c r="J948" t="s">
+        <v>99</v>
+      </c>
+      <c r="K948">
+        <v>47</v>
+      </c>
+      <c r="L948" t="s">
+        <v>822</v>
+      </c>
+      <c r="M948" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="949" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A949">
+        <v>1727</v>
+      </c>
+      <c r="B949">
+        <v>29</v>
+      </c>
+      <c r="C949" t="s">
+        <v>936</v>
+      </c>
+      <c r="J949" t="s">
+        <v>99</v>
+      </c>
+      <c r="K949">
+        <v>47</v>
+      </c>
+      <c r="L949" t="s">
+        <v>822</v>
+      </c>
+      <c r="M949" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="950" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A950">
+        <v>1727</v>
+      </c>
+      <c r="B950">
+        <v>29</v>
+      </c>
+      <c r="C950" t="s">
+        <v>937</v>
+      </c>
+      <c r="J950" t="s">
+        <v>99</v>
+      </c>
+      <c r="K950">
+        <v>47</v>
+      </c>
+      <c r="L950" t="s">
+        <v>822</v>
+      </c>
+      <c r="M950" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="951" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A951">
+        <v>1727</v>
+      </c>
+      <c r="B951">
+        <v>29</v>
+      </c>
+      <c r="C951" t="s">
+        <v>937</v>
+      </c>
+      <c r="J951" t="s">
+        <v>99</v>
+      </c>
+      <c r="K951">
+        <v>47</v>
+      </c>
+      <c r="L951" t="s">
+        <v>822</v>
+      </c>
+      <c r="M951" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="952" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A952">
+        <v>1728</v>
+      </c>
+      <c r="B952">
+        <v>30</v>
+      </c>
+      <c r="C952" t="s">
+        <v>938</v>
+      </c>
+      <c r="J952" t="s">
+        <v>99</v>
+      </c>
+      <c r="K952">
+        <v>47</v>
+      </c>
+      <c r="L952" t="s">
+        <v>822</v>
+      </c>
+      <c r="M952" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="953" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A953">
+        <v>1728</v>
+      </c>
+      <c r="B953">
+        <v>30</v>
+      </c>
+      <c r="C953" t="s">
+        <v>756</v>
+      </c>
+      <c r="J953" t="s">
+        <v>99</v>
+      </c>
+      <c r="K953">
+        <v>47</v>
+      </c>
+      <c r="L953" t="s">
+        <v>822</v>
+      </c>
+      <c r="M953" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="954" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A954">
+        <v>1728</v>
+      </c>
+      <c r="B954">
+        <v>30</v>
+      </c>
+      <c r="C954" t="s">
+        <v>939</v>
+      </c>
+      <c r="J954" t="s">
+        <v>99</v>
+      </c>
+      <c r="K954">
+        <v>47</v>
+      </c>
+      <c r="L954" t="s">
+        <v>822</v>
+      </c>
+      <c r="M954" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="955" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A955">
+        <v>1729</v>
+      </c>
+      <c r="B955">
+        <v>30</v>
+      </c>
+      <c r="C955" t="s">
+        <v>940</v>
+      </c>
+      <c r="J955" t="s">
+        <v>99</v>
+      </c>
+      <c r="K955">
+        <v>47</v>
+      </c>
+      <c r="L955" t="s">
+        <v>822</v>
+      </c>
+      <c r="M955" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="956" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A956">
+        <v>1729</v>
+      </c>
+      <c r="B956">
+        <v>30</v>
+      </c>
+      <c r="C956" t="s">
+        <v>941</v>
+      </c>
+      <c r="J956" t="s">
+        <v>99</v>
+      </c>
+      <c r="K956">
+        <v>47</v>
+      </c>
+      <c r="L956" t="s">
+        <v>822</v>
+      </c>
+      <c r="M956" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="957" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A957">
+        <v>1729</v>
+      </c>
+      <c r="B957">
+        <v>30</v>
+      </c>
+      <c r="C957" t="s">
+        <v>942</v>
+      </c>
+      <c r="J957" t="s">
+        <v>99</v>
+      </c>
+      <c r="K957">
+        <v>47</v>
+      </c>
+      <c r="L957" t="s">
+        <v>822</v>
+      </c>
+      <c r="M957" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="958" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A958">
+        <v>1729</v>
+      </c>
+      <c r="B958">
+        <v>31</v>
+      </c>
+      <c r="C958" t="s">
+        <v>738</v>
+      </c>
+      <c r="J958" t="s">
+        <v>99</v>
+      </c>
+      <c r="K958">
+        <v>47</v>
+      </c>
+      <c r="L958" t="s">
+        <v>822</v>
+      </c>
+      <c r="M958" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="959" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A959">
+        <v>1729</v>
+      </c>
+      <c r="B959">
+        <v>31</v>
+      </c>
+      <c r="C959" t="s">
+        <v>943</v>
+      </c>
+      <c r="J959" t="s">
+        <v>99</v>
+      </c>
+      <c r="K959">
+        <v>47</v>
+      </c>
+      <c r="L959" t="s">
+        <v>822</v>
+      </c>
+      <c r="M959" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="960" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A960">
+        <v>1730</v>
+      </c>
+      <c r="B960">
+        <v>31</v>
+      </c>
+      <c r="C960" t="s">
+        <v>944</v>
+      </c>
+      <c r="J960" t="s">
+        <v>99</v>
+      </c>
+      <c r="K960">
+        <v>47</v>
+      </c>
+      <c r="L960" t="s">
+        <v>822</v>
+      </c>
+      <c r="M960" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="961" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A961">
+        <v>1730</v>
+      </c>
+      <c r="B961">
+        <v>31</v>
+      </c>
+      <c r="C961" t="s">
+        <v>897</v>
+      </c>
+      <c r="J961" t="s">
+        <v>99</v>
+      </c>
+      <c r="K961">
+        <v>47</v>
+      </c>
+      <c r="L961" t="s">
+        <v>822</v>
+      </c>
+      <c r="M961" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="962" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A962">
+        <v>1730</v>
+      </c>
+      <c r="B962">
+        <v>31</v>
+      </c>
+      <c r="C962" t="s">
+        <v>945</v>
+      </c>
+      <c r="J962" t="s">
+        <v>99</v>
+      </c>
+      <c r="K962">
+        <v>47</v>
+      </c>
+      <c r="L962" t="s">
+        <v>822</v>
+      </c>
+      <c r="M962" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="963" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A963">
+        <v>1731</v>
+      </c>
+      <c r="B963">
+        <v>32</v>
+      </c>
+      <c r="C963" t="s">
+        <v>946</v>
+      </c>
+      <c r="J963" t="s">
+        <v>99</v>
+      </c>
+      <c r="K963">
+        <v>47</v>
+      </c>
+      <c r="L963" t="s">
+        <v>822</v>
+      </c>
+      <c r="M963" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="964" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A964">
+        <v>1731</v>
+      </c>
+      <c r="B964">
+        <v>32</v>
+      </c>
+      <c r="C964" t="s">
+        <v>947</v>
+      </c>
+      <c r="J964" t="s">
+        <v>99</v>
+      </c>
+      <c r="K964">
+        <v>47</v>
+      </c>
+      <c r="L964" t="s">
+        <v>822</v>
+      </c>
+      <c r="M964" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="965" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A965">
+        <v>1731</v>
+      </c>
+      <c r="B965">
+        <v>32</v>
+      </c>
+      <c r="C965" t="s">
+        <v>948</v>
+      </c>
+      <c r="J965" t="s">
+        <v>99</v>
+      </c>
+      <c r="K965">
+        <v>47</v>
+      </c>
+      <c r="L965" t="s">
+        <v>822</v>
+      </c>
+      <c r="M965" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="966" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A966">
+        <v>1731</v>
+      </c>
+      <c r="B966">
+        <v>32</v>
+      </c>
+      <c r="C966" t="s">
+        <v>949</v>
+      </c>
+      <c r="J966" t="s">
+        <v>99</v>
+      </c>
+      <c r="K966">
+        <v>47</v>
+      </c>
+      <c r="L966" t="s">
+        <v>822</v>
+      </c>
+      <c r="M966" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="967" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A967">
+        <v>1732</v>
+      </c>
+      <c r="B967">
+        <v>33</v>
+      </c>
+      <c r="C967" t="s">
+        <v>950</v>
+      </c>
+      <c r="J967" t="s">
+        <v>99</v>
+      </c>
+      <c r="K967">
+        <v>47</v>
+      </c>
+      <c r="L967" t="s">
+        <v>822</v>
+      </c>
+      <c r="M967" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="968" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A968">
+        <v>1732</v>
+      </c>
+      <c r="B968">
+        <v>33</v>
+      </c>
+      <c r="C968" t="s">
+        <v>951</v>
+      </c>
+      <c r="J968" t="s">
+        <v>99</v>
+      </c>
+      <c r="K968">
+        <v>47</v>
+      </c>
+      <c r="L968" t="s">
+        <v>822</v>
+      </c>
+      <c r="M968" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="969" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A969">
+        <v>1732</v>
+      </c>
+      <c r="B969">
+        <v>33</v>
+      </c>
+      <c r="C969" t="s">
+        <v>952</v>
+      </c>
+      <c r="J969" t="s">
+        <v>99</v>
+      </c>
+      <c r="K969">
+        <v>47</v>
+      </c>
+      <c r="L969" t="s">
+        <v>822</v>
+      </c>
+      <c r="M969" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="970" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A970">
+        <v>1732</v>
+      </c>
+      <c r="B970">
+        <v>34</v>
+      </c>
+      <c r="C970" t="s">
+        <v>953</v>
+      </c>
+      <c r="J970" t="s">
+        <v>99</v>
+      </c>
+      <c r="K970">
+        <v>47</v>
+      </c>
+      <c r="L970" t="s">
+        <v>822</v>
+      </c>
+      <c r="M970" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="971" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A971">
+        <v>1732</v>
+      </c>
+      <c r="B971">
+        <v>34</v>
+      </c>
+      <c r="C971" t="s">
+        <v>954</v>
+      </c>
+      <c r="J971" t="s">
+        <v>99</v>
+      </c>
+      <c r="K971">
+        <v>47</v>
+      </c>
+      <c r="L971" t="s">
+        <v>822</v>
+      </c>
+      <c r="M971" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="972" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A972">
+        <v>1732</v>
+      </c>
+      <c r="B972">
+        <v>34</v>
+      </c>
+      <c r="C972" t="s">
+        <v>955</v>
+      </c>
+      <c r="J972" t="s">
+        <v>99</v>
+      </c>
+      <c r="K972">
+        <v>47</v>
+      </c>
+      <c r="L972" t="s">
+        <v>822</v>
+      </c>
+      <c r="M972" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="973" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A973">
+        <v>1733</v>
+      </c>
+      <c r="B973">
+        <v>35</v>
+      </c>
+      <c r="C973" t="s">
+        <v>956</v>
+      </c>
+      <c r="J973" t="s">
+        <v>99</v>
+      </c>
+      <c r="K973">
+        <v>47</v>
+      </c>
+      <c r="L973" t="s">
+        <v>822</v>
+      </c>
+      <c r="M973" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="974" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A974">
+        <v>1733</v>
+      </c>
+      <c r="B974">
+        <v>35</v>
+      </c>
+      <c r="C974" t="s">
+        <v>957</v>
+      </c>
+      <c r="J974" t="s">
+        <v>99</v>
+      </c>
+      <c r="K974">
+        <v>47</v>
+      </c>
+      <c r="L974" t="s">
+        <v>822</v>
+      </c>
+      <c r="M974" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="975" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A975">
+        <v>1733</v>
+      </c>
+      <c r="B975">
+        <v>35</v>
+      </c>
+      <c r="C975" t="s">
+        <v>958</v>
+      </c>
+      <c r="J975" t="s">
+        <v>99</v>
+      </c>
+      <c r="K975">
+        <v>47</v>
+      </c>
+      <c r="L975" t="s">
+        <v>822</v>
+      </c>
+      <c r="M975" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="976" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A976">
+        <v>1733</v>
+      </c>
+      <c r="B976">
+        <v>36</v>
+      </c>
+      <c r="C976" t="s">
+        <v>959</v>
+      </c>
+      <c r="J976" t="s">
+        <v>99</v>
+      </c>
+      <c r="K976">
+        <v>47</v>
+      </c>
+      <c r="L976" t="s">
+        <v>822</v>
+      </c>
+      <c r="M976" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="977" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A977">
+        <v>1734</v>
+      </c>
+      <c r="B977">
+        <v>36</v>
+      </c>
+      <c r="C977" t="s">
+        <v>960</v>
+      </c>
+      <c r="J977" t="s">
+        <v>99</v>
+      </c>
+      <c r="K977">
+        <v>47</v>
+      </c>
+      <c r="L977" t="s">
+        <v>822</v>
+      </c>
+      <c r="M977" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="978" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A978">
+        <v>1734</v>
+      </c>
+      <c r="B978">
+        <v>36</v>
+      </c>
+      <c r="C978" t="s">
+        <v>961</v>
+      </c>
+      <c r="J978" t="s">
+        <v>99</v>
+      </c>
+      <c r="K978">
+        <v>47</v>
+      </c>
+      <c r="L978" t="s">
+        <v>822</v>
+      </c>
+      <c r="M978" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="979" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A979">
+        <v>1734</v>
+      </c>
+      <c r="B979">
+        <v>36</v>
+      </c>
+      <c r="C979" t="s">
+        <v>962</v>
+      </c>
+      <c r="J979" t="s">
+        <v>99</v>
+      </c>
+      <c r="K979">
+        <v>47</v>
+      </c>
+      <c r="L979" t="s">
+        <v>822</v>
+      </c>
+      <c r="M979" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="980" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A980">
+        <v>1734</v>
+      </c>
+      <c r="B980">
+        <v>36</v>
+      </c>
+      <c r="C980" t="s">
+        <v>963</v>
+      </c>
+      <c r="J980" t="s">
+        <v>99</v>
+      </c>
+      <c r="K980">
+        <v>47</v>
+      </c>
+      <c r="L980" t="s">
+        <v>822</v>
+      </c>
+      <c r="M980" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="981" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A981">
+        <v>1734</v>
+      </c>
+      <c r="B981">
+        <v>37</v>
+      </c>
+      <c r="C981" t="s">
+        <v>964</v>
+      </c>
+      <c r="J981" t="s">
+        <v>99</v>
+      </c>
+      <c r="K981">
+        <v>47</v>
+      </c>
+      <c r="L981" t="s">
+        <v>822</v>
+      </c>
+      <c r="M981" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="982" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A982">
+        <v>1734</v>
+      </c>
+      <c r="B982">
+        <v>37</v>
+      </c>
+      <c r="C982" t="s">
+        <v>965</v>
+      </c>
+      <c r="J982" t="s">
+        <v>99</v>
+      </c>
+      <c r="K982">
+        <v>47</v>
+      </c>
+      <c r="L982" t="s">
+        <v>822</v>
+      </c>
+      <c r="M982" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="983" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A983">
+        <v>1734</v>
+      </c>
+      <c r="B983">
+        <v>37</v>
+      </c>
+      <c r="C983" t="s">
+        <v>966</v>
+      </c>
+      <c r="J983" t="s">
+        <v>99</v>
+      </c>
+      <c r="K983">
+        <v>47</v>
+      </c>
+      <c r="L983" t="s">
+        <v>822</v>
+      </c>
+      <c r="M983" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="984" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A984">
+        <v>1734</v>
+      </c>
+      <c r="B984">
+        <v>37</v>
+      </c>
+      <c r="C984" t="s">
+        <v>967</v>
+      </c>
+      <c r="J984" t="s">
+        <v>99</v>
+      </c>
+      <c r="K984">
+        <v>47</v>
+      </c>
+      <c r="L984" t="s">
+        <v>822</v>
+      </c>
+      <c r="M984" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="985" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A985">
+        <v>1734</v>
+      </c>
+      <c r="B985">
+        <v>38</v>
+      </c>
+      <c r="C985" t="s">
+        <v>968</v>
+      </c>
+      <c r="J985" t="s">
+        <v>99</v>
+      </c>
+      <c r="K985">
+        <v>47</v>
+      </c>
+      <c r="L985" t="s">
+        <v>822</v>
+      </c>
+      <c r="M985" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="986" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A986">
+        <v>1735</v>
+      </c>
+      <c r="B986">
+        <v>38</v>
+      </c>
+      <c r="C986" t="s">
+        <v>969</v>
+      </c>
+      <c r="J986" t="s">
+        <v>99</v>
+      </c>
+      <c r="K986">
+        <v>47</v>
+      </c>
+      <c r="L986" t="s">
+        <v>822</v>
+      </c>
+      <c r="M986" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="987" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A987">
+        <v>1735</v>
+      </c>
+      <c r="B987">
+        <v>38</v>
+      </c>
+      <c r="C987" t="s">
+        <v>970</v>
+      </c>
+      <c r="J987" t="s">
+        <v>99</v>
+      </c>
+      <c r="K987">
+        <v>47</v>
+      </c>
+      <c r="L987" t="s">
+        <v>822</v>
+      </c>
+      <c r="M987" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="988" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A988">
+        <v>1736</v>
+      </c>
+      <c r="B988">
+        <v>38</v>
+      </c>
+      <c r="C988" t="s">
+        <v>971</v>
+      </c>
+      <c r="J988" t="s">
+        <v>99</v>
+      </c>
+      <c r="K988">
+        <v>47</v>
+      </c>
+      <c r="L988" t="s">
+        <v>822</v>
+      </c>
+      <c r="M988" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="989" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A989">
+        <v>1736</v>
+      </c>
+      <c r="B989">
+        <v>39</v>
+      </c>
+      <c r="C989" t="s">
+        <v>972</v>
+      </c>
+      <c r="J989" t="s">
+        <v>99</v>
+      </c>
+      <c r="K989">
+        <v>47</v>
+      </c>
+      <c r="L989" t="s">
+        <v>822</v>
+      </c>
+      <c r="M989" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="990" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A990">
+        <v>1736</v>
+      </c>
+      <c r="B990">
+        <v>39</v>
+      </c>
+      <c r="C990" t="s">
+        <v>973</v>
+      </c>
+      <c r="J990" t="s">
+        <v>99</v>
+      </c>
+      <c r="K990">
+        <v>47</v>
+      </c>
+      <c r="L990" t="s">
+        <v>822</v>
+      </c>
+      <c r="M990" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="991" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A991">
+        <v>1737</v>
+      </c>
+      <c r="B991">
+        <v>39</v>
+      </c>
+      <c r="C991" t="s">
+        <v>974</v>
+      </c>
+      <c r="J991" t="s">
+        <v>99</v>
+      </c>
+      <c r="K991">
+        <v>47</v>
+      </c>
+      <c r="L991" t="s">
+        <v>822</v>
+      </c>
+      <c r="M991" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="992" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A992">
+        <v>1738</v>
+      </c>
+      <c r="B992">
+        <v>39</v>
+      </c>
+      <c r="C992" t="s">
+        <v>975</v>
+      </c>
+      <c r="J992" t="s">
+        <v>99</v>
+      </c>
+      <c r="K992">
+        <v>47</v>
+      </c>
+      <c r="L992" t="s">
+        <v>822</v>
+      </c>
+      <c r="M992" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="993" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A993">
+        <v>1738</v>
+      </c>
+      <c r="B993">
+        <v>40</v>
+      </c>
+      <c r="C993" t="s">
+        <v>976</v>
+      </c>
+      <c r="J993" t="s">
+        <v>99</v>
+      </c>
+      <c r="K993">
+        <v>47</v>
+      </c>
+      <c r="L993" t="s">
+        <v>822</v>
+      </c>
+      <c r="M993" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="994" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A994">
+        <v>1739</v>
+      </c>
+      <c r="B994">
+        <v>40</v>
+      </c>
+      <c r="C994" t="s">
+        <v>977</v>
+      </c>
+      <c r="J994" t="s">
+        <v>99</v>
+      </c>
+      <c r="K994">
+        <v>47</v>
+      </c>
+      <c r="L994" t="s">
+        <v>822</v>
+      </c>
+      <c r="M994" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="995" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A995">
+        <v>1739</v>
+      </c>
+      <c r="B995">
+        <v>40</v>
+      </c>
+      <c r="C995" t="s">
+        <v>978</v>
+      </c>
+      <c r="J995" t="s">
+        <v>99</v>
+      </c>
+      <c r="K995">
+        <v>47</v>
+      </c>
+      <c r="L995" t="s">
+        <v>822</v>
+      </c>
+      <c r="M995" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="996" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A996">
+        <v>1739</v>
+      </c>
+      <c r="B996">
+        <v>40</v>
+      </c>
+      <c r="C996" t="s">
+        <v>979</v>
+      </c>
+      <c r="J996" t="s">
+        <v>99</v>
+      </c>
+      <c r="K996">
+        <v>47</v>
+      </c>
+      <c r="L996" t="s">
+        <v>822</v>
+      </c>
+      <c r="M996" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="997" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A997">
+        <v>1739</v>
+      </c>
+      <c r="B997">
+        <v>40</v>
+      </c>
+      <c r="C997" t="s">
+        <v>980</v>
+      </c>
+      <c r="J997" t="s">
+        <v>99</v>
+      </c>
+      <c r="K997">
+        <v>47</v>
+      </c>
+      <c r="L997" t="s">
+        <v>822</v>
+      </c>
+      <c r="M997" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="998" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A998">
+        <v>1739</v>
+      </c>
+      <c r="B998">
+        <v>40</v>
+      </c>
+      <c r="C998" t="s">
+        <v>981</v>
+      </c>
+      <c r="J998" t="s">
+        <v>99</v>
+      </c>
+      <c r="K998">
+        <v>47</v>
+      </c>
+      <c r="L998" t="s">
+        <v>822</v>
+      </c>
+      <c r="M998" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="999" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A999">
+        <v>1740</v>
+      </c>
+      <c r="B999">
+        <v>41</v>
+      </c>
+      <c r="C999" t="s">
+        <v>982</v>
+      </c>
+      <c r="J999" t="s">
+        <v>99</v>
+      </c>
+      <c r="K999">
+        <v>47</v>
+      </c>
+      <c r="L999" t="s">
+        <v>822</v>
+      </c>
+      <c r="M999" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1000">
+        <v>1740</v>
+      </c>
+      <c r="B1000">
+        <v>41</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>983</v>
+      </c>
+      <c r="J1000" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1000">
+        <v>47</v>
+      </c>
+      <c r="L1000" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1000" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1001">
+        <v>1740</v>
+      </c>
+      <c r="B1001">
+        <v>41</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>984</v>
+      </c>
+      <c r="J1001" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1001">
+        <v>47</v>
+      </c>
+      <c r="L1001" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1001" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1002">
+        <v>1740</v>
+      </c>
+      <c r="B1002">
+        <v>42</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>985</v>
+      </c>
+      <c r="J1002" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1002">
+        <v>47</v>
+      </c>
+      <c r="L1002" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1002" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1003">
+        <v>1741</v>
+      </c>
+      <c r="B1003">
+        <v>42</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>986</v>
+      </c>
+      <c r="J1003" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1003">
+        <v>47</v>
+      </c>
+      <c r="L1003" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1003" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1004">
+        <v>1741</v>
+      </c>
+      <c r="B1004">
+        <v>42</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>987</v>
+      </c>
+      <c r="J1004" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1004">
+        <v>47</v>
+      </c>
+      <c r="L1004" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1004" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1005">
+        <v>1741</v>
+      </c>
+      <c r="B1005">
+        <v>42</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>988</v>
+      </c>
+      <c r="J1005" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1005">
+        <v>47</v>
+      </c>
+      <c r="L1005" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1005" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1006">
+        <v>1742</v>
+      </c>
+      <c r="B1006">
+        <v>43</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>989</v>
+      </c>
+      <c r="J1006" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1006">
+        <v>47</v>
+      </c>
+      <c r="L1006" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1006" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1007">
+        <v>1742</v>
+      </c>
+      <c r="B1007">
+        <v>43</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>990</v>
+      </c>
+      <c r="J1007" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1007">
+        <v>47</v>
+      </c>
+      <c r="L1007" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1007" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1008">
+        <v>1743</v>
+      </c>
+      <c r="B1008">
+        <v>43</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>991</v>
+      </c>
+      <c r="J1008" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1008">
+        <v>47</v>
+      </c>
+      <c r="L1008" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1008" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1009">
+        <v>1743</v>
+      </c>
+      <c r="B1009">
+        <v>43</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>992</v>
+      </c>
+      <c r="J1009" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1009">
+        <v>47</v>
+      </c>
+      <c r="L1009" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1009" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1010">
+        <v>1743</v>
+      </c>
+      <c r="B1010">
+        <v>44</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>993</v>
+      </c>
+      <c r="J1010" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1010">
+        <v>47</v>
+      </c>
+      <c r="L1010" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1010" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1011">
+        <v>1743</v>
+      </c>
+      <c r="B1011">
+        <v>44</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>994</v>
+      </c>
+      <c r="J1011" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1011">
+        <v>47</v>
+      </c>
+      <c r="L1011" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1011" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1012">
+        <v>1744</v>
+      </c>
+      <c r="B1012">
+        <v>44</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>995</v>
+      </c>
+      <c r="J1012" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1012">
+        <v>47</v>
+      </c>
+      <c r="L1012" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1012" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1013">
+        <v>1745</v>
+      </c>
+      <c r="B1013">
+        <v>45</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>996</v>
+      </c>
+      <c r="J1013" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1013">
+        <v>47</v>
+      </c>
+      <c r="L1013" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1013" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1014">
+        <v>1745</v>
+      </c>
+      <c r="B1014">
+        <v>45</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>997</v>
+      </c>
+      <c r="J1014" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1014">
+        <v>47</v>
+      </c>
+      <c r="L1014" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1014" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1015">
+        <v>1745</v>
+      </c>
+      <c r="B1015">
+        <v>45</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>998</v>
+      </c>
+      <c r="J1015" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1015">
+        <v>47</v>
+      </c>
+      <c r="L1015" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1015" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1016">
+        <v>1745</v>
+      </c>
+      <c r="B1016">
+        <v>45</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>999</v>
+      </c>
+      <c r="J1016" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1016">
+        <v>47</v>
+      </c>
+      <c r="L1016" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1016" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1017">
+        <v>1746</v>
+      </c>
+      <c r="B1017">
+        <v>46</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>1000</v>
+      </c>
+      <c r="J1017" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1017">
+        <v>47</v>
+      </c>
+      <c r="L1017" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1017" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1018">
+        <v>1746</v>
+      </c>
+      <c r="B1018">
+        <v>46</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J1018" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1018">
+        <v>47</v>
+      </c>
+      <c r="L1018" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1018" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1019">
+        <v>1746</v>
+      </c>
+      <c r="B1019">
+        <v>47</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J1019" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1019">
+        <v>47</v>
+      </c>
+      <c r="L1019" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1019" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1020">
+        <v>1746</v>
+      </c>
+      <c r="B1020">
+        <v>47</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J1020" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1020">
+        <v>47</v>
+      </c>
+      <c r="L1020" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1020" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1021">
+        <v>1747</v>
+      </c>
+      <c r="B1021">
+        <v>48</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>1004</v>
+      </c>
+      <c r="J1021" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1021">
+        <v>47</v>
+      </c>
+      <c r="L1021" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1021" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1022">
+        <v>1747</v>
+      </c>
+      <c r="B1022">
+        <v>48</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>1005</v>
+      </c>
+      <c r="J1022" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1022">
+        <v>47</v>
+      </c>
+      <c r="L1022" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1022" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1023">
+        <v>1747</v>
+      </c>
+      <c r="B1023">
+        <v>48</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>1006</v>
+      </c>
+      <c r="J1023" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1023">
+        <v>47</v>
+      </c>
+      <c r="L1023" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1023" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1024">
+        <v>1747</v>
+      </c>
+      <c r="B1024">
+        <v>48</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>1007</v>
+      </c>
+      <c r="J1024" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1024">
+        <v>47</v>
+      </c>
+      <c r="L1024" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1024" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1025">
+        <v>1747</v>
+      </c>
+      <c r="B1025">
+        <v>49</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>1008</v>
+      </c>
+      <c r="J1025" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1025">
+        <v>47</v>
+      </c>
+      <c r="L1025" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1025" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1026">
+        <v>1748</v>
+      </c>
+      <c r="B1026">
+        <v>49</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J1026" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1026">
+        <v>47</v>
+      </c>
+      <c r="L1026" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1026" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1027">
+        <v>1748</v>
+      </c>
+      <c r="B1027">
+        <v>49</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>1010</v>
+      </c>
+      <c r="J1027" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1027">
+        <v>47</v>
+      </c>
+      <c r="L1027" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1027" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1028">
+        <v>1748</v>
+      </c>
+      <c r="B1028">
+        <v>49</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J1028" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1028">
+        <v>47</v>
+      </c>
+      <c r="L1028" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1028" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1029">
+        <v>1749</v>
+      </c>
+      <c r="B1029">
+        <v>50</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>1012</v>
+      </c>
+      <c r="J1029" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1029">
+        <v>47</v>
+      </c>
+      <c r="L1029" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1029" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1030">
+        <v>1749</v>
+      </c>
+      <c r="B1030">
+        <v>50</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>1013</v>
+      </c>
+      <c r="J1030" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1030">
+        <v>47</v>
+      </c>
+      <c r="L1030" t="s">
+        <v>822</v>
+      </c>
+      <c r="M1030" t="s">
+        <v>821</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M715" xr:uid="{26F4E75F-C79D-4AC9-AFD8-C6AF1AD32317}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>